<commit_message>
Added a new US state chart excluding New York to zoom in on the other states
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programming\Projects\DS Projects\CoronaVirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A05232F-173F-4629-B1A0-3C20B6675905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D927812-F4D4-4421-8ECA-C6299C879CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -532,7 +532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0A91CA-B277-40C5-9F76-C8642C725AE7}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1132,29 +1134,28 @@
         <f t="shared" si="0"/>
         <v>43910</v>
       </c>
-      <c r="I14" s="19">
-        <f>I13*(1+AVERAGE(M11:M13))</f>
-        <v>19802.640909607599</v>
+      <c r="I14" s="18">
+        <v>19383</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ref="J14" si="15">IF(I14&lt;=0,0, I14-B14)</f>
-        <v>3384.6409096075986</v>
+        <v>2965</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>60.521518672394862</v>
+        <v>59.238997555012226</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="11"/>
-        <v>6013.6409096075986</v>
+        <v>5594</v>
       </c>
       <c r="M14" s="10">
         <f t="shared" si="12"/>
-        <v>0.43611871126315166</v>
+        <v>0.40568569149321926</v>
       </c>
       <c r="N14" s="10">
         <f t="shared" si="8"/>
-        <v>0.10431593809096112</v>
+        <v>7.3882918321028723E-2</v>
       </c>
       <c r="P14" s="20">
         <v>327200000</v>
@@ -1185,28 +1186,28 @@
         <v>43911</v>
       </c>
       <c r="I15" s="19">
-        <f>I14*(1+AVERAGE(M12:M14))</f>
-        <v>28843.265181670002</v>
+        <f>I14*(1+AVERAGE(M10:M14))</f>
+        <v>27063.170246412556</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="2"/>
-        <v>6977.2651816700018</v>
+        <v>5197.1702464125556</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>88.151788452536678</v>
+        <v>82.71140050859583</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="11"/>
-        <v>9040.6242720624032</v>
+        <v>7680.1702464125556</v>
       </c>
       <c r="M15" s="10">
         <f t="shared" si="12"/>
-        <v>0.45653629297879084</v>
+        <v>0.39623227810001316</v>
       </c>
       <c r="N15" s="10">
         <f t="shared" si="8"/>
-        <v>0.1247335198066003</v>
+        <v>6.4429504927822623E-2</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1231,28 +1232,28 @@
         <v>43912</v>
       </c>
       <c r="I16" s="19">
-        <f>I15*(1+AVERAGE(M13:M15))</f>
-        <v>42129.518244154169</v>
+        <f t="shared" ref="I16:I28" si="16">I15*(1+AVERAGE(M11:M15))</f>
+        <v>38485.311711700815</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="2"/>
-        <v>13008.518244154169</v>
+        <v>9364.3117117008151</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>128.75769634521444</v>
+        <v>117.62014581815653</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="11"/>
-        <v>13286.253062484167</v>
+        <v>11422.141465288259</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="12"/>
-        <v>0.46063623444850582</v>
+        <v>0.4220548206765376</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="8"/>
-        <v>0.12883346127631529</v>
+        <v>9.0252047504347066E-2</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
@@ -1281,28 +1282,28 @@
         <v>43913</v>
       </c>
       <c r="I17" s="19">
-        <f>I16*(1+AVERAGE(M14:M16))</f>
-        <v>61134.020887508581</v>
+        <f t="shared" si="16"/>
+        <v>55091.438600277623</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="2"/>
-        <v>22351.020887508581</v>
+        <v>16308.438600277623</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>186.83991713786241</v>
+        <v>168.37236736026168</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="11"/>
-        <v>19004.502643354412</v>
+        <v>16606.126888576808</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" si="12"/>
-        <v>0.45109707956348277</v>
+        <v>0.43149259158859798</v>
       </c>
       <c r="N17" s="11">
         <f t="shared" si="8"/>
-        <v>0.11929430639129224</v>
+        <v>9.968981841640745E-2</v>
       </c>
       <c r="P17" s="20">
         <v>24747</v>
@@ -1313,7 +1314,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <f t="shared" ref="A18:A28" si="16">+A17+1</f>
+        <f t="shared" ref="A18:A28" si="17">+A17+1</f>
         <v>43914</v>
       </c>
       <c r="B18" s="7">
@@ -1337,28 +1338,28 @@
         <v>43914</v>
       </c>
       <c r="I18" s="19">
-        <f>I17*(1+AVERAGE(M15:M17))</f>
-        <v>89016.628465347734</v>
+        <f t="shared" si="16"/>
+        <v>78722.57051300937</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="2"/>
-        <v>37365.628465347734</v>
+        <v>27071.57051300937</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="7"/>
-        <v>272.05571046866669</v>
+        <v>240.5946531571191</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="11"/>
-        <v>27882.607577839153</v>
+        <v>23631.131912731747</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="12"/>
-        <v>0.45608986899692644</v>
+        <v>0.42894381619238858</v>
       </c>
       <c r="N18" s="11">
         <f t="shared" si="8"/>
-        <v>0.1242870958247359</v>
+        <v>9.7141043020198048E-2</v>
       </c>
       <c r="P18" s="20">
         <v>7375</v>
@@ -1369,7 +1370,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43915</v>
       </c>
       <c r="B19" s="7">
@@ -1393,28 +1394,28 @@
         <v>43915</v>
       </c>
       <c r="I19" s="19">
-        <f>I18*(1+AVERAGE(M16:M18))</f>
-        <v>129602.96449474571</v>
+        <f t="shared" si="16"/>
+        <v>111540.58052731256</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="2"/>
-        <v>60813.964494745713</v>
+        <v>42751.580527312559</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="7"/>
-        <v>396.09707975166782</v>
+        <v>340.89419476562517</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="11"/>
-        <v>40586.336029397979</v>
+        <v>32818.010014303189</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" si="12"/>
-        <v>0.45594106100297171</v>
+        <v>0.41688183961015118</v>
       </c>
       <c r="N19" s="11">
         <f t="shared" si="8"/>
-        <v>0.12413828783078118</v>
+        <v>8.5079066437960649E-2</v>
       </c>
       <c r="P19" s="21">
         <f>+P18/P17</f>
@@ -1423,7 +1424,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43916</v>
       </c>
       <c r="B20" s="7">
@@ -1447,28 +1448,28 @@
         <v>43916</v>
       </c>
       <c r="I20" s="19">
-        <f>I19*(1+AVERAGE(M17:M19))</f>
-        <v>188491.44150315781</v>
+        <f t="shared" si="16"/>
+        <v>158289.58790084932</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="2"/>
-        <v>96878.44150315781</v>
+        <v>66676.587900849321</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="7"/>
-        <v>576.07408772358735</v>
+        <v>483.7701341712999</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="11"/>
-        <v>58888.477008412097</v>
+        <v>46749.007373536762</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="12"/>
-        <v>0.45437600318779375</v>
+        <v>0.41912106923353776</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="8"/>
-        <v>0.12257323001560322</v>
+        <v>8.7318296061347223E-2</v>
       </c>
       <c r="P20" s="22">
         <v>409</v>
@@ -1479,7 +1480,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43917</v>
       </c>
       <c r="B21" s="7">
@@ -1503,28 +1504,28 @@
         <v>43917</v>
       </c>
       <c r="I21" s="19">
-        <f>I20*(1+AVERAGE(M18:M20))</f>
-        <v>274343.44567531015</v>
+        <f t="shared" si="16"/>
+        <v>225356.70069360419</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="2"/>
-        <v>152333.44567531015</v>
+        <v>103346.70069360419</v>
       </c>
       <c r="K21" s="8">
         <f t="shared" si="7"/>
-        <v>838.4579635553489</v>
+        <v>688.74297277996391</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="11"/>
-        <v>85852.004172152345</v>
+        <v>67067.112792754866</v>
       </c>
       <c r="M21" s="11">
         <f t="shared" si="12"/>
-        <v>0.45546897772923056</v>
+        <v>0.42369882746024262</v>
       </c>
       <c r="N21" s="11">
         <f t="shared" si="8"/>
-        <v>0.12366620455704003</v>
+        <v>9.1896054288052087E-2</v>
       </c>
       <c r="P21" s="23">
         <f>+P20*P19</f>
@@ -1536,7 +1537,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43918</v>
       </c>
       <c r="B22" s="7">
@@ -1560,33 +1561,33 @@
         <v>43918</v>
       </c>
       <c r="I22" s="19">
-        <f>I21*(1+AVERAGE(M19:M21))</f>
-        <v>399241.59527383524</v>
+        <f t="shared" si="16"/>
+        <v>320914.16812673182</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="2"/>
-        <v>236748.59527383524</v>
+        <v>158421.16812673182</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="7"/>
-        <v>1220.1760246755357</v>
+        <v>980.78902239221213</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="11"/>
-        <v>124898.14959852508</v>
+        <v>95557.467433127633</v>
       </c>
       <c r="M22" s="11">
         <f t="shared" si="12"/>
-        <v>0.45526201397333194</v>
+        <v>0.42402762881698347</v>
       </c>
       <c r="N22" s="11">
         <f t="shared" si="8"/>
-        <v>0.1234592408011414</v>
+        <v>9.2224855644792936E-2</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43919</v>
       </c>
       <c r="B23" s="7">
@@ -1610,28 +1611,28 @@
         <v>43919</v>
       </c>
       <c r="I23" s="19">
-        <f>I22*(1+AVERAGE(M20:M22))</f>
-        <v>580910.76006033435</v>
+        <f t="shared" si="16"/>
+        <v>456511.51942769479</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="2"/>
-        <v>364501.76006033435</v>
+        <v>240102.51942769479</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="7"/>
-        <v>1775.3996334362296</v>
+        <v>1395.2063552191159</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="11"/>
-        <v>181669.16478649911</v>
+        <v>135597.35130096297</v>
       </c>
       <c r="M23" s="11">
         <f t="shared" si="12"/>
-        <v>0.45503566496345232</v>
+        <v>0.42253463626266069</v>
       </c>
       <c r="N23" s="11">
         <f t="shared" si="8"/>
-        <v>0.12323289179126179</v>
+        <v>9.0731863090470155E-2</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>16</v>
@@ -1646,7 +1647,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43920</v>
       </c>
       <c r="B24" s="7">
@@ -1670,33 +1671,33 @@
         <v>43920</v>
       </c>
       <c r="I24" s="19">
-        <f>I23*(1+AVERAGE(M21:M23))</f>
-        <v>845373.60892330646</v>
+        <f t="shared" si="16"/>
+        <v>648818.27534518926</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="2"/>
-        <v>557159.60892330646</v>
+        <v>360604.27534518926</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="7"/>
-        <v>2583.6601739709854</v>
+        <v>1982.9409393190383</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="11"/>
-        <v>264462.84886297211</v>
+        <v>192306.75591749448</v>
       </c>
       <c r="M24" s="11">
         <f t="shared" si="12"/>
-        <v>0.45525555222200492</v>
+        <v>0.42125280027671513</v>
       </c>
       <c r="N24" s="11">
         <f t="shared" si="8"/>
-        <v>0.12345277904981439</v>
+        <v>8.9450027104524599E-2</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43921</v>
       </c>
       <c r="B25" s="7">
@@ -1720,33 +1721,33 @@
         <v>43921</v>
       </c>
       <c r="I25" s="19">
-        <f>I24*(1+AVERAGE(M22:M24))</f>
-        <v>1230174.496657169</v>
+        <f t="shared" si="16"/>
+        <v>922701.98253731534</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="2"/>
-        <v>846330.49665716896</v>
+        <v>538857.98253731534</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="7"/>
-        <v>3759.702006898438</v>
+        <v>2819.9938341604993</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="11"/>
-        <v>384800.8877338625</v>
+        <v>273883.70719212608</v>
       </c>
       <c r="M25" s="11">
         <f t="shared" si="12"/>
-        <v>0.45518441038626295</v>
+        <v>0.42212699241002788</v>
       </c>
       <c r="N25" s="11">
         <f t="shared" si="8"/>
-        <v>0.12338163721407241</v>
+        <v>9.0324219237837344E-2</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43922</v>
       </c>
       <c r="B26" s="7">
@@ -1770,33 +1771,33 @@
         <v>43922</v>
       </c>
       <c r="I26" s="19">
-        <f>I25*(1+AVERAGE(M23:M25))</f>
-        <v>1790098.9276057265</v>
+        <f t="shared" si="16"/>
+        <v>1312754.1095714229</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="2"/>
-        <v>1278893.9276057265</v>
+        <v>801549.10957142292</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="7"/>
-        <v>5470.9624926825381</v>
+        <v>4012.0846869542261</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="11"/>
-        <v>559924.43094855756</v>
+        <v>390052.12703410757</v>
       </c>
       <c r="M26" s="11">
         <f t="shared" si="12"/>
-        <v>0.4551585425239067</v>
+        <v>0.42272817704532606</v>
       </c>
       <c r="N26" s="11">
         <f t="shared" si="8"/>
-        <v>0.12335576935171616</v>
+        <v>9.0925403873135524E-2</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43923</v>
       </c>
       <c r="B27" s="7">
@@ -1820,33 +1821,33 @@
         <v>43923</v>
       </c>
       <c r="I27" s="19">
-        <f>I26*(1+AVERAGE(M24:M26))</f>
-        <v>2604951.0674647563</v>
+        <f t="shared" si="16"/>
+        <v>1867437.4161550829</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="2"/>
-        <v>1924127.0674647563</v>
+        <v>1186613.4161550829</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="7"/>
-        <v>7961.3418932296954</v>
+        <v>5707.3270664886404</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="11"/>
-        <v>814852.13985902979</v>
+        <v>554683.30658365996</v>
       </c>
       <c r="M27" s="11">
         <f t="shared" si="12"/>
-        <v>0.45519950171072493</v>
+        <v>0.4225340469623427</v>
       </c>
       <c r="N27" s="11">
         <f t="shared" si="8"/>
-        <v>0.12339672853853439</v>
+        <v>9.0731273790152167E-2</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43924</v>
       </c>
       <c r="B28" s="7">
@@ -1870,28 +1871,28 @@
         <v>43924</v>
       </c>
       <c r="I28" s="19">
-        <f>I27*(1+AVERAGE(M25:M27))</f>
-        <v>3790674.8257424706</v>
+        <f t="shared" si="16"/>
+        <v>2655935.4709241008</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="2"/>
-        <v>2883951.8257424706</v>
+        <v>1749212.4709241008</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="7"/>
-        <v>11585.192010215374</v>
+        <v>8117.1621972007979</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="11"/>
-        <v>1185723.7582777143</v>
+        <v>788498.05476901797</v>
       </c>
       <c r="M28" s="11">
         <f t="shared" si="12"/>
-        <v>0.45518081820696482</v>
+        <v>0.42223533059141433</v>
       </c>
       <c r="N28" s="11">
         <f t="shared" si="8"/>
-        <v>0.12337804503477429</v>
+        <v>9.0432557419223791E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refreshed stats and charts with new data
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Programming\Projects\DS Projects\CoronaVirus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D927812-F4D4-4421-8ECA-C6299C879CA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB8B86-13D8-7A47-BC35-F7930EACED27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -533,30 +535,30 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="3" customWidth="1"/>
-    <col min="3" max="5" width="7.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.85546875" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="3" customWidth="1"/>
+    <col min="3" max="5" width="7.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.83203125" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.5" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -595,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43899</v>
       </c>
@@ -627,7 +629,7 @@
       <c r="M2"/>
       <c r="N2"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f>+A2+1</f>
         <v>43900</v>
@@ -676,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A7" si="4">+A3+1</f>
         <v>43901</v>
@@ -725,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="4"/>
         <v>43902</v>
@@ -774,7 +776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="4"/>
         <v>43903</v>
@@ -823,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="4"/>
         <v>43904</v>
@@ -872,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
@@ -887,7 +889,7 @@
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f>+A7+1</f>
         <v>43905</v>
@@ -933,7 +935,7 @@
         <v>-8.1378036508921781E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" ref="A10" si="9">+A9+1</f>
         <v>43906</v>
@@ -978,7 +980,7 @@
         <v>-6.4683207954799204E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" ref="A11:A17" si="13">+A10+1</f>
         <v>43907</v>
@@ -1023,7 +1025,7 @@
         <v>4.3063192944043649E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="13"/>
         <v>43908</v>
@@ -1068,7 +1070,7 @@
         <v>0.1124336953974554</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="13"/>
         <v>43909</v>
@@ -1113,7 +1115,7 @@
         <v>0.15745092593138438</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="13"/>
         <v>43910</v>
@@ -1164,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="13"/>
         <v>43911</v>
@@ -1185,32 +1187,31 @@
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
-      <c r="I15" s="19">
-        <f>I14*(1+AVERAGE(M10:M14))</f>
-        <v>27063.170246412556</v>
+      <c r="I15" s="18">
+        <v>24207</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" si="2"/>
-        <v>5197.1702464125556</v>
+        <v>2341</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>82.71140050859583</v>
+        <v>73.982273838630803</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" si="11"/>
-        <v>7680.1702464125556</v>
+        <v>4824</v>
       </c>
       <c r="M15" s="10">
         <f t="shared" si="12"/>
-        <v>0.39623227810001316</v>
+        <v>0.24887788268069957</v>
       </c>
       <c r="N15" s="10">
         <f t="shared" si="8"/>
-        <v>6.4429504927822623E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>-8.292489049149096E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="13"/>
         <v>43912</v>
@@ -1233,30 +1234,30 @@
       </c>
       <c r="I16" s="19">
         <f t="shared" ref="I16:I28" si="16">I15*(1+AVERAGE(M11:M15))</f>
-        <v>38485.311711700815</v>
+        <v>33710.27947413388</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="2"/>
-        <v>9364.3117117008151</v>
+        <v>4589.2794741338803</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>117.62014581815653</v>
+        <v>103.02652651018913</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="11"/>
-        <v>11422.141465288259</v>
+        <v>9503.2794741338803</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="12"/>
-        <v>0.4220548206765376</v>
+        <v>0.39258394159267485</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="8"/>
-        <v>9.0252047504347066E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+        <v>6.0781168420484311E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <f t="shared" si="13"/>
         <v>43913</v>
@@ -1283,27 +1284,27 @@
       </c>
       <c r="I17" s="19">
         <f t="shared" si="16"/>
-        <v>55091.438600277623</v>
+        <v>47063.849443285333</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="2"/>
-        <v>16308.438600277623</v>
+        <v>8280.8494432853331</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>168.37236736026168</v>
+        <v>143.83817067018745</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="11"/>
-        <v>16606.126888576808</v>
+        <v>13353.569969151453</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" si="12"/>
-        <v>0.43149259158859798</v>
+        <v>0.39612753668796297</v>
       </c>
       <c r="N17" s="11">
         <f t="shared" si="8"/>
-        <v>9.968981841640745E-2</v>
+        <v>6.4324763515772432E-2</v>
       </c>
       <c r="P17" s="20">
         <v>24747</v>
@@ -1312,7 +1313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <f t="shared" ref="A18:A28" si="17">+A17+1</f>
         <v>43914</v>
@@ -1339,27 +1340,27 @@
       </c>
       <c r="I18" s="19">
         <f t="shared" si="16"/>
-        <v>78722.57051300937</v>
+        <v>65254.297884915744</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="2"/>
-        <v>27071.57051300937</v>
+        <v>13603.297884915744</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="7"/>
-        <v>240.5946531571191</v>
+        <v>199.43245074852001</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="11"/>
-        <v>23631.131912731747</v>
+        <v>18190.448441630411</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="12"/>
-        <v>0.42894381619238858</v>
+        <v>0.38650575031162626</v>
       </c>
       <c r="N18" s="11">
         <f t="shared" si="8"/>
-        <v>9.7141043020198048E-2</v>
+        <v>5.4702977139435727E-2</v>
       </c>
       <c r="P18" s="20">
         <v>7375</v>
@@ -1368,7 +1369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <f t="shared" si="17"/>
         <v>43915</v>
@@ -1395,34 +1396,34 @@
       </c>
       <c r="I19" s="19">
         <f t="shared" si="16"/>
-        <v>111540.58052731256</v>
+        <v>89134.510198476695</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="2"/>
-        <v>42751.580527312559</v>
+        <v>20345.510198476695</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="7"/>
-        <v>340.89419476562517</v>
+        <v>272.41598471417086</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="11"/>
-        <v>32818.010014303189</v>
+        <v>23880.212313560951</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" si="12"/>
-        <v>0.41688183961015118</v>
+        <v>0.36595616055323654</v>
       </c>
       <c r="N19" s="11">
         <f t="shared" si="8"/>
-        <v>8.5079066437960649E-2</v>
+        <v>3.4153387381046008E-2</v>
       </c>
       <c r="P19" s="21">
         <f>+P18/P17</f>
         <v>0.29801592112175213</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <f t="shared" si="17"/>
         <v>43916</v>
@@ -1449,27 +1450,27 @@
       </c>
       <c r="I20" s="19">
         <f t="shared" si="16"/>
-        <v>158289.58790084932</v>
+        <v>121045.57886735443</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="2"/>
-        <v>66676.587900849321</v>
+        <v>29432.57886735443</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="7"/>
-        <v>483.7701341712999</v>
+        <v>369.94370069484853</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="11"/>
-        <v>46749.007373536762</v>
+        <v>31911.068668877735</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="12"/>
-        <v>0.41912106923353776</v>
+        <v>0.35801025436524014</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="8"/>
-        <v>8.7318296061347223E-2</v>
+        <v>2.6207481193049609E-2</v>
       </c>
       <c r="P20" s="22">
         <v>409</v>
@@ -1478,7 +1479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <f t="shared" si="17"/>
         <v>43917</v>
@@ -1505,27 +1506,27 @@
       </c>
       <c r="I21" s="19">
         <f t="shared" si="16"/>
-        <v>225356.70069360419</v>
+        <v>167023.13556818821</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="2"/>
-        <v>103346.70069360419</v>
+        <v>45013.135568188212</v>
       </c>
       <c r="K21" s="8">
         <f t="shared" si="7"/>
-        <v>688.74297277996391</v>
+        <v>510.4619057707464</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="11"/>
-        <v>67067.112792754866</v>
+        <v>45977.556700833782</v>
       </c>
       <c r="M21" s="11">
         <f t="shared" si="12"/>
-        <v>0.42369882746024262</v>
+        <v>0.37983672870214813</v>
       </c>
       <c r="N21" s="11">
         <f t="shared" si="8"/>
-        <v>9.1896054288052087E-2</v>
+        <v>4.8033955529957595E-2</v>
       </c>
       <c r="P21" s="23">
         <f>+P20*P19</f>
@@ -1535,7 +1536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <f t="shared" si="17"/>
         <v>43918</v>
@@ -1562,30 +1563,30 @@
       </c>
       <c r="I22" s="19">
         <f t="shared" si="16"/>
-        <v>320914.16812673182</v>
+        <v>230038.84110663802</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="2"/>
-        <v>158421.16812673182</v>
+        <v>67545.841106638021</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="7"/>
-        <v>980.78902239221213</v>
+        <v>703.05269286869805</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="11"/>
-        <v>95557.467433127633</v>
+        <v>63015.705538449809</v>
       </c>
       <c r="M22" s="11">
         <f t="shared" si="12"/>
-        <v>0.42402762881698347</v>
+        <v>0.37728728612404278</v>
       </c>
       <c r="N22" s="11">
         <f t="shared" si="8"/>
-        <v>9.2224855644792936E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4.5484512951852241E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <f t="shared" si="17"/>
         <v>43919</v>
@@ -1612,27 +1613,27 @@
       </c>
       <c r="I23" s="19">
         <f t="shared" si="16"/>
-        <v>456511.51942769479</v>
+        <v>315962.77328970481</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="2"/>
-        <v>240102.51942769479</v>
+        <v>99553.773289704812</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="7"/>
-        <v>1395.2063552191159</v>
+        <v>965.65639758467239</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="11"/>
-        <v>135597.35130096297</v>
+        <v>85923.93218306679</v>
       </c>
       <c r="M23" s="11">
         <f t="shared" si="12"/>
-        <v>0.42253463626266069</v>
+        <v>0.3735192360112588</v>
       </c>
       <c r="N23" s="11">
         <f t="shared" si="8"/>
-        <v>9.0731863090470155E-2</v>
+        <v>4.1716462839068269E-2</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>16</v>
@@ -1645,7 +1646,7 @@
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <f t="shared" si="17"/>
         <v>43920</v>
@@ -1672,30 +1673,30 @@
       </c>
       <c r="I24" s="19">
         <f t="shared" si="16"/>
-        <v>648818.27534518926</v>
+        <v>433160.29596213182</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="2"/>
-        <v>360604.27534518926</v>
+        <v>144946.29596213182</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="7"/>
-        <v>1982.9409393190383</v>
+        <v>1323.8395353365886</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="11"/>
-        <v>192306.75591749448</v>
+        <v>117197.522672427</v>
       </c>
       <c r="M24" s="11">
         <f t="shared" si="12"/>
-        <v>0.42125280027671513</v>
+        <v>0.37092193315118532</v>
       </c>
       <c r="N24" s="11">
         <f t="shared" si="8"/>
-        <v>8.9450027104524599E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+        <v>3.9119159978994789E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <f t="shared" si="17"/>
         <v>43921</v>
@@ -1722,30 +1723,30 @@
       </c>
       <c r="I25" s="19">
         <f t="shared" si="16"/>
-        <v>922701.98253731534</v>
+        <v>594259.14541038696</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="2"/>
-        <v>538857.98253731534</v>
+        <v>210415.14541038696</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="7"/>
-        <v>2819.9938341604993</v>
+        <v>1816.1954321833343</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="11"/>
-        <v>273883.70719212608</v>
+        <v>161098.84944825515</v>
       </c>
       <c r="M25" s="11">
         <f t="shared" si="12"/>
-        <v>0.42212699241002788</v>
+        <v>0.37191508767077514</v>
       </c>
       <c r="N25" s="11">
         <f t="shared" si="8"/>
-        <v>9.0324219237837344E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4.01123144985846E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <f t="shared" si="17"/>
         <v>43922</v>
@@ -1772,30 +1773,30 @@
       </c>
       <c r="I26" s="19">
         <f t="shared" si="16"/>
-        <v>1312754.1095714229</v>
+        <v>816925.70244629506</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="2"/>
-        <v>801549.10957142292</v>
+        <v>305720.70244629506</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="7"/>
-        <v>4012.0846869542261</v>
+        <v>2496.716694518017</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="11"/>
-        <v>390052.12703410757</v>
+        <v>222666.5570359081</v>
       </c>
       <c r="M26" s="11">
         <f t="shared" si="12"/>
-        <v>0.42272817704532606</v>
+        <v>0.37469605433188197</v>
       </c>
       <c r="N26" s="11">
         <f t="shared" si="8"/>
-        <v>9.0925403873135524E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4.2893281159691432E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <f t="shared" si="17"/>
         <v>43923</v>
@@ -1822,30 +1823,30 @@
       </c>
       <c r="I27" s="19">
         <f t="shared" si="16"/>
-        <v>1867437.4161550829</v>
+        <v>1122184.6300310274</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="2"/>
-        <v>1186613.4161550829</v>
+        <v>441360.63003102737</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="7"/>
-        <v>5707.3270664886404</v>
+        <v>3429.6596272341912</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="11"/>
-        <v>554683.30658365996</v>
+        <v>305258.9275847323</v>
       </c>
       <c r="M27" s="11">
         <f t="shared" si="12"/>
-        <v>0.4225340469623427</v>
+        <v>0.37366791945782868</v>
       </c>
       <c r="N27" s="11">
         <f t="shared" si="8"/>
-        <v>9.0731273790152167E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4.1865146285638144E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <f t="shared" si="17"/>
         <v>43924</v>
@@ -1872,27 +1873,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="16"/>
-        <v>2655935.4709241008</v>
+        <v>1540696.7064536202</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="2"/>
-        <v>1749212.4709241008</v>
+        <v>633973.70645362022</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="7"/>
-        <v>8117.1621972007979</v>
+        <v>4708.7307654450497</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="11"/>
-        <v>788498.05476901797</v>
+        <v>418512.07642259286</v>
       </c>
       <c r="M28" s="11">
         <f t="shared" si="12"/>
-        <v>0.42223533059141433</v>
+        <v>0.37294404612458593</v>
       </c>
       <c r="N28" s="11">
         <f t="shared" si="8"/>
-        <v>9.0432557419223791E-2</v>
+        <v>4.1141272952395391E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the US Lockdown forecast in Excel
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AACB8B86-13D8-7A47-BC35-F7930EACED27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE8B2CE-8F80-3441-B2D5-03C0DC66D090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1232,29 +1232,28 @@
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
-      <c r="I16" s="19">
-        <f t="shared" ref="I16:I28" si="16">I15*(1+AVERAGE(M11:M15))</f>
-        <v>33710.27947413388</v>
+      <c r="I16" s="18">
+        <v>33546</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" si="2"/>
-        <v>4589.2794741338803</v>
+        <v>4425</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>103.02652651018913</v>
+        <v>102.52444987775061</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" si="11"/>
-        <v>9503.2794741338803</v>
+        <v>9339</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="12"/>
-        <v>0.39258394159267485</v>
+        <v>0.38579749659189488</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" si="8"/>
-        <v>6.0781168420484311E-2</v>
+        <v>5.3994723419704349E-2</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
@@ -1283,28 +1282,28 @@
         <v>43913</v>
       </c>
       <c r="I17" s="19">
-        <f t="shared" si="16"/>
-        <v>47063.849443285333</v>
+        <f t="shared" ref="I16:I28" si="16">I16*(1+AVERAGE(M12:M16))</f>
+        <v>46788.96272893517</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="2"/>
-        <v>8280.8494432853331</v>
+        <v>8005.9627289351702</v>
       </c>
       <c r="K17" s="8">
         <f t="shared" si="7"/>
-        <v>143.83817067018745</v>
+        <v>142.99805235004638</v>
       </c>
       <c r="L17" s="7">
         <f t="shared" si="11"/>
-        <v>13353.569969151453</v>
+        <v>13242.96272893517</v>
       </c>
       <c r="M17" s="11">
         <f t="shared" si="12"/>
-        <v>0.39612753668796297</v>
+        <v>0.39477024768780689</v>
       </c>
       <c r="N17" s="11">
         <f t="shared" si="8"/>
-        <v>6.4324763515772432E-2</v>
+        <v>6.2967474515616351E-2</v>
       </c>
       <c r="P17" s="20">
         <v>24747</v>
@@ -1340,27 +1339,27 @@
       </c>
       <c r="I18" s="19">
         <f t="shared" si="16"/>
-        <v>65254.297884915744</v>
+        <v>64796.958501456145</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="2"/>
-        <v>13603.297884915744</v>
+        <v>13145.958501456145</v>
       </c>
       <c r="K18" s="8">
         <f t="shared" si="7"/>
-        <v>199.43245074852001</v>
+        <v>198.03471424650411</v>
       </c>
       <c r="L18" s="7">
         <f t="shared" si="11"/>
-        <v>18190.448441630411</v>
+        <v>18007.995772520975</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" si="12"/>
-        <v>0.38650575031162626</v>
+        <v>0.38487700351143911</v>
       </c>
       <c r="N18" s="11">
         <f t="shared" si="8"/>
-        <v>5.4702977139435727E-2</v>
+        <v>5.3074230339248574E-2</v>
       </c>
       <c r="P18" s="20">
         <v>7375</v>
@@ -1396,27 +1395,27 @@
       </c>
       <c r="I19" s="19">
         <f t="shared" si="16"/>
-        <v>89134.510198476695</v>
+        <v>88383.159243591115</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="2"/>
-        <v>20345.510198476695</v>
+        <v>19594.159243591115</v>
       </c>
       <c r="K19" s="8">
         <f t="shared" si="7"/>
-        <v>272.41598471417086</v>
+        <v>270.11967983982612</v>
       </c>
       <c r="L19" s="7">
         <f t="shared" si="11"/>
-        <v>23880.212313560951</v>
+        <v>23586.20074213497</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" si="12"/>
-        <v>0.36595616055323654</v>
+        <v>0.36400166439301207</v>
       </c>
       <c r="N19" s="11">
         <f t="shared" si="8"/>
-        <v>3.4153387381046008E-2</v>
+        <v>3.2198891220821535E-2</v>
       </c>
       <c r="P19" s="21">
         <f>+P18/P17</f>
@@ -1450,27 +1449,27 @@
       </c>
       <c r="I20" s="19">
         <f t="shared" si="16"/>
-        <v>121045.57886735443</v>
+        <v>119817.94311154855</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="2"/>
-        <v>29432.57886735443</v>
+        <v>28204.943111548549</v>
       </c>
       <c r="K20" s="8">
         <f t="shared" si="7"/>
-        <v>369.94370069484853</v>
+        <v>366.19175767588189</v>
       </c>
       <c r="L20" s="7">
         <f t="shared" si="11"/>
-        <v>31911.068668877735</v>
+        <v>31434.783867957434</v>
       </c>
       <c r="M20" s="11">
         <f t="shared" si="12"/>
-        <v>0.35801025436524014</v>
+        <v>0.35566485897297057</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="8"/>
-        <v>2.6207481193049609E-2</v>
+        <v>2.3862085800780031E-2</v>
       </c>
       <c r="P20" s="22">
         <v>409</v>
@@ -1506,27 +1505,27 @@
       </c>
       <c r="I21" s="19">
         <f t="shared" si="16"/>
-        <v>167023.13556818821</v>
+        <v>164991.9741208372</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="2"/>
-        <v>45013.135568188212</v>
+        <v>42981.9741208372</v>
       </c>
       <c r="K21" s="8">
         <f t="shared" si="7"/>
-        <v>510.4619057707464</v>
+        <v>504.25419963581049</v>
       </c>
       <c r="L21" s="7">
         <f t="shared" si="11"/>
-        <v>45977.556700833782</v>
+        <v>45174.03100928865</v>
       </c>
       <c r="M21" s="11">
         <f t="shared" si="12"/>
-        <v>0.37983672870214813</v>
+        <v>0.37702225423142477</v>
       </c>
       <c r="N21" s="11">
         <f t="shared" si="8"/>
-        <v>4.8033955529957595E-2</v>
+        <v>4.5219481059234234E-2</v>
       </c>
       <c r="P21" s="23">
         <f>+P20*P19</f>
@@ -1563,27 +1562,27 @@
       </c>
       <c r="I22" s="19">
         <f t="shared" si="16"/>
-        <v>230038.84110663802</v>
+        <v>226908.05122187958</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="2"/>
-        <v>67545.841106638021</v>
+        <v>64415.051221879577</v>
       </c>
       <c r="K22" s="8">
         <f t="shared" si="7"/>
-        <v>703.05269286869805</v>
+        <v>693.48426412554886</v>
       </c>
       <c r="L22" s="7">
         <f t="shared" si="11"/>
-        <v>63015.705538449809</v>
+        <v>61916.077101042378</v>
       </c>
       <c r="M22" s="11">
         <f t="shared" si="12"/>
-        <v>0.37728728612404278</v>
+        <v>0.3752672057593307</v>
       </c>
       <c r="N22" s="11">
         <f t="shared" si="8"/>
-        <v>4.5484512951852241E-2</v>
+        <v>4.3464432587140167E-2</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
@@ -1613,27 +1612,27 @@
       </c>
       <c r="I23" s="19">
         <f t="shared" si="16"/>
-        <v>315962.77328970481</v>
+        <v>311174.12212083163</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="2"/>
-        <v>99553.773289704812</v>
+        <v>94765.122120831627</v>
       </c>
       <c r="K23" s="8">
         <f t="shared" si="7"/>
-        <v>965.65639758467239</v>
+        <v>951.02115562601352</v>
       </c>
       <c r="L23" s="7">
         <f t="shared" si="11"/>
-        <v>85923.93218306679</v>
+        <v>84266.07089895205</v>
       </c>
       <c r="M23" s="11">
         <f t="shared" si="12"/>
-        <v>0.3735192360112588</v>
+        <v>0.37136659737363564</v>
       </c>
       <c r="N23" s="11">
         <f t="shared" si="8"/>
-        <v>4.1716462839068269E-2</v>
+        <v>3.9563824201445108E-2</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>16</v>
@@ -1673,27 +1672,27 @@
       </c>
       <c r="I24" s="19">
         <f t="shared" si="16"/>
-        <v>433160.29596213182</v>
+        <v>425892.97928968759</v>
       </c>
       <c r="J24" s="7">
         <f t="shared" si="2"/>
-        <v>144946.29596213182</v>
+        <v>137678.97928968759</v>
       </c>
       <c r="K24" s="8">
         <f t="shared" si="7"/>
-        <v>1323.8395353365886</v>
+        <v>1301.6289098095585</v>
       </c>
       <c r="L24" s="7">
         <f t="shared" si="11"/>
-        <v>117197.522672427</v>
+        <v>114718.85716885596</v>
       </c>
       <c r="M24" s="11">
         <f t="shared" si="12"/>
-        <v>0.37092193315118532</v>
+        <v>0.36866451614607471</v>
       </c>
       <c r="N24" s="11">
         <f t="shared" si="8"/>
-        <v>3.9119159978994789E-2</v>
+        <v>3.6861742973884171E-2</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
@@ -1723,27 +1722,27 @@
       </c>
       <c r="I25" s="19">
         <f t="shared" si="16"/>
-        <v>594259.14541038696</v>
+        <v>583301.7835945501</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="2"/>
-        <v>210415.14541038696</v>
+        <v>199457.7835945501</v>
       </c>
       <c r="K25" s="8">
         <f t="shared" si="7"/>
-        <v>1816.1954321833343</v>
+        <v>1782.7071625750309</v>
       </c>
       <c r="L25" s="7">
         <f t="shared" si="11"/>
-        <v>161098.84944825515</v>
+        <v>157408.80430486251</v>
       </c>
       <c r="M25" s="11">
         <f t="shared" si="12"/>
-        <v>0.37191508767077514</v>
+        <v>0.36959708649668727</v>
       </c>
       <c r="N25" s="11">
         <f t="shared" si="8"/>
-        <v>4.01123144985846E-2</v>
+        <v>3.7794313324496731E-2</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1773,27 +1772,27 @@
       </c>
       <c r="I26" s="19">
         <f t="shared" si="16"/>
-        <v>816925.70244629506</v>
+        <v>800513.76199222275</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="2"/>
-        <v>305720.70244629506</v>
+        <v>289308.76199222275</v>
       </c>
       <c r="K26" s="8">
         <f t="shared" si="7"/>
-        <v>2496.716694518017</v>
+        <v>2446.5579522989692</v>
       </c>
       <c r="L26" s="7">
         <f t="shared" si="11"/>
-        <v>222666.5570359081</v>
+        <v>217211.97839767265</v>
       </c>
       <c r="M26" s="11">
         <f t="shared" si="12"/>
-        <v>0.37469605433188197</v>
+        <v>0.37238353200143054</v>
       </c>
       <c r="N26" s="11">
         <f t="shared" si="8"/>
-        <v>4.2893281159691432E-2</v>
+        <v>4.0580758829240005E-2</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1823,27 +1822,27 @@
       </c>
       <c r="I27" s="19">
         <f t="shared" si="16"/>
-        <v>1122184.6300310274</v>
+        <v>1097869.2319020054</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="2"/>
-        <v>441360.63003102737</v>
+        <v>417045.23190200538</v>
       </c>
       <c r="K27" s="8">
         <f t="shared" si="7"/>
-        <v>3429.6596272341912</v>
+        <v>3355.3460632701876</v>
       </c>
       <c r="L27" s="7">
         <f t="shared" si="11"/>
-        <v>305258.9275847323</v>
+        <v>297355.46990978264</v>
       </c>
       <c r="M27" s="11">
         <f t="shared" si="12"/>
-        <v>0.37366791945782868</v>
+        <v>0.37145578755543185</v>
       </c>
       <c r="N27" s="11">
         <f t="shared" si="8"/>
-        <v>4.1865146285638144E-2</v>
+        <v>3.9653014383241314E-2</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1873,27 +1872,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="16"/>
-        <v>1540696.7064536202</v>
+        <v>1504842.2243158473</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="2"/>
-        <v>633973.70645362022</v>
+        <v>598119.22431584727</v>
       </c>
       <c r="K28" s="8">
         <f t="shared" si="7"/>
-        <v>4708.7307654450497</v>
+        <v>4599.1510523100469</v>
       </c>
       <c r="L28" s="7">
         <f t="shared" si="11"/>
-        <v>418512.07642259286</v>
+        <v>406972.99241384189</v>
       </c>
       <c r="M28" s="11">
         <f t="shared" si="12"/>
-        <v>0.37294404612458593</v>
+        <v>0.37069350391465189</v>
       </c>
       <c r="N28" s="11">
         <f t="shared" si="8"/>
-        <v>4.1141272952395391E-2</v>
+        <v>3.8890730742461355E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Jupyter Coronavirus to handle changes in JH data structure, updated excel forecaster
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE8B2CE-8F80-3441-B2D5-03C0DC66D090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EE4E26-8917-6346-B39F-33A49FE067D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -189,7 +189,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -216,6 +216,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -535,7 +539,7 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1183,7 +1187,7 @@
         <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="24">
         <f t="shared" si="0"/>
         <v>43911</v>
       </c>
@@ -1228,30 +1232,30 @@
         <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="24">
         <f t="shared" si="0"/>
         <v>43912</v>
       </c>
       <c r="I16" s="18">
         <v>33546</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="25">
         <f t="shared" si="2"/>
         <v>4425</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="26">
         <f t="shared" si="7"/>
         <v>102.52444987775061</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="25">
         <f t="shared" si="11"/>
         <v>9339</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="27">
         <f t="shared" si="12"/>
         <v>0.38579749659189488</v>
       </c>
-      <c r="N16" s="10">
+      <c r="N16" s="27">
         <f t="shared" si="8"/>
         <v>5.3994723419704349E-2</v>
       </c>
@@ -1277,33 +1281,32 @@
       <c r="F17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="24">
         <f t="shared" si="0"/>
         <v>43913</v>
       </c>
-      <c r="I17" s="19">
-        <f t="shared" ref="I16:I28" si="16">I16*(1+AVERAGE(M12:M16))</f>
-        <v>46788.96272893517</v>
-      </c>
-      <c r="J17" s="7">
-        <f t="shared" si="2"/>
-        <v>8005.9627289351702</v>
-      </c>
-      <c r="K17" s="8">
+      <c r="I17" s="18">
+        <v>43734</v>
+      </c>
+      <c r="J17" s="25">
+        <f t="shared" si="2"/>
+        <v>4951</v>
+      </c>
+      <c r="K17" s="26">
         <f t="shared" si="7"/>
-        <v>142.99805235004638</v>
-      </c>
-      <c r="L17" s="7">
+        <v>133.66136919315403</v>
+      </c>
+      <c r="L17" s="25">
         <f t="shared" si="11"/>
-        <v>13242.96272893517</v>
-      </c>
-      <c r="M17" s="11">
+        <v>10188</v>
+      </c>
+      <c r="M17" s="27">
         <f t="shared" si="12"/>
-        <v>0.39477024768780689</v>
-      </c>
-      <c r="N17" s="11">
+        <v>0.30370237882310858</v>
+      </c>
+      <c r="N17" s="27">
         <f t="shared" si="8"/>
-        <v>6.2967474515616351E-2</v>
+        <v>-2.8100394349081959E-2</v>
       </c>
       <c r="P17" s="20">
         <v>24747</v>
@@ -1314,7 +1317,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <f t="shared" ref="A18:A28" si="17">+A17+1</f>
+        <f t="shared" ref="A18:A28" si="16">+A17+1</f>
         <v>43914</v>
       </c>
       <c r="B18" s="7">
@@ -1333,33 +1336,33 @@
       <c r="F18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="24">
         <f t="shared" si="0"/>
         <v>43914</v>
       </c>
       <c r="I18" s="19">
-        <f t="shared" si="16"/>
-        <v>64796.958501456145</v>
-      </c>
-      <c r="J18" s="7">
-        <f t="shared" si="2"/>
-        <v>13145.958501456145</v>
-      </c>
-      <c r="K18" s="8">
+        <f t="shared" ref="I17:I28" si="17">I17*(1+AVERAGE(M13:M17))</f>
+        <v>59769.658436183534</v>
+      </c>
+      <c r="J18" s="25">
+        <f t="shared" si="2"/>
+        <v>8118.6584361835339</v>
+      </c>
+      <c r="K18" s="26">
         <f t="shared" si="7"/>
-        <v>198.03471424650411</v>
-      </c>
-      <c r="L18" s="7">
+        <v>182.67010524505969</v>
+      </c>
+      <c r="L18" s="25">
         <f t="shared" si="11"/>
-        <v>18007.995772520975</v>
-      </c>
-      <c r="M18" s="11">
+        <v>16035.658436183534</v>
+      </c>
+      <c r="M18" s="27">
         <f t="shared" si="12"/>
-        <v>0.38487700351143911</v>
-      </c>
-      <c r="N18" s="11">
+        <v>0.36666342973849941</v>
+      </c>
+      <c r="N18" s="27">
         <f t="shared" si="8"/>
-        <v>5.3074230339248574E-2</v>
+        <v>3.4860656566308879E-2</v>
       </c>
       <c r="P18" s="20">
         <v>7375</v>
@@ -1370,7 +1373,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43915</v>
       </c>
       <c r="B19" s="7">
@@ -1389,33 +1392,33 @@
       <c r="F19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="24">
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
       <c r="I19" s="19">
-        <f t="shared" si="16"/>
-        <v>88383.159243591115</v>
-      </c>
-      <c r="J19" s="7">
-        <f t="shared" si="2"/>
-        <v>19594.159243591115</v>
-      </c>
-      <c r="K19" s="8">
+        <f t="shared" si="17"/>
+        <v>80219.570687183179</v>
+      </c>
+      <c r="J19" s="25">
+        <f t="shared" si="2"/>
+        <v>11430.570687183179</v>
+      </c>
+      <c r="K19" s="26">
         <f t="shared" si="7"/>
-        <v>270.11967983982612</v>
-      </c>
-      <c r="L19" s="7">
+        <v>245.16983706351826</v>
+      </c>
+      <c r="L19" s="25">
         <f t="shared" si="11"/>
-        <v>23586.20074213497</v>
-      </c>
-      <c r="M19" s="11">
+        <v>20449.912250999645</v>
+      </c>
+      <c r="M19" s="27">
         <f t="shared" si="12"/>
-        <v>0.36400166439301207</v>
-      </c>
-      <c r="N19" s="11">
+        <v>0.34214537586548455</v>
+      </c>
+      <c r="N19" s="27">
         <f t="shared" si="8"/>
-        <v>3.2198891220821535E-2</v>
+        <v>1.0342602693294012E-2</v>
       </c>
       <c r="P19" s="21">
         <f>+P18/P17</f>
@@ -1424,7 +1427,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43916</v>
       </c>
       <c r="B20" s="7">
@@ -1443,33 +1446,33 @@
       <c r="F20" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="24">
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
       <c r="I20" s="19">
-        <f t="shared" si="16"/>
-        <v>119817.94311154855</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" si="2"/>
-        <v>28204.943111548549</v>
-      </c>
-      <c r="K20" s="8">
+        <f t="shared" si="17"/>
+        <v>106646.89048352027</v>
+      </c>
+      <c r="J20" s="25">
+        <f t="shared" si="2"/>
+        <v>15033.89048352027</v>
+      </c>
+      <c r="K20" s="26">
         <f t="shared" si="7"/>
-        <v>366.19175767588189</v>
-      </c>
-      <c r="L20" s="7">
+        <v>325.93792935061208</v>
+      </c>
+      <c r="L20" s="25">
         <f t="shared" si="11"/>
-        <v>31434.783867957434</v>
-      </c>
-      <c r="M20" s="11">
+        <v>26427.319796337091</v>
+      </c>
+      <c r="M20" s="27">
         <f t="shared" si="12"/>
-        <v>0.35566485897297057</v>
-      </c>
-      <c r="N20" s="11">
+        <v>0.32943731273993754</v>
+      </c>
+      <c r="N20" s="27">
         <f t="shared" si="8"/>
-        <v>2.3862085800780031E-2</v>
+        <v>-2.3654604322529971E-3</v>
       </c>
       <c r="P20" s="22">
         <v>409</v>
@@ -1480,7 +1483,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43917</v>
       </c>
       <c r="B21" s="7">
@@ -1499,33 +1502,33 @@
       <c r="F21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="24">
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
       <c r="I21" s="19">
-        <f t="shared" si="16"/>
-        <v>164991.9741208372</v>
-      </c>
-      <c r="J21" s="7">
-        <f t="shared" si="2"/>
-        <v>42981.9741208372</v>
-      </c>
-      <c r="K21" s="8">
+        <f t="shared" si="17"/>
+        <v>143498.63803947007</v>
+      </c>
+      <c r="J21" s="25">
+        <f t="shared" si="2"/>
+        <v>21488.638039470068</v>
+      </c>
+      <c r="K21" s="26">
         <f t="shared" si="7"/>
-        <v>504.25419963581049</v>
-      </c>
-      <c r="L21" s="7">
+        <v>438.56551968053196</v>
+      </c>
+      <c r="L21" s="25">
         <f t="shared" si="11"/>
-        <v>45174.03100928865</v>
-      </c>
-      <c r="M21" s="11">
+        <v>36851.747555949798</v>
+      </c>
+      <c r="M21" s="27">
         <f t="shared" si="12"/>
-        <v>0.37702225423142477</v>
-      </c>
-      <c r="N21" s="11">
+        <v>0.34554919875178502</v>
+      </c>
+      <c r="N21" s="27">
         <f t="shared" si="8"/>
-        <v>4.5219481059234234E-2</v>
+        <v>1.374642557959449E-2</v>
       </c>
       <c r="P21" s="23">
         <f>+P20*P19</f>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43918</v>
       </c>
       <c r="B22" s="7">
@@ -1556,38 +1559,38 @@
       <c r="F22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="24">
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
       <c r="I22" s="19">
-        <f t="shared" si="16"/>
-        <v>226908.05122187958</v>
-      </c>
-      <c r="J22" s="7">
-        <f t="shared" si="2"/>
-        <v>64415.051221879577</v>
-      </c>
-      <c r="K22" s="8">
+        <f t="shared" si="17"/>
+        <v>191929.36225128881</v>
+      </c>
+      <c r="J22" s="25">
+        <f t="shared" si="2"/>
+        <v>29436.362251288811</v>
+      </c>
+      <c r="K22" s="26">
         <f t="shared" si="7"/>
-        <v>693.48426412554886</v>
-      </c>
-      <c r="L22" s="7">
+        <v>586.58118047459914</v>
+      </c>
+      <c r="L22" s="25">
         <f t="shared" si="11"/>
-        <v>61916.077101042378</v>
-      </c>
-      <c r="M22" s="11">
+        <v>48430.724211818742</v>
+      </c>
+      <c r="M22" s="27">
         <f t="shared" si="12"/>
-        <v>0.3752672057593307</v>
-      </c>
-      <c r="N22" s="11">
+        <v>0.33749953918376291</v>
+      </c>
+      <c r="N22" s="27">
         <f t="shared" si="8"/>
-        <v>4.3464432587140167E-2</v>
+        <v>5.6967660115723739E-3</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43919</v>
       </c>
       <c r="B23" s="7">
@@ -1606,33 +1609,33 @@
       <c r="F23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="24">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
       <c r="I23" s="19">
-        <f t="shared" si="16"/>
-        <v>311174.12212083163</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="2"/>
-        <v>94765.122120831627</v>
-      </c>
-      <c r="K23" s="8">
+        <f t="shared" si="17"/>
+        <v>258002.76705371728</v>
+      </c>
+      <c r="J23" s="25">
+        <f t="shared" si="2"/>
+        <v>41593.767053717282</v>
+      </c>
+      <c r="K23" s="26">
         <f t="shared" si="7"/>
-        <v>951.02115562601352</v>
-      </c>
-      <c r="L23" s="7">
+        <v>788.51701422285237</v>
+      </c>
+      <c r="L23" s="25">
         <f t="shared" si="11"/>
-        <v>84266.07089895205</v>
-      </c>
-      <c r="M23" s="11">
+        <v>66073.404802428471</v>
+      </c>
+      <c r="M23" s="27">
         <f t="shared" si="12"/>
-        <v>0.37136659737363564</v>
-      </c>
-      <c r="N23" s="11">
+        <v>0.34425897125589383</v>
+      </c>
+      <c r="N23" s="27">
         <f t="shared" si="8"/>
-        <v>3.9563824201445108E-2</v>
+        <v>1.2456198083703296E-2</v>
       </c>
       <c r="P23" s="13" t="s">
         <v>16</v>
@@ -1647,7 +1650,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43920</v>
       </c>
       <c r="B24" s="7">
@@ -1666,38 +1669,38 @@
       <c r="F24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="24">
         <f t="shared" si="0"/>
         <v>43920</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="16"/>
-        <v>425892.97928968759</v>
-      </c>
-      <c r="J24" s="7">
-        <f t="shared" si="2"/>
-        <v>137678.97928968759</v>
-      </c>
-      <c r="K24" s="8">
+        <f t="shared" si="17"/>
+        <v>345666.45176423353</v>
+      </c>
+      <c r="J24" s="25">
+        <f t="shared" si="2"/>
+        <v>57452.451764233527</v>
+      </c>
+      <c r="K24" s="26">
         <f t="shared" si="7"/>
-        <v>1301.6289098095585</v>
-      </c>
-      <c r="L24" s="7">
+        <v>1056.4378110153837</v>
+      </c>
+      <c r="L24" s="25">
         <f t="shared" si="11"/>
-        <v>114718.85716885596</v>
-      </c>
-      <c r="M24" s="11">
+        <v>87663.684710516245</v>
+      </c>
+      <c r="M24" s="27">
         <f t="shared" si="12"/>
-        <v>0.36866451614607471</v>
-      </c>
-      <c r="N24" s="11">
+        <v>0.33977807955937267</v>
+      </c>
+      <c r="N24" s="27">
         <f t="shared" si="8"/>
-        <v>3.6861742973884171E-2</v>
+        <v>7.975306387182135E-3</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43921</v>
       </c>
       <c r="B25" s="7">
@@ -1716,38 +1719,38 @@
       <c r="F25" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="24">
         <f t="shared" si="0"/>
         <v>43921</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" si="16"/>
-        <v>583301.7835945501</v>
-      </c>
-      <c r="J25" s="7">
-        <f t="shared" si="2"/>
-        <v>199457.7835945501</v>
-      </c>
-      <c r="K25" s="8">
+        <f t="shared" si="17"/>
+        <v>462952.67592990573</v>
+      </c>
+      <c r="J25" s="25">
+        <f t="shared" si="2"/>
+        <v>79108.67592990573</v>
+      </c>
+      <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>1782.7071625750309</v>
-      </c>
-      <c r="L25" s="7">
+        <v>1414.8920413505675</v>
+      </c>
+      <c r="L25" s="25">
         <f t="shared" si="11"/>
-        <v>157408.80430486251</v>
-      </c>
-      <c r="M25" s="11">
+        <v>117286.2241656722</v>
+      </c>
+      <c r="M25" s="27">
         <f t="shared" si="12"/>
-        <v>0.36959708649668727</v>
-      </c>
-      <c r="N25" s="11">
+        <v>0.33930462029815045</v>
+      </c>
+      <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>3.7794313324496731E-2</v>
+        <v>7.5018471259599151E-3</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43922</v>
       </c>
       <c r="B26" s="7">
@@ -1766,38 +1769,38 @@
       <c r="F26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="24">
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="16"/>
-        <v>800513.76199222275</v>
-      </c>
-      <c r="J26" s="7">
-        <f t="shared" si="2"/>
-        <v>289308.76199222275</v>
-      </c>
-      <c r="K26" s="8">
+        <f t="shared" si="17"/>
+        <v>620948.27713997464</v>
+      </c>
+      <c r="J26" s="25">
+        <f t="shared" si="2"/>
+        <v>109743.27713997464</v>
+      </c>
+      <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>2446.5579522989692</v>
-      </c>
-      <c r="L26" s="7">
+        <v>1897.7636831906314</v>
+      </c>
+      <c r="L26" s="25">
         <f t="shared" si="11"/>
-        <v>217211.97839767265</v>
-      </c>
-      <c r="M26" s="11">
+        <v>157995.60121006891</v>
+      </c>
+      <c r="M26" s="27">
         <f t="shared" si="12"/>
-        <v>0.37238353200143054</v>
-      </c>
-      <c r="N26" s="11">
+        <v>0.34127808180979291</v>
+      </c>
+      <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>4.0580758829240005E-2</v>
+        <v>9.4753086376023754E-3</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43923</v>
       </c>
       <c r="B27" s="7">
@@ -1816,38 +1819,38 @@
       <c r="F27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="24">
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
       <c r="I27" s="19">
-        <f t="shared" si="16"/>
-        <v>1097869.2319020054</v>
-      </c>
-      <c r="J27" s="7">
-        <f t="shared" si="2"/>
-        <v>417045.23190200538</v>
-      </c>
-      <c r="K27" s="8">
+        <f t="shared" si="17"/>
+        <v>832333.88552408223</v>
+      </c>
+      <c r="J27" s="25">
+        <f t="shared" si="2"/>
+        <v>151509.88552408223</v>
+      </c>
+      <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>3355.3460632701876</v>
-      </c>
-      <c r="L27" s="7">
+        <v>2543.807718594383</v>
+      </c>
+      <c r="L27" s="25">
         <f t="shared" si="11"/>
-        <v>297355.46990978264</v>
-      </c>
-      <c r="M27" s="11">
+        <v>211385.60838410759</v>
+      </c>
+      <c r="M27" s="27">
         <f t="shared" si="12"/>
-        <v>0.37145578755543185</v>
-      </c>
-      <c r="N27" s="11">
+        <v>0.34042385842139455</v>
+      </c>
+      <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>3.9653014383241314E-2</v>
+        <v>8.6210852492040191E-3</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>43924</v>
       </c>
       <c r="B28" s="7">
@@ -1866,33 +1869,33 @@
       <c r="F28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="24">
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
       <c r="I28" s="19">
-        <f t="shared" si="16"/>
-        <v>1504842.2243158473</v>
-      </c>
-      <c r="J28" s="7">
-        <f t="shared" si="2"/>
-        <v>598119.22431584727</v>
-      </c>
-      <c r="K28" s="8">
+        <f t="shared" si="17"/>
+        <v>1116167.0003277757</v>
+      </c>
+      <c r="J28" s="25">
+        <f t="shared" si="2"/>
+        <v>209444.00032777572</v>
+      </c>
+      <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>4599.1510523100469</v>
-      </c>
-      <c r="L28" s="7">
+        <v>3411.2683384100724</v>
+      </c>
+      <c r="L28" s="25">
         <f t="shared" si="11"/>
-        <v>406972.99241384189</v>
-      </c>
-      <c r="M28" s="11">
+        <v>283833.11480369349</v>
+      </c>
+      <c r="M28" s="27">
         <f t="shared" si="12"/>
-        <v>0.37069350391465189</v>
-      </c>
-      <c r="N28" s="11">
+        <v>0.34100872226892082</v>
+      </c>
+      <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>3.8890730742461355E-2</v>
+        <v>9.2059490967302815E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated metrics for 3-25
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3363F2-6F9A-EA4C-9230-76E3607AF1A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600235A2-B249-1640-99CA-A962D495F2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29500" yWindow="1780" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -996,7 +996,7 @@
         <v>43906</v>
       </c>
       <c r="B11" s="3">
-        <f>ROUND(B10+(B10*$E$10),0)</f>
+        <f t="shared" ref="B11:B40" si="10">ROUND(B10+(B10*$E$10),0)</f>
         <v>5219</v>
       </c>
       <c r="C11" s="5">
@@ -1023,11 +1023,11 @@
         <v>14.25122249388753</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" ref="L11:L29" si="10">IF(I11&lt;=0,0, I11-I10)</f>
+        <f t="shared" ref="L11:L29" si="11">IF(I11&lt;=0,0, I11-I10)</f>
         <v>983</v>
       </c>
       <c r="M11" s="10">
-        <f t="shared" ref="M11:M29" si="11">IF(I11&lt;=0,0, L11/I10)</f>
+        <f t="shared" ref="M11:M29" si="12">IF(I11&lt;=0,0, L11/I10)</f>
         <v>0.26711956521739133</v>
       </c>
       <c r="N11" s="10">
@@ -1037,11 +1037,11 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <f t="shared" ref="A12:A18" si="12">+A11+1</f>
+        <f t="shared" ref="A12:A18" si="13">+A11+1</f>
         <v>43907</v>
       </c>
       <c r="B12" s="3">
-        <f>ROUND(B11+(B11*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>6951</v>
       </c>
       <c r="C12" s="5">
@@ -1049,7 +1049,7 @@
         <v>21.24388753056235</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" ref="E12:E40" si="13">+E11</f>
+        <f t="shared" ref="E12:E40" si="14">+E11</f>
         <v>0.33180277317219053</v>
       </c>
       <c r="H12" s="2">
@@ -1068,11 +1068,11 @@
         <v>19.593520782396091</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1748</v>
       </c>
       <c r="M12" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.37486596611623418</v>
       </c>
       <c r="N12" s="10">
@@ -1082,11 +1082,11 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43908</v>
       </c>
       <c r="B13" s="3">
-        <f>ROUND(B12+(B12*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>9257</v>
       </c>
       <c r="C13" s="5">
@@ -1094,7 +1094,7 @@
         <v>28.291564792176036</v>
       </c>
       <c r="E13" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="H13" s="2">
@@ -1113,11 +1113,11 @@
         <v>28.297677261613689</v>
       </c>
       <c r="L13" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2848</v>
       </c>
       <c r="M13" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44423646856964594</v>
       </c>
       <c r="N13" s="10">
@@ -1127,11 +1127,11 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43909</v>
       </c>
       <c r="B14" s="3">
-        <f>ROUND(B13+(B13*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>12328</v>
       </c>
       <c r="C14" s="5">
@@ -1139,7 +1139,7 @@
         <v>37.677261613691932</v>
       </c>
       <c r="E14" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="H14" s="2">
@@ -1158,11 +1158,11 @@
         <v>42.142420537897308</v>
       </c>
       <c r="L14" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4530</v>
       </c>
       <c r="M14" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.48925369910357491</v>
       </c>
       <c r="N14" s="10">
@@ -1172,11 +1172,11 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43910</v>
       </c>
       <c r="B15" s="3">
-        <f>ROUND(B14+(B14*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>16418</v>
       </c>
       <c r="C15" s="5">
@@ -1184,7 +1184,7 @@
         <v>50.177261613691932</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="H15" s="2">
@@ -1195,7 +1195,7 @@
         <v>19383</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" ref="J15" si="14">IF(I15&lt;=0,0, I15-B15)</f>
+        <f t="shared" ref="J15" si="15">IF(I15&lt;=0,0, I15-B15)</f>
         <v>2965</v>
       </c>
       <c r="K15" s="5">
@@ -1203,11 +1203,11 @@
         <v>59.238997555012226</v>
       </c>
       <c r="L15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5594</v>
       </c>
       <c r="M15" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.40568569149321926</v>
       </c>
       <c r="N15" s="10">
@@ -1223,11 +1223,11 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43911</v>
       </c>
       <c r="B16" s="3">
-        <f>ROUND(B15+(B15*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>21866</v>
       </c>
       <c r="C16" s="5">
@@ -1235,7 +1235,7 @@
         <v>66.827628361858189</v>
       </c>
       <c r="E16" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="H16" s="24">
@@ -1254,11 +1254,11 @@
         <v>73.982273838630803</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4824</v>
       </c>
       <c r="M16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.24887788268069957</v>
       </c>
       <c r="N16" s="10">
@@ -1268,11 +1268,11 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43912</v>
       </c>
       <c r="B17" s="3">
-        <f>ROUND(B16+(B16*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>29121</v>
       </c>
       <c r="C17" s="5">
@@ -1280,7 +1280,7 @@
         <v>89.000611246943762</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="H17" s="24">
@@ -1299,11 +1299,11 @@
         <v>102.52444987775061</v>
       </c>
       <c r="L17" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9339</v>
       </c>
       <c r="M17" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.38579749659189488</v>
       </c>
       <c r="N17" s="27">
@@ -1313,11 +1313,11 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>43913</v>
       </c>
       <c r="B18" s="7">
-        <f>ROUND(B17+(B17*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>38783</v>
       </c>
       <c r="C18" s="8">
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -1348,11 +1348,11 @@
         <v>133.66136919315403</v>
       </c>
       <c r="L18" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>10188</v>
       </c>
       <c r="M18" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.30370237882310858</v>
       </c>
       <c r="N18" s="27">
@@ -1368,11 +1368,11 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <f t="shared" ref="A19:A40" si="15">+A18+1</f>
+        <f t="shared" ref="A19:A40" si="16">+A18+1</f>
         <v>43914</v>
       </c>
       <c r="B19" s="7">
-        <f>ROUND(B18+(B18*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>51651</v>
       </c>
       <c r="C19" s="8">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1403,11 +1403,11 @@
         <v>167.6528117359413</v>
       </c>
       <c r="L19" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11122</v>
       </c>
       <c r="M19" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25431014771116295</v>
       </c>
       <c r="N19" s="27">
@@ -1423,11 +1423,11 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43915</v>
       </c>
       <c r="B20" s="7">
-        <f>ROUND(B19+(B19*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>68789</v>
       </c>
       <c r="C20" s="8">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F20" s="12" t="s">
@@ -1446,29 +1446,28 @@
         <f t="shared" si="0"/>
         <v>43915</v>
       </c>
-      <c r="I20" s="19">
-        <f>I19*(1+AVERAGE(M17:M19))</f>
-        <v>72113.880876202995</v>
+      <c r="I20" s="18">
+        <v>68211</v>
       </c>
       <c r="J20" s="25">
         <f t="shared" si="2"/>
-        <v>3324.8808762029948</v>
+        <v>-578</v>
       </c>
       <c r="K20" s="26">
         <f t="shared" si="7"/>
-        <v>220.39694644316319</v>
+        <v>208.46882640586799</v>
       </c>
       <c r="L20" s="25">
-        <f t="shared" si="10"/>
-        <v>17257.880876202995</v>
+        <f t="shared" si="11"/>
+        <v>13355</v>
       </c>
       <c r="M20" s="27">
-        <f t="shared" si="11"/>
-        <v>0.31460334104205545</v>
+        <f t="shared" si="12"/>
+        <v>0.24345559282485052</v>
       </c>
       <c r="N20" s="27">
         <f t="shared" si="8"/>
-        <v>-1.7199432130135084E-2</v>
+        <v>-8.8347180347340015E-2</v>
       </c>
       <c r="P20" s="21">
         <f>+P19/P18</f>
@@ -1477,11 +1476,11 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43916</v>
       </c>
       <c r="B21" s="7">
-        <f>ROUND(B20+(B20*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>91613</v>
       </c>
       <c r="C21" s="8">
@@ -1490,7 +1489,7 @@
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -1501,28 +1500,28 @@
         <v>43916</v>
       </c>
       <c r="I21" s="19">
-        <f t="shared" ref="I21:I29" si="16">I20*(1+AVERAGE(M18:M20))</f>
-        <v>93089.786451230917</v>
+        <f t="shared" ref="I21:I29" si="17">I20*(1+AVERAGE(M18:M20))</f>
+        <v>86433.980629868354</v>
       </c>
       <c r="J21" s="25">
         <f t="shared" si="2"/>
-        <v>1476.786451230917</v>
+        <v>-5179.0193701316457</v>
       </c>
       <c r="K21" s="26">
         <f t="shared" si="7"/>
-        <v>284.50423732038786</v>
+        <v>264.16253248737274</v>
       </c>
       <c r="L21" s="25">
-        <f t="shared" si="10"/>
-        <v>20975.905575027922</v>
+        <f t="shared" si="11"/>
+        <v>18222.980629868354</v>
       </c>
       <c r="M21" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29087195585877562</v>
+        <f t="shared" si="12"/>
+        <v>0.26715603978637398</v>
       </c>
       <c r="N21" s="27">
         <f t="shared" si="8"/>
-        <v>-4.0930817313414913E-2</v>
+        <v>-6.4646733385816557E-2</v>
       </c>
       <c r="P21" s="22">
         <v>409</v>
@@ -1533,11 +1532,11 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43917</v>
       </c>
       <c r="B22" s="7">
-        <f>ROUND(B21+(B21*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>122010</v>
       </c>
       <c r="C22" s="8">
@@ -1546,7 +1545,7 @@
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -1557,28 +1556,28 @@
         <v>43917</v>
       </c>
       <c r="I22" s="19">
-        <f t="shared" si="16"/>
-        <v>119768.86759549996</v>
+        <f t="shared" si="17"/>
+        <v>108472.3920777849</v>
       </c>
       <c r="J22" s="25">
         <f t="shared" si="2"/>
-        <v>-2241.1324045000365</v>
+        <v>-13537.607922215102</v>
       </c>
       <c r="K22" s="26">
         <f t="shared" si="7"/>
-        <v>366.04177137988989</v>
+        <v>331.51709070227656</v>
       </c>
       <c r="L22" s="25">
-        <f t="shared" si="10"/>
-        <v>26679.081144269046</v>
+        <f t="shared" si="11"/>
+        <v>22038.411447916544</v>
       </c>
       <c r="M22" s="27">
-        <f t="shared" si="11"/>
-        <v>0.28659514820399795</v>
+        <f t="shared" si="12"/>
+        <v>0.25497392677412906</v>
       </c>
       <c r="N22" s="27">
         <f t="shared" si="8"/>
-        <v>-4.5207624968192583E-2</v>
+        <v>-7.6828846398061479E-2</v>
       </c>
       <c r="P22" s="23">
         <f>+P21*P20</f>
@@ -1590,11 +1589,11 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43918</v>
       </c>
       <c r="B23" s="7">
-        <f>ROUND(B22+(B22*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>162493</v>
       </c>
       <c r="C23" s="8">
@@ -1603,7 +1602,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -1614,37 +1613,37 @@
         <v>43918</v>
       </c>
       <c r="I23" s="19">
-        <f t="shared" si="16"/>
-        <v>155382.95660403962</v>
+        <f t="shared" si="17"/>
+        <v>136154.02440003102</v>
       </c>
       <c r="J23" s="25">
         <f t="shared" si="2"/>
-        <v>-7110.0433959603834</v>
+        <v>-26338.975599968981</v>
       </c>
       <c r="K23" s="26">
         <f t="shared" si="7"/>
-        <v>474.88678668716261</v>
+        <v>416.11865647931239</v>
       </c>
       <c r="L23" s="25">
-        <f t="shared" si="10"/>
-        <v>35614.089008539653</v>
+        <f t="shared" si="11"/>
+        <v>27681.632322246121</v>
       </c>
       <c r="M23" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29735681503494293</v>
+        <f t="shared" si="12"/>
+        <v>0.25519518646178457</v>
       </c>
       <c r="N23" s="27">
         <f t="shared" si="8"/>
-        <v>-3.4445958137247601E-2</v>
+        <v>-7.6607586710405962E-2</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43919</v>
       </c>
       <c r="B24" s="7">
-        <f>ROUND(B23+(B23*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>216409</v>
       </c>
       <c r="C24" s="8">
@@ -1653,7 +1652,7 @@
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F24" s="12" t="s">
@@ -1664,28 +1663,28 @@
         <v>43919</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="16"/>
-        <v>200693.86562315174</v>
+        <f t="shared" si="17"/>
+        <v>171432.67368381581</v>
       </c>
       <c r="J24" s="25">
         <f t="shared" si="2"/>
-        <v>-15715.134376848262</v>
+        <v>-44976.32631618419</v>
       </c>
       <c r="K24" s="26">
         <f t="shared" si="7"/>
-        <v>613.36755997295768</v>
+        <v>523.93848925371583</v>
       </c>
       <c r="L24" s="25">
-        <f t="shared" si="10"/>
-        <v>45310.909019112121</v>
+        <f t="shared" si="11"/>
+        <v>35278.649283784791</v>
       </c>
       <c r="M24" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29160797303257219</v>
+        <f t="shared" si="12"/>
+        <v>0.2591083843407625</v>
       </c>
       <c r="N24" s="27">
         <f t="shared" si="8"/>
-        <v>-4.0194800139618347E-2</v>
+        <v>-7.2694388831428036E-2</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>16</v>
@@ -1700,11 +1699,11 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43920</v>
       </c>
       <c r="B25" s="7">
-        <f>ROUND(B24+(B24*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>288214</v>
       </c>
       <c r="C25" s="8">
@@ -1713,7 +1712,7 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -1724,37 +1723,37 @@
         <v>43920</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" si="16"/>
-        <v>259267.03502151521</v>
+        <f t="shared" si="17"/>
+        <v>215392.43975527069</v>
       </c>
       <c r="J25" s="25">
         <f t="shared" si="2"/>
-        <v>-28946.964978484786</v>
+        <v>-72821.560244729306</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>792.38091387993643</v>
+        <v>658.28985255278326</v>
       </c>
       <c r="L25" s="25">
-        <f t="shared" si="10"/>
-        <v>58573.169398363476</v>
+        <f t="shared" si="11"/>
+        <v>43959.766071454884</v>
       </c>
       <c r="M25" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29185331209050452</v>
+        <f t="shared" si="12"/>
+        <v>0.25642583252555856</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>-3.9949461081686011E-2</v>
+        <v>-7.5376940646631974E-2</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43921</v>
       </c>
       <c r="B26" s="7">
-        <f>ROUND(B25+(B25*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>383844</v>
       </c>
       <c r="C26" s="8">
@@ -1763,7 +1762,7 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F26" s="12" t="s">
@@ -1774,37 +1773,37 @@
         <v>43921</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="16"/>
-        <v>335389.40076193312</v>
+        <f t="shared" si="17"/>
+        <v>270728.86861325894</v>
       </c>
       <c r="J26" s="25">
         <f t="shared" si="2"/>
-        <v>-48454.599238066876</v>
+        <v>-113115.13138674106</v>
       </c>
       <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>1025.0287309350033</v>
+        <v>827.41096764443444</v>
       </c>
       <c r="L26" s="25">
-        <f t="shared" si="10"/>
-        <v>76122.36574041791</v>
+        <f t="shared" si="11"/>
+        <v>55336.428857988241</v>
       </c>
       <c r="M26" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29360603338600649</v>
+        <f t="shared" si="12"/>
+        <v>0.25690980110936856</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>-3.8196739786184042E-2</v>
+        <v>-7.4892972062821972E-2</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43922</v>
       </c>
       <c r="B27" s="7">
-        <f>ROUND(B26+(B26*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>511205</v>
       </c>
       <c r="C27" s="8">
@@ -1813,7 +1812,7 @@
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F27" s="12" t="s">
@@ -1824,37 +1823,37 @@
         <v>43922</v>
       </c>
       <c r="I27" s="19">
-        <f t="shared" si="16"/>
-        <v>433442.42822281213</v>
+        <f t="shared" si="17"/>
+        <v>340436.50029780506</v>
       </c>
       <c r="J27" s="25">
         <f t="shared" si="2"/>
-        <v>-77762.57177718787</v>
+        <v>-170768.49970219494</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>1324.7017977469809</v>
+        <v>1040.4538517659078</v>
       </c>
       <c r="L27" s="25">
-        <f t="shared" si="10"/>
-        <v>98053.027460879006</v>
+        <f t="shared" si="11"/>
+        <v>69707.631684546126</v>
       </c>
       <c r="M27" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29235577283636116</v>
+        <f t="shared" si="12"/>
+        <v>0.25748133932522999</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>-3.9447000335829374E-2</v>
+        <v>-7.432143384696055E-2</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43923</v>
       </c>
       <c r="B28" s="7">
-        <f>ROUND(B27+(B27*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>680824</v>
       </c>
       <c r="C28" s="8">
@@ -1863,7 +1862,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F28" s="12" t="s">
@@ -1874,37 +1873,37 @@
         <v>43923</v>
       </c>
       <c r="I28" s="19">
-        <f t="shared" si="16"/>
-        <v>560269.8670268876</v>
+        <f t="shared" si="17"/>
+        <v>427907.91117937298</v>
       </c>
       <c r="J28" s="25">
         <f t="shared" si="2"/>
-        <v>-120554.1329731124</v>
+        <v>-252916.08882062702</v>
       </c>
       <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>1712.3162195198277</v>
+        <v>1307.7870146068858</v>
       </c>
       <c r="L28" s="25">
-        <f t="shared" si="10"/>
-        <v>126827.43880407547</v>
+        <f t="shared" si="11"/>
+        <v>87471.410881567921</v>
       </c>
       <c r="M28" s="27">
-        <f t="shared" si="11"/>
-        <v>0.29260503943762406</v>
+        <f t="shared" si="12"/>
+        <v>0.25693899098671907</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>-3.9197733734566476E-2</v>
+        <v>-7.4863782185471461E-2</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43924</v>
       </c>
       <c r="B29" s="7">
-        <f>ROUND(B28+(B28*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>906723</v>
       </c>
       <c r="C29" s="8">
@@ -1913,7 +1912,7 @@
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F29" s="12" t="s">
@@ -1924,578 +1923,578 @@
         <v>43924</v>
       </c>
       <c r="I29" s="19">
-        <f t="shared" si="16"/>
-        <v>724348.0436242728</v>
+        <f t="shared" si="17"/>
+        <v>537927.33296810871</v>
       </c>
       <c r="J29" s="25">
         <f t="shared" si="2"/>
-        <v>-182374.9563757272</v>
+        <v>-368795.66703189129</v>
       </c>
       <c r="K29" s="26">
         <f t="shared" si="7"/>
-        <v>2213.7776394384869</v>
+        <v>1644.0321912228262</v>
       </c>
       <c r="L29" s="25">
-        <f t="shared" si="10"/>
-        <v>164078.1765973852</v>
+        <f t="shared" si="11"/>
+        <v>110019.42178873572</v>
       </c>
       <c r="M29" s="27">
-        <f t="shared" si="11"/>
-        <v>0.2928556152199972</v>
+        <f t="shared" si="12"/>
+        <v>0.25711004380710578</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="8"/>
-        <v>-3.8947157952193334E-2</v>
+        <v>-7.4692729365084753E-2</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43925</v>
       </c>
       <c r="B30" s="7">
-        <f>ROUND(B29+(B29*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>1207576</v>
       </c>
       <c r="C30" s="8">
-        <f>+B30/$P$15*1000000</f>
+        <f t="shared" ref="C30:C40" si="18">+B30/$P$15*1000000</f>
         <v>3690.6356968215155</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H30" s="24">
-        <f t="shared" ref="H30:H40" si="17">A30</f>
+        <f t="shared" ref="H30:H40" si="19">A30</f>
         <v>43925</v>
       </c>
       <c r="I30" s="19">
-        <f t="shared" ref="I30:I40" si="18">I29*(1+AVERAGE(M27:M29))</f>
-        <v>936296.24759644433</v>
+        <f t="shared" ref="I30:I40" si="20">I29*(1+AVERAGE(M27:M29))</f>
+        <v>676269.75845269219</v>
       </c>
       <c r="J30" s="25">
-        <f t="shared" ref="J30:J40" si="19">IF(I30&lt;=0,0, I30-B30)</f>
-        <v>-271279.75240355567</v>
+        <f t="shared" ref="J30:J40" si="21">IF(I30&lt;=0,0, I30-B30)</f>
+        <v>-531306.24154730781</v>
       </c>
       <c r="K30" s="26">
-        <f>IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
-        <v>2861.5410990111377</v>
+        <f t="shared" ref="K30:K40" si="22">IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
+        <v>2066.8391150754651</v>
       </c>
       <c r="L30" s="25">
-        <f t="shared" ref="L30:L40" si="20">IF(I30&lt;=0,0, I30-I29)</f>
-        <v>211948.20397217153</v>
+        <f t="shared" ref="L30:L40" si="23">IF(I30&lt;=0,0, I30-I29)</f>
+        <v>138342.42548458348</v>
       </c>
       <c r="M30" s="27">
-        <f t="shared" ref="M30:M40" si="21">IF(I30&lt;=0,0, L30/I29)</f>
-        <v>0.29260547583132751</v>
+        <f t="shared" ref="M30:M40" si="24">IF(I30&lt;=0,0, L30/I29)</f>
+        <v>0.25717679137301835</v>
       </c>
       <c r="N30" s="27">
-        <f t="shared" ref="N30:N40" si="22">IF(I30&lt;=0,0,M30-E30)</f>
-        <v>-3.9197297340863024E-2</v>
+        <f t="shared" ref="N30:N40" si="25">IF(I30&lt;=0,0,M30-E30)</f>
+        <v>-7.4625981799172181E-2</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43926</v>
       </c>
       <c r="B31" s="7">
-        <f>ROUND(B30+(B30*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>1608253</v>
       </c>
       <c r="C31" s="8">
-        <f>+B31/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>4915.1986552567241</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H31" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43926</v>
       </c>
       <c r="I31" s="19">
-        <f t="shared" si="18"/>
-        <v>1210339.5886358884</v>
+        <f t="shared" si="20"/>
+        <v>850121.99284413527</v>
       </c>
       <c r="J31" s="25">
-        <f t="shared" si="19"/>
-        <v>-397913.41136411158</v>
+        <f t="shared" si="21"/>
+        <v>-758131.00715586473</v>
       </c>
       <c r="K31" s="26">
-        <f>IF(I31&lt;=0,0, I31/$P$15*1000000)</f>
-        <v>3699.0818723590719</v>
+        <f t="shared" si="22"/>
+        <v>2598.1723497681396</v>
       </c>
       <c r="L31" s="25">
-        <f t="shared" si="20"/>
-        <v>274043.34103944409</v>
+        <f t="shared" si="23"/>
+        <v>173852.23439144308</v>
       </c>
       <c r="M31" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29268871016298281</v>
+        <f t="shared" si="24"/>
+        <v>0.25707527538894787</v>
       </c>
       <c r="N31" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9114063009207722E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4727497783242669E-2</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43927</v>
       </c>
       <c r="B32" s="7">
-        <f>ROUND(B31+(B31*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>2141876</v>
       </c>
       <c r="C32" s="8">
-        <f>+B32/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>6546.0757946210269</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H32" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43927</v>
       </c>
       <c r="I32" s="19">
-        <f t="shared" si="18"/>
-        <v>1564626.0783566926</v>
+        <f t="shared" si="20"/>
+        <v>1068705.9577246145</v>
       </c>
       <c r="J32" s="25">
-        <f t="shared" si="19"/>
-        <v>-577249.92164330743</v>
+        <f t="shared" si="21"/>
+        <v>-1073170.0422753855</v>
       </c>
       <c r="K32" s="26">
-        <f>IF(I32&lt;=0,0, I32/$P$15*1000000)</f>
-        <v>4781.8645426549283</v>
+        <f t="shared" si="22"/>
+        <v>3266.2162522145923</v>
       </c>
       <c r="L32" s="25">
-        <f t="shared" si="20"/>
-        <v>354286.48972080415</v>
+        <f t="shared" si="23"/>
+        <v>218583.96488047927</v>
       </c>
       <c r="M32" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29271660040476927</v>
+        <f t="shared" si="24"/>
+        <v>0.25712070352302402</v>
       </c>
       <c r="N32" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9086172767421268E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4682069649166516E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43928</v>
       </c>
       <c r="B33" s="7">
-        <f>ROUND(B32+(B32*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>2852556</v>
       </c>
       <c r="C33" s="8">
-        <f>+B33/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>8718.0806845965762</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43928</v>
       </c>
       <c r="I33" s="19">
-        <f t="shared" si="18"/>
-        <v>2022545.6028495152</v>
+        <f t="shared" si="20"/>
+        <v>1343496.1828013177</v>
       </c>
       <c r="J33" s="25">
-        <f t="shared" si="19"/>
-        <v>-830010.39715048485</v>
+        <f t="shared" si="21"/>
+        <v>-1509059.8171986823</v>
       </c>
       <c r="K33" s="26">
-        <f>IF(I33&lt;=0,0, I33/$P$15*1000000)</f>
-        <v>6181.3740918383719</v>
+        <f t="shared" si="22"/>
+        <v>4106.0396784881341</v>
       </c>
       <c r="L33" s="25">
-        <f t="shared" si="20"/>
-        <v>457919.52449282259</v>
+        <f t="shared" si="23"/>
+        <v>274790.22507670312</v>
       </c>
       <c r="M33" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29267026213302655</v>
+        <f t="shared" si="24"/>
+        <v>0.25712425676166334</v>
       </c>
       <c r="N33" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9132511039163986E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4678516410527196E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43929</v>
       </c>
       <c r="B34" s="7">
-        <f>ROUND(B33+(B33*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>3799042</v>
       </c>
       <c r="C34" s="8">
-        <f>+B34/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>11610.764058679706</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H34" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43929</v>
       </c>
       <c r="I34" s="19">
-        <f t="shared" si="18"/>
-        <v>2614528.2323613581</v>
+        <f t="shared" si="20"/>
+        <v>1688918.1135829648</v>
       </c>
       <c r="J34" s="25">
-        <f t="shared" si="19"/>
-        <v>-1184513.7676386419</v>
+        <f t="shared" si="21"/>
+        <v>-2110123.886417035</v>
       </c>
       <c r="K34" s="26">
-        <f>IF(I34&lt;=0,0, I34/$P$15*1000000)</f>
-        <v>7990.6119570946148</v>
+        <f t="shared" si="22"/>
+        <v>5161.7301759870561</v>
       </c>
       <c r="L34" s="25">
-        <f t="shared" si="20"/>
-        <v>591982.62951184297</v>
+        <f t="shared" si="23"/>
+        <v>345421.9307816471</v>
       </c>
       <c r="M34" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29269185756692612</v>
+        <f t="shared" si="24"/>
+        <v>0.25710674522454496</v>
       </c>
       <c r="N34" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9110915605264418E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4696027947645571E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43930</v>
       </c>
       <c r="B35" s="7">
-        <f>ROUND(B34+(B34*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>5059575</v>
       </c>
       <c r="C35" s="8">
-        <f>+B35/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>15463.248777506113</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H35" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43930</v>
       </c>
       <c r="I35" s="19">
-        <f t="shared" si="18"/>
-        <v>3379782.1003445322</v>
+        <f t="shared" si="20"/>
+        <v>2123168.0693755164</v>
       </c>
       <c r="J35" s="25">
-        <f t="shared" si="19"/>
-        <v>-1679792.8996554678</v>
+        <f t="shared" si="21"/>
+        <v>-2936406.9306244836</v>
       </c>
       <c r="K35" s="26">
-        <f>IF(I35&lt;=0,0, I35/$P$15*1000000)</f>
-        <v>10329.407397140991</v>
+        <f t="shared" si="22"/>
+        <v>6488.8999675290843</v>
       </c>
       <c r="L35" s="25">
-        <f t="shared" si="20"/>
-        <v>765253.86798317404</v>
+        <f t="shared" si="23"/>
+        <v>434249.95579255163</v>
       </c>
       <c r="M35" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29269290670157394</v>
+        <f t="shared" si="24"/>
+        <v>0.25711723516974405</v>
       </c>
       <c r="N35" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9109866470616594E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4685538002446483E-2</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43931</v>
       </c>
       <c r="B36" s="7">
-        <f>ROUND(B35+(B35*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>6738356</v>
       </c>
       <c r="C36" s="8">
-        <f>+B36/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>20593.997555012225</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F36" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H36" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43931</v>
       </c>
       <c r="I36" s="19">
-        <f t="shared" si="18"/>
-        <v>4368993.6541276742</v>
+        <f t="shared" si="20"/>
+        <v>2669068.7185417204</v>
       </c>
       <c r="J36" s="25">
-        <f t="shared" si="19"/>
-        <v>-2369362.3458723258</v>
+        <f t="shared" si="21"/>
+        <v>-4069287.2814582796</v>
       </c>
       <c r="K36" s="26">
-        <f>IF(I36&lt;=0,0, I36/$P$15*1000000)</f>
-        <v>13352.670092077244</v>
+        <f t="shared" si="22"/>
+        <v>8157.3004845407104</v>
       </c>
       <c r="L36" s="25">
-        <f t="shared" si="20"/>
-        <v>989211.55378314201</v>
+        <f t="shared" si="23"/>
+        <v>545900.64916620404</v>
       </c>
       <c r="M36" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29268500880050896</v>
+        <f t="shared" si="24"/>
+        <v>0.25711607905198425</v>
       </c>
       <c r="N36" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9117764371681574E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4686694120206287E-2</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43932</v>
       </c>
       <c r="B37" s="7">
-        <f>ROUND(B36+(B36*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>8974161</v>
       </c>
       <c r="C37" s="8">
-        <f>+B37/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>27427.142420537897</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H37" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43932</v>
       </c>
       <c r="I37" s="19">
-        <f t="shared" si="18"/>
-        <v>5647754.0762676168</v>
+        <f t="shared" si="20"/>
+        <v>3355321.92655044</v>
       </c>
       <c r="J37" s="25">
-        <f t="shared" si="19"/>
-        <v>-3326406.9237323832</v>
+        <f t="shared" si="21"/>
+        <v>-5618839.0734495595</v>
       </c>
       <c r="K37" s="26">
-        <f>IF(I37&lt;=0,0, I37/$P$15*1000000)</f>
-        <v>17260.862091282448</v>
+        <f t="shared" si="22"/>
+        <v>10254.651364762958</v>
       </c>
       <c r="L37" s="25">
-        <f t="shared" si="20"/>
-        <v>1278760.4221399426</v>
+        <f t="shared" si="23"/>
+        <v>686253.20800871961</v>
       </c>
       <c r="M37" s="27">
-        <f t="shared" si="21"/>
-        <v>0.2926899243563364</v>
+        <f t="shared" si="24"/>
+        <v>0.25711335314875772</v>
       </c>
       <c r="N37" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.911284881585414E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4689420023432818E-2</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43933</v>
       </c>
       <c r="B38" s="7">
-        <f>ROUND(B37+(B37*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>11951813</v>
       </c>
       <c r="C38" s="8">
-        <f>+B38/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>36527.545843520784</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F38" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43933</v>
       </c>
       <c r="I38" s="19">
-        <f t="shared" si="18"/>
-        <v>7300791.1502009137</v>
+        <f t="shared" si="20"/>
+        <v>4218027.3885503737</v>
       </c>
       <c r="J38" s="25">
-        <f t="shared" si="19"/>
-        <v>-4651021.8497990863</v>
+        <f t="shared" si="21"/>
+        <v>-7733785.6114496263</v>
       </c>
       <c r="K38" s="26">
-        <f>IF(I38&lt;=0,0, I38/$P$15*1000000)</f>
-        <v>22312.9313881446</v>
+        <f t="shared" si="22"/>
+        <v>12891.281749848331</v>
       </c>
       <c r="L38" s="25">
-        <f t="shared" si="20"/>
-        <v>1653037.0739332968</v>
+        <f t="shared" si="23"/>
+        <v>862705.4619999337</v>
       </c>
       <c r="M38" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29268927995280652</v>
+        <f t="shared" si="24"/>
+        <v>0.25711555579016204</v>
       </c>
       <c r="N38" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.911349321938401E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4687217382028492E-2</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43934</v>
       </c>
       <c r="B39" s="7">
-        <f>ROUND(B38+(B38*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>15917458</v>
       </c>
       <c r="C39" s="8">
-        <f>+B39/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>48647.487775061119</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H39" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43934</v>
       </c>
       <c r="I39" s="19">
-        <f t="shared" si="18"/>
-        <v>9437645.6289939396</v>
+        <f t="shared" si="20"/>
+        <v>5302545.4836726049</v>
       </c>
       <c r="J39" s="25">
-        <f t="shared" si="19"/>
-        <v>-6479812.3710060604</v>
+        <f t="shared" si="21"/>
+        <v>-10614912.516327396</v>
       </c>
       <c r="K39" s="26">
-        <f>IF(I39&lt;=0,0, I39/$P$15*1000000)</f>
-        <v>28843.660235311552</v>
+        <f t="shared" si="22"/>
+        <v>16205.823605356371</v>
       </c>
       <c r="L39" s="25">
-        <f t="shared" si="20"/>
-        <v>2136854.4787930259</v>
+        <f t="shared" si="23"/>
+        <v>1084518.0951222312</v>
       </c>
       <c r="M39" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29268807103655076</v>
+        <f t="shared" si="24"/>
+        <v>0.25711499599696813</v>
       </c>
       <c r="N39" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9114702135639778E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4687777175222403E-2</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>43935</v>
       </c>
       <c r="B40" s="7">
-        <f>ROUND(B39+(B39*$E$10),0)</f>
+        <f t="shared" si="10"/>
         <v>21198915</v>
       </c>
       <c r="C40" s="8">
-        <f>+B40/$P$15*1000000</f>
+        <f t="shared" si="18"/>
         <v>64788.860024449874</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.33180277317219053</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>43935</v>
       </c>
       <c r="I40" s="19">
-        <f t="shared" si="18"/>
-        <v>12199941.556703573</v>
+        <f t="shared" si="20"/>
+        <v>6665907.5301646665</v>
       </c>
       <c r="J40" s="25">
-        <f t="shared" si="19"/>
-        <v>-8998973.4432964269</v>
+        <f t="shared" si="21"/>
+        <v>-14533007.469835334</v>
       </c>
       <c r="K40" s="26">
-        <f>IF(I40&lt;=0,0, I40/$P$15*1000000)</f>
-        <v>37285.884953250534</v>
+        <f t="shared" si="22"/>
+        <v>20372.57802617563</v>
       </c>
       <c r="L40" s="25">
-        <f t="shared" si="20"/>
-        <v>2762295.9277096335</v>
+        <f t="shared" si="23"/>
+        <v>1363362.0464920616</v>
       </c>
       <c r="M40" s="27">
-        <f t="shared" si="21"/>
-        <v>0.29268909178189778</v>
+        <f t="shared" si="24"/>
+        <v>0.25711463497862935</v>
       </c>
       <c r="N40" s="27">
-        <f t="shared" si="22"/>
-        <v>-3.9113681390292754E-2</v>
+        <f t="shared" si="25"/>
+        <v>-7.4688138193561182E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stats for Mar 27
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600235A2-B249-1640-99CA-A962D495F2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2FE235-085F-A341-8FD8-F8468C2CC1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>US Population</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>ACTUAL STATS - UPDATED DAILY</t>
+  </si>
+  <si>
+    <t>EASTER SUNDAY - THE DAY TRUMP WANTS CORONAVIRUS TO BE DONE</t>
   </si>
 </sst>
 </file>
@@ -574,11 +577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0A91CA-B277-40C5-9F76-C8642C725AE7}">
-  <dimension ref="A1:W40"/>
+  <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,7 +598,7 @@
     <col min="11" max="11" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="3" customWidth="1"/>
     <col min="15" max="15" width="4.83203125" customWidth="1"/>
     <col min="16" max="16" width="11.5" customWidth="1"/>
     <col min="17" max="17" width="12.5" customWidth="1"/>
@@ -996,7 +999,7 @@
         <v>43906</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" ref="B11:B40" si="10">ROUND(B10+(B10*$E$10),0)</f>
+        <f t="shared" ref="B11:B41" si="10">ROUND(B10+(B10*$E$10),0)</f>
         <v>5219</v>
       </c>
       <c r="C11" s="5">
@@ -1049,7 +1052,7 @@
         <v>21.24388753056235</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" ref="E12:E40" si="14">+E11</f>
+        <f t="shared" ref="E12:E41" si="14">+E11</f>
         <v>0.33180277317219053</v>
       </c>
       <c r="H12" s="2">
@@ -1368,7 +1371,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <f t="shared" ref="A19:A40" si="16">+A18+1</f>
+        <f t="shared" ref="A19:A41" si="16">+A18+1</f>
         <v>43914</v>
       </c>
       <c r="B19" s="7">
@@ -1499,29 +1502,28 @@
         <f t="shared" si="0"/>
         <v>43916</v>
       </c>
-      <c r="I21" s="19">
-        <f t="shared" ref="I21:I29" si="17">I20*(1+AVERAGE(M18:M20))</f>
-        <v>86433.980629868354</v>
+      <c r="I21" s="18">
+        <v>85435</v>
       </c>
       <c r="J21" s="25">
         <f t="shared" si="2"/>
-        <v>-5179.0193701316457</v>
+        <v>-6178</v>
       </c>
       <c r="K21" s="26">
         <f t="shared" si="7"/>
-        <v>264.16253248737274</v>
+        <v>261.10941320293398</v>
       </c>
       <c r="L21" s="25">
         <f t="shared" si="11"/>
-        <v>18222.980629868354</v>
+        <v>17224</v>
       </c>
       <c r="M21" s="27">
         <f t="shared" si="12"/>
-        <v>0.26715603978637398</v>
+        <v>0.25251059213323362</v>
       </c>
       <c r="N21" s="27">
         <f t="shared" si="8"/>
-        <v>-6.4646733385816557E-2</v>
+        <v>-7.929218103895691E-2</v>
       </c>
       <c r="P21" s="22">
         <v>409</v>
@@ -1555,29 +1557,28 @@
         <f t="shared" si="0"/>
         <v>43917</v>
       </c>
-      <c r="I22" s="19">
-        <f t="shared" si="17"/>
-        <v>108472.3920777849</v>
+      <c r="I22" s="18">
+        <v>104126</v>
       </c>
       <c r="J22" s="25">
         <f t="shared" si="2"/>
-        <v>-13537.607922215102</v>
+        <v>-17884</v>
       </c>
       <c r="K22" s="26">
         <f t="shared" si="7"/>
-        <v>331.51709070227656</v>
+        <v>318.23349633251831</v>
       </c>
       <c r="L22" s="25">
         <f t="shared" si="11"/>
-        <v>22038.411447916544</v>
+        <v>18691</v>
       </c>
       <c r="M22" s="27">
         <f t="shared" si="12"/>
-        <v>0.25497392677412906</v>
+        <v>0.21877450693509687</v>
       </c>
       <c r="N22" s="27">
         <f t="shared" si="8"/>
-        <v>-7.6828846398061479E-2</v>
+        <v>-0.11302826623709367</v>
       </c>
       <c r="P22" s="23">
         <f>+P21*P20</f>
@@ -1613,28 +1614,28 @@
         <v>43918</v>
       </c>
       <c r="I23" s="19">
-        <f t="shared" si="17"/>
-        <v>136154.02440003102</v>
+        <f t="shared" ref="I22:I29" si="17">I22*(1+AVERAGE(M20:M22))</f>
+        <v>128933.69642802312</v>
       </c>
       <c r="J23" s="25">
         <f t="shared" si="2"/>
-        <v>-26338.975599968981</v>
+        <v>-33559.303571976881</v>
       </c>
       <c r="K23" s="26">
         <f t="shared" si="7"/>
-        <v>416.11865647931239</v>
+        <v>394.05163944994842</v>
       </c>
       <c r="L23" s="25">
         <f t="shared" si="11"/>
-        <v>27681.632322246121</v>
+        <v>24807.696428023119</v>
       </c>
       <c r="M23" s="27">
         <f t="shared" si="12"/>
-        <v>0.25519518646178457</v>
+        <v>0.23824689729772697</v>
       </c>
       <c r="N23" s="27">
         <f t="shared" si="8"/>
-        <v>-7.6607586710405962E-2</v>
+        <v>-9.3555875874463568E-2</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1664,27 +1665,27 @@
       </c>
       <c r="I24" s="19">
         <f t="shared" si="17"/>
-        <v>171432.67368381581</v>
+        <v>159427.89076983329</v>
       </c>
       <c r="J24" s="25">
         <f t="shared" si="2"/>
-        <v>-44976.32631618419</v>
+        <v>-56981.109230166709</v>
       </c>
       <c r="K24" s="26">
         <f t="shared" si="7"/>
-        <v>523.93848925371583</v>
+        <v>487.24905492002841</v>
       </c>
       <c r="L24" s="25">
         <f t="shared" si="11"/>
-        <v>35278.649283784791</v>
+        <v>30494.194341810173</v>
       </c>
       <c r="M24" s="27">
         <f t="shared" si="12"/>
-        <v>0.2591083843407625</v>
+        <v>0.23651066545535265</v>
       </c>
       <c r="N24" s="27">
         <f t="shared" si="8"/>
-        <v>-7.2694388831428036E-2</v>
+        <v>-9.5292107716837882E-2</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>16</v>
@@ -1724,27 +1725,27 @@
       </c>
       <c r="I25" s="19">
         <f t="shared" si="17"/>
-        <v>215392.43975527069</v>
+        <v>196284.00912037431</v>
       </c>
       <c r="J25" s="25">
         <f t="shared" si="2"/>
-        <v>-72821.560244729306</v>
+        <v>-91929.990879625693</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>658.28985255278326</v>
+        <v>599.8900034241268</v>
       </c>
       <c r="L25" s="25">
         <f t="shared" si="11"/>
-        <v>43959.766071454884</v>
+        <v>36856.118350541015</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="12"/>
-        <v>0.25642583252555856</v>
+        <v>0.23117735656272556</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>-7.5376940646631974E-2</v>
+        <v>-0.10062541660946497</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1774,27 +1775,27 @@
       </c>
       <c r="I26" s="19">
         <f t="shared" si="17"/>
-        <v>270728.86861325894</v>
+        <v>242471.92116749904</v>
       </c>
       <c r="J26" s="25">
         <f t="shared" si="2"/>
-        <v>-113115.13138674106</v>
+        <v>-141372.07883250096</v>
       </c>
       <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>827.41096764443444</v>
+        <v>741.05110381264979</v>
       </c>
       <c r="L26" s="25">
         <f t="shared" si="11"/>
-        <v>55336.428857988241</v>
+        <v>46187.91204712473</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="12"/>
-        <v>0.25690980110936856</v>
+        <v>0.23531163977193503</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>-7.4892972062821972E-2</v>
+        <v>-9.6491133400255502E-2</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1824,27 +1825,27 @@
       </c>
       <c r="I27" s="19">
         <f t="shared" si="17"/>
-        <v>340436.50029780506</v>
+        <v>299291.14735894121</v>
       </c>
       <c r="J27" s="25">
         <f t="shared" si="2"/>
-        <v>-170768.49970219494</v>
+        <v>-211913.85264105879</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>1040.4538517659078</v>
+        <v>914.70399559578607</v>
       </c>
       <c r="L27" s="25">
         <f t="shared" si="11"/>
-        <v>69707.631684546126</v>
+        <v>56819.226191442169</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="12"/>
-        <v>0.25748133932522999</v>
+        <v>0.234333220596671</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>-7.432143384696055E-2</v>
+        <v>-9.7469552575519536E-2</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1874,27 +1875,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="17"/>
-        <v>427907.91117937298</v>
+        <v>369207.77582561289</v>
       </c>
       <c r="J28" s="25">
         <f t="shared" si="2"/>
-        <v>-252916.08882062702</v>
+        <v>-311616.22417438711</v>
       </c>
       <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>1307.7870146068858</v>
+        <v>1128.3856229389146</v>
       </c>
       <c r="L28" s="25">
         <f t="shared" si="11"/>
-        <v>87471.410881567921</v>
+        <v>69916.628466671682</v>
       </c>
       <c r="M28" s="27">
         <f t="shared" si="12"/>
-        <v>0.25693899098671907</v>
+        <v>0.23360740564377722</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>-7.4863782185471461E-2</v>
+        <v>-9.8195367528413319E-2</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1924,27 +1925,27 @@
       </c>
       <c r="I29" s="19">
         <f t="shared" si="17"/>
-        <v>537927.33296810871</v>
+        <v>455756.51081853098</v>
       </c>
       <c r="J29" s="25">
         <f t="shared" si="2"/>
-        <v>-368795.66703189129</v>
+        <v>-450966.48918146902</v>
       </c>
       <c r="K29" s="26">
         <f t="shared" si="7"/>
-        <v>1644.0321912228262</v>
+        <v>1392.8988716947767</v>
       </c>
       <c r="L29" s="25">
         <f t="shared" si="11"/>
-        <v>110019.42178873572</v>
+        <v>86548.734992918093</v>
       </c>
       <c r="M29" s="27">
         <f t="shared" si="12"/>
-        <v>0.25711004380710578</v>
+        <v>0.23441742200412774</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="8"/>
-        <v>-7.4692729365084753E-2</v>
+        <v>-9.7385351168062795E-2</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1974,27 +1975,27 @@
       </c>
       <c r="I30" s="19">
         <f t="shared" ref="I30:I40" si="20">I29*(1+AVERAGE(M27:M29))</f>
-        <v>676269.75845269219</v>
+        <v>562457.92862295138</v>
       </c>
       <c r="J30" s="25">
         <f t="shared" ref="J30:J40" si="21">IF(I30&lt;=0,0, I30-B30)</f>
-        <v>-531306.24154730781</v>
+        <v>-645118.07137704862</v>
       </c>
       <c r="K30" s="26">
         <f t="shared" ref="K30:K40" si="22">IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
-        <v>2066.8391150754651</v>
+        <v>1719.0034493366484</v>
       </c>
       <c r="L30" s="25">
         <f t="shared" ref="L30:L40" si="23">IF(I30&lt;=0,0, I30-I29)</f>
-        <v>138342.42548458348</v>
+        <v>106701.4178044204</v>
       </c>
       <c r="M30" s="27">
         <f t="shared" ref="M30:M40" si="24">IF(I30&lt;=0,0, L30/I29)</f>
-        <v>0.25717679137301835</v>
+        <v>0.23411934941485851</v>
       </c>
       <c r="N30" s="27">
         <f t="shared" ref="N30:N40" si="25">IF(I30&lt;=0,0,M30-E30)</f>
-        <v>-7.4625981799172181E-2</v>
+        <v>-9.7683423757332022E-2</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -2024,27 +2025,27 @@
       </c>
       <c r="I31" s="19">
         <f t="shared" si="20"/>
-        <v>850121.99284413527</v>
+        <v>694100.11509808095</v>
       </c>
       <c r="J31" s="25">
         <f t="shared" si="21"/>
-        <v>-758131.00715586473</v>
+        <v>-914152.88490191905</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="22"/>
-        <v>2598.1723497681396</v>
+        <v>2121.3328701041592</v>
       </c>
       <c r="L31" s="25">
         <f t="shared" si="23"/>
-        <v>173852.23439144308</v>
+        <v>131642.18647512957</v>
       </c>
       <c r="M31" s="27">
         <f t="shared" si="24"/>
-        <v>0.25707527538894787</v>
+        <v>0.23404805902092113</v>
       </c>
       <c r="N31" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4727497783242669E-2</v>
+        <v>-9.7754714151269406E-2</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -2074,30 +2075,30 @@
       </c>
       <c r="I32" s="19">
         <f t="shared" si="20"/>
-        <v>1068705.9577246145</v>
+        <v>856654.85232291603</v>
       </c>
       <c r="J32" s="25">
         <f t="shared" si="21"/>
-        <v>-1073170.0422753855</v>
+        <v>-1285221.147677084</v>
       </c>
       <c r="K32" s="26">
         <f t="shared" si="22"/>
-        <v>3266.2162522145923</v>
+        <v>2618.1383017204034</v>
       </c>
       <c r="L32" s="25">
         <f t="shared" si="23"/>
-        <v>218583.96488047927</v>
+        <v>162554.73722483509</v>
       </c>
       <c r="M32" s="27">
         <f t="shared" si="24"/>
-        <v>0.25712070352302402</v>
+        <v>0.23419494347996905</v>
       </c>
       <c r="N32" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4682069649166516E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7607829692221482E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <f t="shared" si="16"/>
         <v>43928</v>
@@ -2124,30 +2125,30 @@
       </c>
       <c r="I33" s="19">
         <f t="shared" si="20"/>
-        <v>1343496.1828013177</v>
+        <v>1057215.5579421031</v>
       </c>
       <c r="J33" s="25">
         <f t="shared" si="21"/>
-        <v>-1509059.8171986823</v>
+        <v>-1795340.4420578969</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="22"/>
-        <v>4106.0396784881341</v>
+        <v>3231.0988934660854</v>
       </c>
       <c r="L33" s="25">
         <f t="shared" si="23"/>
-        <v>274790.22507670312</v>
+        <v>200560.70561918709</v>
       </c>
       <c r="M33" s="27">
         <f t="shared" si="24"/>
-        <v>0.25712425676166334</v>
+        <v>0.23412078397191607</v>
       </c>
       <c r="N33" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4678516410527196E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7681989200274461E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <f t="shared" si="16"/>
         <v>43929</v>
@@ -2174,30 +2175,30 @@
       </c>
       <c r="I34" s="19">
         <f t="shared" si="20"/>
-        <v>1688918.1135829648</v>
+        <v>1304732.1987401617</v>
       </c>
       <c r="J34" s="25">
         <f t="shared" si="21"/>
-        <v>-2110123.886417035</v>
+        <v>-2494309.801259838</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="22"/>
-        <v>5161.7301759870561</v>
+        <v>3987.5678445603967</v>
       </c>
       <c r="L34" s="25">
         <f t="shared" si="23"/>
-        <v>345421.9307816471</v>
+        <v>247516.64079805859</v>
       </c>
       <c r="M34" s="27">
         <f t="shared" si="24"/>
-        <v>0.25710674522454496</v>
+        <v>0.23412126215760201</v>
       </c>
       <c r="N34" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4696027947645571E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7681511014588523E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <f t="shared" si="16"/>
         <v>43930</v>
@@ -2224,30 +2225,30 @@
       </c>
       <c r="I35" s="19">
         <f t="shared" si="20"/>
-        <v>2123168.0693755164</v>
+        <v>1610229.5847166972</v>
       </c>
       <c r="J35" s="25">
         <f t="shared" si="21"/>
-        <v>-2936406.9306244836</v>
+        <v>-3449345.4152833028</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="22"/>
-        <v>6488.8999675290843</v>
+        <v>4921.2395620925954</v>
       </c>
       <c r="L35" s="25">
         <f t="shared" si="23"/>
-        <v>434249.95579255163</v>
+        <v>305497.3859765355</v>
       </c>
       <c r="M35" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711723516974405</v>
+        <v>0.23414566320316244</v>
       </c>
       <c r="N35" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4685538002446483E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.76571099690281E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <f t="shared" si="16"/>
         <v>43931</v>
@@ -2274,30 +2275,30 @@
       </c>
       <c r="I36" s="19">
         <f t="shared" si="20"/>
-        <v>2669068.7185417204</v>
+        <v>1987231.4078863221</v>
       </c>
       <c r="J36" s="25">
         <f t="shared" si="21"/>
-        <v>-4069287.2814582796</v>
+        <v>-4751124.5921136774</v>
       </c>
       <c r="K36" s="26">
         <f t="shared" si="22"/>
-        <v>8157.3004845407104</v>
+        <v>6073.4456231244567</v>
       </c>
       <c r="L36" s="25">
         <f t="shared" si="23"/>
-        <v>545900.64916620404</v>
+        <v>377001.8231696249</v>
       </c>
       <c r="M36" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711607905198425</v>
+        <v>0.2341292364442269</v>
       </c>
       <c r="N36" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4686694120206287E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7673536727963639E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <f t="shared" si="16"/>
         <v>43932</v>
@@ -2324,30 +2325,30 @@
       </c>
       <c r="I37" s="19">
         <f t="shared" si="20"/>
-        <v>3355321.92655044</v>
+        <v>2452505.9790588827</v>
       </c>
       <c r="J37" s="25">
         <f t="shared" si="21"/>
-        <v>-5618839.0734495595</v>
+        <v>-6521655.0209411178</v>
       </c>
       <c r="K37" s="26">
         <f t="shared" si="22"/>
-        <v>10254.651364762958</v>
+        <v>7495.4339213291032</v>
       </c>
       <c r="L37" s="25">
         <f t="shared" si="23"/>
-        <v>686253.20800871961</v>
+        <v>465274.57117256057</v>
       </c>
       <c r="M37" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711335314875772</v>
+        <v>0.23413205393499709</v>
       </c>
       <c r="N37" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4689420023432818E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7670719237193449E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <f t="shared" si="16"/>
         <v>43933</v>
@@ -2374,30 +2375,33 @@
       </c>
       <c r="I38" s="19">
         <f t="shared" si="20"/>
-        <v>4218027.3885503737</v>
+        <v>3026725.0635233289</v>
       </c>
       <c r="J38" s="25">
         <f t="shared" si="21"/>
-        <v>-7733785.6114496263</v>
+        <v>-8925087.9364766702</v>
       </c>
       <c r="K38" s="26">
         <f t="shared" si="22"/>
-        <v>12891.281749848331</v>
+        <v>9250.3822234820564</v>
       </c>
       <c r="L38" s="25">
         <f t="shared" si="23"/>
-        <v>862705.4619999337</v>
+        <v>574219.08446444618</v>
       </c>
       <c r="M38" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711555579016204</v>
+        <v>0.23413565119412891</v>
       </c>
       <c r="N38" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4687217382028492E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7667121978061627E-2</v>
+      </c>
+      <c r="P38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <f t="shared" si="16"/>
         <v>43934</v>
@@ -2424,30 +2428,30 @@
       </c>
       <c r="I39" s="19">
         <f t="shared" si="20"/>
-        <v>5302545.4836726049</v>
+        <v>3735379.2060573949</v>
       </c>
       <c r="J39" s="25">
         <f t="shared" si="21"/>
-        <v>-10614912.516327396</v>
+        <v>-12182078.793942604</v>
       </c>
       <c r="K39" s="26">
         <f t="shared" si="22"/>
-        <v>16205.823605356371</v>
+        <v>11416.195617534826</v>
       </c>
       <c r="L39" s="25">
         <f t="shared" si="23"/>
-        <v>1084518.0951222312</v>
+        <v>708654.14253406599</v>
       </c>
       <c r="M39" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711499599696813</v>
+        <v>0.23413231385778424</v>
       </c>
       <c r="N39" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4687777175222403E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+        <v>-9.7670459314406294E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <f t="shared" si="16"/>
         <v>43935</v>
@@ -2474,27 +2478,77 @@
       </c>
       <c r="I40" s="19">
         <f t="shared" si="20"/>
-        <v>6665907.5301646665</v>
+        <v>4609956.0144767361</v>
       </c>
       <c r="J40" s="25">
         <f t="shared" si="21"/>
-        <v>-14533007.469835334</v>
+        <v>-16588958.985523265</v>
       </c>
       <c r="K40" s="26">
         <f t="shared" si="22"/>
-        <v>20372.57802617563</v>
+        <v>14089.107623706406</v>
       </c>
       <c r="L40" s="25">
         <f t="shared" si="23"/>
-        <v>1363362.0464920616</v>
+        <v>874576.80841934122</v>
       </c>
       <c r="M40" s="27">
         <f t="shared" si="24"/>
-        <v>0.25711463497862935</v>
+        <v>0.2341333396623034</v>
       </c>
       <c r="N40" s="27">
         <f t="shared" si="25"/>
-        <v>-7.4688138193561182E-2</v>
+        <v>-9.7669433509887132E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <f t="shared" si="16"/>
+        <v>43936</v>
+      </c>
+      <c r="B41" s="7">
+        <f t="shared" si="10"/>
+        <v>28232774</v>
+      </c>
+      <c r="C41" s="8">
+        <f t="shared" ref="C41" si="26">+B41/$P$15*1000000</f>
+        <v>86285.984107579454</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="11">
+        <f t="shared" si="14"/>
+        <v>0.33180277317219053</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H41" s="24">
+        <f t="shared" ref="H41" si="27">A41</f>
+        <v>43936</v>
+      </c>
+      <c r="I41" s="19">
+        <f t="shared" ref="I41" si="28">I40*(1+AVERAGE(M38:M40))</f>
+        <v>5689302.3875579396</v>
+      </c>
+      <c r="J41" s="25">
+        <f t="shared" ref="J41" si="29">IF(I41&lt;=0,0, I41-B41)</f>
+        <v>-22543471.612442061</v>
+      </c>
+      <c r="K41" s="26">
+        <f t="shared" ref="K41" si="30">IF(I41&lt;=0,0, I41/$P$15*1000000)</f>
+        <v>17387.84348275654</v>
+      </c>
+      <c r="L41" s="25">
+        <f t="shared" ref="L41" si="31">IF(I41&lt;=0,0, I41-I40)</f>
+        <v>1079346.3730812036</v>
+      </c>
+      <c r="M41" s="27">
+        <f t="shared" ref="M41" si="32">IF(I41&lt;=0,0, L41/I40)</f>
+        <v>0.23413376823807228</v>
+      </c>
+      <c r="N41" s="27">
+        <f t="shared" ref="N41" si="33">IF(I41&lt;=0,0,M41-E41)</f>
+        <v>-9.7669004934118259E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stats for Mar 28
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2FE235-085F-A341-8FD8-F8468C2CC1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16A3026-78C0-084C-976C-7BD720BAF40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
+    <workbookView xWindow="28720" yWindow="1860" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <t>ACTUAL STATS - UPDATED DAILY</t>
   </si>
   <si>
-    <t>EASTER SUNDAY - THE DAY TRUMP WANTS CORONAVIRUS TO BE DONE</t>
+    <t>EASTER SUNDAY - THE DAY TRUMP WANTS CORONAVIRUS TO GO AWAY</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:W41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -1613,29 +1613,28 @@
         <f t="shared" si="0"/>
         <v>43918</v>
       </c>
-      <c r="I23" s="19">
-        <f t="shared" ref="I22:I29" si="17">I22*(1+AVERAGE(M20:M22))</f>
-        <v>128933.69642802312</v>
+      <c r="I23" s="18">
+        <v>123578</v>
       </c>
       <c r="J23" s="25">
         <f t="shared" si="2"/>
-        <v>-33559.303571976881</v>
+        <v>-38915</v>
       </c>
       <c r="K23" s="26">
         <f t="shared" si="7"/>
-        <v>394.05163944994842</v>
+        <v>377.68337408312959</v>
       </c>
       <c r="L23" s="25">
         <f t="shared" si="11"/>
-        <v>24807.696428023119</v>
+        <v>19452</v>
       </c>
       <c r="M23" s="27">
         <f t="shared" si="12"/>
-        <v>0.23824689729772697</v>
+        <v>0.18681213145612047</v>
       </c>
       <c r="N23" s="27">
         <f t="shared" si="8"/>
-        <v>-9.3555875874463568E-2</v>
+        <v>-0.14499064171607007</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
@@ -1664,28 +1663,28 @@
         <v>43919</v>
       </c>
       <c r="I24" s="19">
-        <f t="shared" si="17"/>
-        <v>159427.89076983329</v>
+        <f>I23*(1+AVERAGE(M22:M23))</f>
+        <v>148638.79279955491</v>
       </c>
       <c r="J24" s="25">
         <f t="shared" si="2"/>
-        <v>-56981.109230166709</v>
+        <v>-67770.207200445089</v>
       </c>
       <c r="K24" s="26">
         <f t="shared" si="7"/>
-        <v>487.24905492002841</v>
+        <v>454.27503911844411</v>
       </c>
       <c r="L24" s="25">
         <f t="shared" si="11"/>
-        <v>30494.194341810173</v>
+        <v>25060.792799554911</v>
       </c>
       <c r="M24" s="27">
         <f t="shared" si="12"/>
-        <v>0.23651066545535265</v>
+        <v>0.20279331919560853</v>
       </c>
       <c r="N24" s="27">
         <f t="shared" si="8"/>
-        <v>-9.5292107716837882E-2</v>
+        <v>-0.12900945397658201</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>16</v>
@@ -1724,28 +1723,28 @@
         <v>43920</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" si="17"/>
-        <v>196284.00912037431</v>
+        <f t="shared" ref="I23:I29" si="17">I24*(1+AVERAGE(M22:M24))</f>
+        <v>178781.74695260497</v>
       </c>
       <c r="J25" s="25">
         <f t="shared" si="2"/>
-        <v>-91929.990879625693</v>
+        <v>-109432.25304739503</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>599.8900034241268</v>
+        <v>546.39898212898834</v>
       </c>
       <c r="L25" s="25">
         <f t="shared" si="11"/>
-        <v>36856.118350541015</v>
+        <v>30142.954153050057</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="12"/>
-        <v>0.23117735656272556</v>
+        <v>0.20279331919560853</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>-0.10062541660946497</v>
+        <v>-0.12900945397658201</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1775,27 +1774,27 @@
       </c>
       <c r="I26" s="19">
         <f t="shared" si="17"/>
-        <v>242471.92116749904</v>
+        <v>214085.10927456536</v>
       </c>
       <c r="J26" s="25">
         <f t="shared" si="2"/>
-        <v>-141372.07883250096</v>
+        <v>-169758.89072543464</v>
       </c>
       <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>741.05110381264979</v>
+        <v>654.29434374867162</v>
       </c>
       <c r="L26" s="25">
         <f t="shared" si="11"/>
-        <v>46187.91204712473</v>
+        <v>35303.362321960391</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="12"/>
-        <v>0.23531163977193503</v>
+        <v>0.19746625661577918</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>-9.6491133400255502E-2</v>
+        <v>-0.13433651655641135</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1825,27 +1824,27 @@
       </c>
       <c r="I27" s="19">
         <f t="shared" si="17"/>
-        <v>299291.14735894121</v>
+        <v>257119.99091653727</v>
       </c>
       <c r="J27" s="25">
         <f t="shared" si="2"/>
-        <v>-211913.85264105879</v>
+        <v>-254085.00908346273</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>914.70399559578607</v>
+        <v>785.81904314345127</v>
       </c>
       <c r="L27" s="25">
         <f t="shared" si="11"/>
-        <v>56819.226191442169</v>
+        <v>43034.881641971908</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="12"/>
-        <v>0.234333220596671</v>
+        <v>0.20101763166899866</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>-9.7469552575519536E-2</v>
+        <v>-0.13078514150319187</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1875,27 +1874,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="17"/>
-        <v>369207.77582561289</v>
+        <v>308653.45429176325</v>
       </c>
       <c r="J28" s="25">
         <f t="shared" si="2"/>
-        <v>-311616.22417438711</v>
+        <v>-372170.54570823675</v>
       </c>
       <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>1128.3856229389146</v>
+        <v>943.31740309218594</v>
       </c>
       <c r="L28" s="25">
         <f t="shared" si="11"/>
-        <v>69916.628466671682</v>
+        <v>51533.463375225983</v>
       </c>
       <c r="M28" s="27">
         <f t="shared" si="12"/>
-        <v>0.23360740564377722</v>
+        <v>0.2004257358267956</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>-9.8195367528413319E-2</v>
+        <v>-0.13137703734539494</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1925,27 +1924,27 @@
       </c>
       <c r="I29" s="19">
         <f t="shared" si="17"/>
-        <v>455756.51081853098</v>
+        <v>370271.96238863614</v>
       </c>
       <c r="J29" s="25">
         <f t="shared" si="2"/>
-        <v>-450966.48918146902</v>
+        <v>-536451.03761136392</v>
       </c>
       <c r="K29" s="26">
         <f t="shared" si="7"/>
-        <v>1392.8988716947767</v>
+        <v>1131.6380268601349</v>
       </c>
       <c r="L29" s="25">
         <f t="shared" si="11"/>
-        <v>86548.734992918093</v>
+        <v>61618.508096872887</v>
       </c>
       <c r="M29" s="27">
         <f t="shared" si="12"/>
-        <v>0.23441742200412774</v>
+        <v>0.1996365413705245</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="8"/>
-        <v>-9.7385351168062795E-2</v>
+        <v>-0.13216623180166603</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1975,27 +1974,27 @@
       </c>
       <c r="I30" s="19">
         <f t="shared" ref="I30:I40" si="20">I29*(1+AVERAGE(M27:M29))</f>
-        <v>562457.92862295138</v>
+        <v>444459.64152474096</v>
       </c>
       <c r="J30" s="25">
         <f t="shared" ref="J30:J40" si="21">IF(I30&lt;=0,0, I30-B30)</f>
-        <v>-645118.07137704862</v>
+        <v>-763116.35847525904</v>
       </c>
       <c r="K30" s="26">
         <f t="shared" ref="K30:K40" si="22">IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
-        <v>1719.0034493366484</v>
+        <v>1358.372987545052</v>
       </c>
       <c r="L30" s="25">
         <f t="shared" ref="L30:L40" si="23">IF(I30&lt;=0,0, I30-I29)</f>
-        <v>106701.4178044204</v>
+        <v>74187.679136104824</v>
       </c>
       <c r="M30" s="27">
         <f t="shared" ref="M30:M40" si="24">IF(I30&lt;=0,0, L30/I29)</f>
-        <v>0.23411934941485851</v>
+        <v>0.20035996962210631</v>
       </c>
       <c r="N30" s="27">
         <f t="shared" ref="N30:N40" si="25">IF(I30&lt;=0,0,M30-E30)</f>
-        <v>-9.7683423757332022E-2</v>
+        <v>-0.13144280355008423</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -2025,27 +2024,27 @@
       </c>
       <c r="I31" s="19">
         <f t="shared" si="20"/>
-        <v>694100.11509808095</v>
+        <v>533414.12705302157</v>
       </c>
       <c r="J31" s="25">
         <f t="shared" si="21"/>
-        <v>-914152.88490191905</v>
+        <v>-1074838.8729469785</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="22"/>
-        <v>2121.3328701041592</v>
+        <v>1630.2387746119241</v>
       </c>
       <c r="L31" s="25">
         <f t="shared" si="23"/>
-        <v>131642.18647512957</v>
+        <v>88954.485528280609</v>
       </c>
       <c r="M31" s="27">
         <f t="shared" si="24"/>
-        <v>0.23404805902092113</v>
+        <v>0.20014074893980882</v>
       </c>
       <c r="N31" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7754714151269406E-2</v>
+        <v>-0.13166202423238171</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -2075,27 +2074,27 @@
       </c>
       <c r="I32" s="19">
         <f t="shared" si="20"/>
-        <v>856654.85232291603</v>
+        <v>640121.35792597302</v>
       </c>
       <c r="J32" s="25">
         <f t="shared" si="21"/>
-        <v>-1285221.147677084</v>
+        <v>-1501754.6420740271</v>
       </c>
       <c r="K32" s="26">
         <f t="shared" si="22"/>
-        <v>2618.1383017204034</v>
+        <v>1956.3611183556632</v>
       </c>
       <c r="L32" s="25">
         <f t="shared" si="23"/>
-        <v>162554.73722483509</v>
+        <v>106707.23087295145</v>
       </c>
       <c r="M32" s="27">
         <f t="shared" si="24"/>
-        <v>0.23419494347996905</v>
+        <v>0.20004575331081306</v>
       </c>
       <c r="N32" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7607829692221482E-2</v>
+        <v>-0.13175701986137747</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -2125,27 +2124,27 @@
       </c>
       <c r="I33" s="19">
         <f t="shared" si="20"/>
-        <v>1057215.5579421031</v>
+        <v>768262.2322835807</v>
       </c>
       <c r="J33" s="25">
         <f t="shared" si="21"/>
-        <v>-1795340.4420578969</v>
+        <v>-2084293.7677164194</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="22"/>
-        <v>3231.0988934660854</v>
+        <v>2347.9897074681562</v>
       </c>
       <c r="L33" s="25">
         <f t="shared" si="23"/>
-        <v>200560.70561918709</v>
+        <v>128140.87435760768</v>
       </c>
       <c r="M33" s="27">
         <f t="shared" si="24"/>
-        <v>0.23412078397191607</v>
+        <v>0.20018215729090946</v>
       </c>
       <c r="N33" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7681989200274461E-2</v>
+        <v>-0.13162061588128107</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
@@ -2175,27 +2174,27 @@
       </c>
       <c r="I34" s="19">
         <f t="shared" si="20"/>
-        <v>1304732.1987401617</v>
+        <v>922009.08780773997</v>
       </c>
       <c r="J34" s="25">
         <f t="shared" si="21"/>
-        <v>-2494309.801259838</v>
+        <v>-2877032.9121922599</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="22"/>
-        <v>3987.5678445603967</v>
+        <v>2817.8761852314792</v>
       </c>
       <c r="L34" s="25">
         <f t="shared" si="23"/>
-        <v>247516.64079805859</v>
+        <v>153746.85552415927</v>
       </c>
       <c r="M34" s="27">
         <f t="shared" si="24"/>
-        <v>0.23412126215760201</v>
+        <v>0.20012288651384372</v>
       </c>
       <c r="N34" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7681511014588523E-2</v>
+        <v>-0.13167988665834682</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
@@ -2225,27 +2224,27 @@
       </c>
       <c r="I35" s="19">
         <f t="shared" si="20"/>
-        <v>1610229.5847166972</v>
+        <v>1106518.7180787977</v>
       </c>
       <c r="J35" s="25">
         <f t="shared" si="21"/>
-        <v>-3449345.4152833028</v>
+        <v>-3953056.2819212023</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="22"/>
-        <v>4921.2395620925954</v>
+        <v>3381.7809232237091</v>
       </c>
       <c r="L35" s="25">
         <f t="shared" si="23"/>
-        <v>305497.3859765355</v>
+        <v>184509.63027105771</v>
       </c>
       <c r="M35" s="27">
         <f t="shared" si="24"/>
-        <v>0.23414566320316244</v>
+        <v>0.20011693237185554</v>
       </c>
       <c r="N35" s="27">
         <f t="shared" si="25"/>
-        <v>-9.76571099690281E-2</v>
+        <v>-0.13168584080033499</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -2275,27 +2274,27 @@
       </c>
       <c r="I36" s="19">
         <f t="shared" si="20"/>
-        <v>1987231.4078863221</v>
+        <v>1327978.1032072243</v>
       </c>
       <c r="J36" s="25">
         <f t="shared" si="21"/>
-        <v>-4751124.5921136774</v>
+        <v>-5410377.896792776</v>
       </c>
       <c r="K36" s="26">
         <f t="shared" si="22"/>
-        <v>6073.4456231244567</v>
+        <v>4058.612784863155</v>
       </c>
       <c r="L36" s="25">
         <f t="shared" si="23"/>
-        <v>377001.8231696249</v>
+        <v>221459.3851284266</v>
       </c>
       <c r="M36" s="27">
         <f t="shared" si="24"/>
-        <v>0.2341292364442269</v>
+        <v>0.20014065872553632</v>
       </c>
       <c r="N36" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7673536727963639E-2</v>
+        <v>-0.13166211444665421</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -2325,27 +2324,27 @@
       </c>
       <c r="I37" s="19">
         <f t="shared" si="20"/>
-        <v>2452505.9790588827</v>
+        <v>1593742.1458274962</v>
       </c>
       <c r="J37" s="25">
         <f t="shared" si="21"/>
-        <v>-6521655.0209411178</v>
+        <v>-7380418.8541725036</v>
       </c>
       <c r="K37" s="26">
         <f t="shared" si="22"/>
-        <v>7495.4339213291032</v>
+        <v>4870.85007893489</v>
       </c>
       <c r="L37" s="25">
         <f t="shared" si="23"/>
-        <v>465274.57117256057</v>
+        <v>265764.04262027191</v>
       </c>
       <c r="M37" s="27">
         <f t="shared" si="24"/>
-        <v>0.23413205393499709</v>
+        <v>0.20012682587041178</v>
       </c>
       <c r="N37" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7670719237193449E-2</v>
+        <v>-0.13167594730177876</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
@@ -2375,27 +2374,27 @@
       </c>
       <c r="I38" s="19">
         <f t="shared" si="20"/>
-        <v>3026725.0635233289</v>
+        <v>1912694.7955007155</v>
       </c>
       <c r="J38" s="25">
         <f t="shared" si="21"/>
-        <v>-8925087.9364766702</v>
+        <v>-10039118.204499284</v>
       </c>
       <c r="K38" s="26">
         <f t="shared" si="22"/>
-        <v>9250.3822234820564</v>
+        <v>5845.6442405278594</v>
       </c>
       <c r="L38" s="25">
         <f t="shared" si="23"/>
-        <v>574219.08446444618</v>
+        <v>318952.6496732193</v>
       </c>
       <c r="M38" s="27">
         <f t="shared" si="24"/>
-        <v>0.23413565119412891</v>
+        <v>0.20012813898926796</v>
       </c>
       <c r="N38" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7667121978061627E-2</v>
+        <v>-0.13167463418292258</v>
       </c>
       <c r="P38" t="s">
         <v>20</v>
@@ -2428,27 +2427,27 @@
       </c>
       <c r="I39" s="19">
         <f t="shared" si="20"/>
-        <v>3735379.2060573949</v>
+        <v>2295485.9903249987</v>
       </c>
       <c r="J39" s="25">
         <f t="shared" si="21"/>
-        <v>-12182078.793942604</v>
+        <v>-13621972.009675002</v>
       </c>
       <c r="K39" s="26">
         <f t="shared" si="22"/>
-        <v>11416.195617534826</v>
+        <v>7015.5439802108758</v>
       </c>
       <c r="L39" s="25">
         <f t="shared" si="23"/>
-        <v>708654.14253406599</v>
+        <v>382791.19482428324</v>
       </c>
       <c r="M39" s="27">
         <f t="shared" si="24"/>
-        <v>0.23413231385778424</v>
+        <v>0.20013187452840542</v>
       </c>
       <c r="N39" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7670459314406294E-2</v>
+        <v>-0.13167089864378512</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -2478,27 +2477,27 @@
       </c>
       <c r="I40" s="19">
         <f t="shared" si="20"/>
-        <v>4609956.0144767361</v>
+        <v>2754879.1831886168</v>
       </c>
       <c r="J40" s="25">
         <f t="shared" si="21"/>
-        <v>-16588958.985523265</v>
+        <v>-18444035.816811383</v>
       </c>
       <c r="K40" s="26">
         <f t="shared" si="22"/>
-        <v>14089.107623706406</v>
+        <v>8419.5574058331804</v>
       </c>
       <c r="L40" s="25">
         <f t="shared" si="23"/>
-        <v>874576.80841934122</v>
+        <v>459393.19286361802</v>
       </c>
       <c r="M40" s="27">
         <f t="shared" si="24"/>
-        <v>0.2341333396623034</v>
+        <v>0.20012894646269497</v>
       </c>
       <c r="N40" s="27">
         <f t="shared" si="25"/>
-        <v>-9.7669433509887132E-2</v>
+        <v>-0.13167382670949557</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
@@ -2528,27 +2527,27 @@
       </c>
       <c r="I41" s="19">
         <f t="shared" ref="I41" si="28">I40*(1+AVERAGE(M38:M40))</f>
-        <v>5689302.3875579396</v>
+        <v>3306212.199077344</v>
       </c>
       <c r="J41" s="25">
         <f t="shared" ref="J41" si="29">IF(I41&lt;=0,0, I41-B41)</f>
-        <v>-22543471.612442061</v>
+        <v>-24926561.800922655</v>
       </c>
       <c r="K41" s="26">
         <f t="shared" ref="K41" si="30">IF(I41&lt;=0,0, I41/$P$15*1000000)</f>
-        <v>17387.84348275654</v>
+        <v>10104.56051062758</v>
       </c>
       <c r="L41" s="25">
         <f t="shared" ref="L41" si="31">IF(I41&lt;=0,0, I41-I40)</f>
-        <v>1079346.3730812036</v>
+        <v>551333.01588872727</v>
       </c>
       <c r="M41" s="27">
         <f t="shared" ref="M41" si="32">IF(I41&lt;=0,0, L41/I40)</f>
-        <v>0.23413376823807228</v>
+        <v>0.20012965332678964</v>
       </c>
       <c r="N41" s="27">
         <f t="shared" ref="N41" si="33">IF(I41&lt;=0,0,M41-E41)</f>
-        <v>-9.7669004934118259E-2</v>
+        <v>-0.13167311984540089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stats for Mar 29
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16A3026-78C0-084C-976C-7BD720BAF40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208A9C51-EC4D-844D-A1E3-831C91E6EDC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28720" yWindow="1860" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1662,29 +1662,28 @@
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
-      <c r="I24" s="19">
-        <f>I23*(1+AVERAGE(M22:M23))</f>
-        <v>148638.79279955491</v>
+      <c r="I24" s="18">
+        <v>142460</v>
       </c>
       <c r="J24" s="25">
         <f t="shared" si="2"/>
-        <v>-67770.207200445089</v>
+        <v>-73949</v>
       </c>
       <c r="K24" s="26">
         <f t="shared" si="7"/>
-        <v>454.27503911844411</v>
+        <v>435.3911980440098</v>
       </c>
       <c r="L24" s="25">
         <f t="shared" si="11"/>
-        <v>25060.792799554911</v>
+        <v>18882</v>
       </c>
       <c r="M24" s="27">
         <f t="shared" si="12"/>
-        <v>0.20279331919560853</v>
+        <v>0.15279418666752981</v>
       </c>
       <c r="N24" s="27">
         <f t="shared" si="8"/>
-        <v>-0.12900945397658201</v>
+        <v>-0.17900858650466073</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>16</v>
@@ -1723,28 +1722,28 @@
         <v>43920</v>
       </c>
       <c r="I25" s="19">
-        <f t="shared" ref="I23:I29" si="17">I24*(1+AVERAGE(M22:M24))</f>
-        <v>178781.74695260497</v>
+        <f t="shared" ref="I25:I29" si="17">I24*(1+AVERAGE(M22:M24))</f>
+        <v>168975.64411262303</v>
       </c>
       <c r="J25" s="25">
         <f t="shared" si="2"/>
-        <v>-109432.25304739503</v>
+        <v>-119238.35588737697</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>546.39898212898834</v>
+        <v>516.42923017305327</v>
       </c>
       <c r="L25" s="25">
         <f t="shared" si="11"/>
-        <v>30142.954153050057</v>
+        <v>26515.644112623035</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="12"/>
-        <v>0.20279331919560853</v>
+        <v>0.18612694168624902</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>-0.12900945397658201</v>
+        <v>-0.14567583148594151</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1774,27 +1773,27 @@
       </c>
       <c r="I26" s="19">
         <f t="shared" si="17"/>
-        <v>214085.10927456536</v>
+        <v>198587.68284855862</v>
       </c>
       <c r="J26" s="25">
         <f t="shared" si="2"/>
-        <v>-169758.89072543464</v>
+        <v>-185256.31715144138</v>
       </c>
       <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>654.29434374867162</v>
+        <v>606.93057105305195</v>
       </c>
       <c r="L26" s="25">
         <f t="shared" si="11"/>
-        <v>35303.362321960391</v>
+        <v>29612.038735935581</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="12"/>
-        <v>0.19746625661577918</v>
+        <v>0.17524441993663314</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>-0.13433651655641135</v>
+        <v>-0.15655835323555739</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1824,27 +1823,27 @@
       </c>
       <c r="I27" s="19">
         <f t="shared" si="17"/>
-        <v>257119.99091653727</v>
+        <v>232623.33112707583</v>
       </c>
       <c r="J27" s="25">
         <f t="shared" si="2"/>
-        <v>-254085.00908346273</v>
+        <v>-278581.66887292417</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>785.81904314345127</v>
+        <v>710.95150099962052</v>
       </c>
       <c r="L27" s="25">
         <f t="shared" si="11"/>
-        <v>43034.881641971908</v>
+        <v>34035.648278517212</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="12"/>
-        <v>0.20101763166899866</v>
+        <v>0.17138851609680408</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>-0.13078514150319187</v>
+        <v>-0.16041425707538645</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1874,27 +1873,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="17"/>
-        <v>308653.45429176325</v>
+        <v>273934.12360907817</v>
       </c>
       <c r="J28" s="25">
         <f t="shared" si="2"/>
-        <v>-372170.54570823675</v>
+        <v>-406889.87639092183</v>
       </c>
       <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>943.31740309218594</v>
+        <v>837.20697924534898</v>
       </c>
       <c r="L28" s="25">
         <f t="shared" si="11"/>
-        <v>51533.463375225983</v>
+        <v>41310.792482002347</v>
       </c>
       <c r="M28" s="27">
         <f t="shared" si="12"/>
-        <v>0.2004257358267956</v>
+        <v>0.17758662590656213</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>-0.13137703734539494</v>
+        <v>-0.15421614726562841</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1924,27 +1923,27 @@
       </c>
       <c r="I29" s="19">
         <f t="shared" si="17"/>
-        <v>370271.96238863614</v>
+        <v>321801.3323686677</v>
       </c>
       <c r="J29" s="25">
         <f t="shared" si="2"/>
-        <v>-536451.03761136392</v>
+        <v>-584921.6676313323</v>
       </c>
       <c r="K29" s="26">
         <f t="shared" si="7"/>
-        <v>1131.6380268601349</v>
+        <v>983.50040454971793</v>
       </c>
       <c r="L29" s="25">
         <f t="shared" si="11"/>
-        <v>61618.508096872887</v>
+        <v>47867.208759589528</v>
       </c>
       <c r="M29" s="27">
         <f t="shared" si="12"/>
-        <v>0.1996365413705245</v>
+        <v>0.17473985397999978</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="8"/>
-        <v>-0.13216623180166603</v>
+        <v>-0.15706291919219076</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1974,27 +1973,27 @@
       </c>
       <c r="I30" s="19">
         <f t="shared" ref="I30:I40" si="20">I29*(1+AVERAGE(M27:M29))</f>
-        <v>444459.64152474096</v>
+        <v>377978.72686496726</v>
       </c>
       <c r="J30" s="25">
         <f t="shared" ref="J30:J40" si="21">IF(I30&lt;=0,0, I30-B30)</f>
-        <v>-763116.35847525904</v>
+        <v>-829597.27313503274</v>
       </c>
       <c r="K30" s="26">
         <f t="shared" ref="K30:K40" si="22">IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
-        <v>1358.372987545052</v>
+        <v>1155.1917080225162</v>
       </c>
       <c r="L30" s="25">
         <f t="shared" ref="L30:L40" si="23">IF(I30&lt;=0,0, I30-I29)</f>
-        <v>74187.679136104824</v>
+        <v>56177.394496299559</v>
       </c>
       <c r="M30" s="27">
         <f t="shared" ref="M30:M40" si="24">IF(I30&lt;=0,0, L30/I29)</f>
-        <v>0.20035996962210631</v>
+        <v>0.1745716653277887</v>
       </c>
       <c r="N30" s="27">
         <f t="shared" ref="N30:N40" si="25">IF(I30&lt;=0,0,M30-E30)</f>
-        <v>-0.13144280355008423</v>
+        <v>-0.15723110784440184</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -2024,27 +2023,27 @@
       </c>
       <c r="I31" s="19">
         <f t="shared" si="20"/>
-        <v>533414.12705302157</v>
+        <v>444364.15690351161</v>
       </c>
       <c r="J31" s="25">
         <f t="shared" si="21"/>
-        <v>-1074838.8729469785</v>
+        <v>-1163888.8430964884</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="22"/>
-        <v>1630.2387746119241</v>
+        <v>1358.0811641305368</v>
       </c>
       <c r="L31" s="25">
         <f t="shared" si="23"/>
-        <v>88954.485528280609</v>
+        <v>66385.430038544349</v>
       </c>
       <c r="M31" s="27">
         <f t="shared" si="24"/>
-        <v>0.20014074893980882</v>
+        <v>0.17563271507145034</v>
       </c>
       <c r="N31" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13166202423238171</v>
+        <v>-0.15617005810074019</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -2074,27 +2073,27 @@
       </c>
       <c r="I32" s="19">
         <f t="shared" si="20"/>
-        <v>640121.35792597302</v>
+        <v>522119.62428060826</v>
       </c>
       <c r="J32" s="25">
         <f t="shared" si="21"/>
-        <v>-1501754.6420740271</v>
+        <v>-1619756.3757193917</v>
       </c>
       <c r="K32" s="26">
         <f t="shared" si="22"/>
-        <v>1956.3611183556632</v>
+        <v>1595.7201231069935</v>
       </c>
       <c r="L32" s="25">
         <f t="shared" si="23"/>
-        <v>106707.23087295145</v>
+        <v>77755.467377096647</v>
       </c>
       <c r="M32" s="27">
         <f t="shared" si="24"/>
-        <v>0.20004575331081306</v>
+        <v>0.17498141145974633</v>
       </c>
       <c r="N32" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13175701986137747</v>
+        <v>-0.15682136171244421</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -2124,27 +2123,27 @@
       </c>
       <c r="I33" s="19">
         <f t="shared" si="20"/>
-        <v>768262.2322835807</v>
+        <v>613522.89372158388</v>
       </c>
       <c r="J33" s="25">
         <f t="shared" si="21"/>
-        <v>-2084293.7677164194</v>
+        <v>-2239033.1062784162</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="22"/>
-        <v>2347.9897074681562</v>
+        <v>1875.0699685867478</v>
       </c>
       <c r="L33" s="25">
         <f t="shared" si="23"/>
-        <v>128140.87435760768</v>
+        <v>91403.269440975622</v>
       </c>
       <c r="M33" s="27">
         <f t="shared" si="24"/>
-        <v>0.20018215729090946</v>
+        <v>0.1750619306196616</v>
       </c>
       <c r="N33" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13162061588128107</v>
+        <v>-0.15674084255252893</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
@@ -2174,27 +2173,27 @@
       </c>
       <c r="I34" s="19">
         <f t="shared" si="20"/>
-        <v>922009.08780773997</v>
+        <v>721027.65896936622</v>
       </c>
       <c r="J34" s="25">
         <f t="shared" si="21"/>
-        <v>-2877032.9121922599</v>
+        <v>-3078014.341030634</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="22"/>
-        <v>2817.8761852314792</v>
+        <v>2203.6297645763029</v>
       </c>
       <c r="L34" s="25">
         <f t="shared" si="23"/>
-        <v>153746.85552415927</v>
+        <v>107504.76524778234</v>
       </c>
       <c r="M34" s="27">
         <f t="shared" si="24"/>
-        <v>0.20012288651384372</v>
+        <v>0.1752253523836193</v>
       </c>
       <c r="N34" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13167988665834682</v>
+        <v>-0.15657742078857123</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
@@ -2224,27 +2223,27 @@
       </c>
       <c r="I35" s="19">
         <f t="shared" si="20"/>
-        <v>1106518.7180787977</v>
+        <v>847272.07800222351</v>
       </c>
       <c r="J35" s="25">
         <f t="shared" si="21"/>
-        <v>-3953056.2819212023</v>
+        <v>-4212302.9219977763</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="22"/>
-        <v>3381.7809232237091</v>
+        <v>2589.4623410825902</v>
       </c>
       <c r="L35" s="25">
         <f t="shared" si="23"/>
-        <v>184509.63027105771</v>
+        <v>126244.41903285729</v>
       </c>
       <c r="M35" s="27">
         <f t="shared" si="24"/>
-        <v>0.20011693237185554</v>
+        <v>0.1750895648210091</v>
       </c>
       <c r="N35" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13168584080033499</v>
+        <v>-0.15671320835118144</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -2274,27 +2273,27 @@
       </c>
       <c r="I36" s="19">
         <f t="shared" si="20"/>
-        <v>1327978.1032072243</v>
+        <v>995651.12253233825</v>
       </c>
       <c r="J36" s="25">
         <f t="shared" si="21"/>
-        <v>-5410377.896792776</v>
+        <v>-5742704.8774676621</v>
       </c>
       <c r="K36" s="26">
         <f t="shared" si="22"/>
-        <v>4058.612784863155</v>
+        <v>3042.9435285218165</v>
       </c>
       <c r="L36" s="25">
         <f t="shared" si="23"/>
-        <v>221459.3851284266</v>
+        <v>148379.04453011474</v>
       </c>
       <c r="M36" s="27">
         <f t="shared" si="24"/>
-        <v>0.20014065872553632</v>
+        <v>0.17512561594143003</v>
       </c>
       <c r="N36" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13166211444665421</v>
+        <v>-0.15667715723076051</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -2324,27 +2323,27 @@
       </c>
       <c r="I37" s="19">
         <f t="shared" si="20"/>
-        <v>1593742.1458274962</v>
+        <v>1170036.2747492928</v>
       </c>
       <c r="J37" s="25">
         <f t="shared" si="21"/>
-        <v>-7380418.8541725036</v>
+        <v>-7804124.725250707</v>
       </c>
       <c r="K37" s="26">
         <f t="shared" si="22"/>
-        <v>4870.85007893489</v>
+        <v>3575.9054851751002</v>
       </c>
       <c r="L37" s="25">
         <f t="shared" si="23"/>
-        <v>265764.04262027191</v>
+        <v>174385.15221695451</v>
       </c>
       <c r="M37" s="27">
         <f t="shared" si="24"/>
-        <v>0.20012682587041178</v>
+        <v>0.17514684438201952</v>
       </c>
       <c r="N37" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13167594730177876</v>
+        <v>-0.15665592879017101</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
@@ -2374,27 +2373,27 @@
       </c>
       <c r="I38" s="19">
         <f t="shared" si="20"/>
-        <v>1912694.7955007155</v>
+        <v>1374933.817014215</v>
       </c>
       <c r="J38" s="25">
         <f t="shared" si="21"/>
-        <v>-10039118.204499284</v>
+        <v>-10576879.182985784</v>
       </c>
       <c r="K38" s="26">
         <f t="shared" si="22"/>
-        <v>5845.6442405278594</v>
+        <v>4202.1204676473571</v>
       </c>
       <c r="L38" s="25">
         <f t="shared" si="23"/>
-        <v>318952.6496732193</v>
+        <v>204897.54226492229</v>
       </c>
       <c r="M38" s="27">
         <f t="shared" si="24"/>
-        <v>0.20012813898926796</v>
+        <v>0.17512067504815293</v>
       </c>
       <c r="N38" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13167463418292258</v>
+        <v>-0.15668209812403761</v>
       </c>
       <c r="P38" t="s">
         <v>20</v>
@@ -2427,27 +2426,27 @@
       </c>
       <c r="I39" s="19">
         <f t="shared" si="20"/>
-        <v>2295485.9903249987</v>
+        <v>1615727.4133640628</v>
       </c>
       <c r="J39" s="25">
         <f t="shared" si="21"/>
-        <v>-13621972.009675002</v>
+        <v>-14301730.586635938</v>
       </c>
       <c r="K39" s="26">
         <f t="shared" si="22"/>
-        <v>7015.5439802108758</v>
+        <v>4938.0422168828318</v>
       </c>
       <c r="L39" s="25">
         <f t="shared" si="23"/>
-        <v>382791.19482428324</v>
+        <v>240793.59634984774</v>
       </c>
       <c r="M39" s="27">
         <f t="shared" si="24"/>
-        <v>0.20013187452840542</v>
+        <v>0.1751310451238674</v>
       </c>
       <c r="N39" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13167089864378512</v>
+        <v>-0.15667172804832313</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -2477,27 +2476,27 @@
       </c>
       <c r="I40" s="19">
         <f t="shared" si="20"/>
-        <v>2754879.1831886168</v>
+        <v>1898694.3679280931</v>
       </c>
       <c r="J40" s="25">
         <f t="shared" si="21"/>
-        <v>-18444035.816811383</v>
+        <v>-19300220.632071909</v>
       </c>
       <c r="K40" s="26">
         <f t="shared" si="22"/>
-        <v>8419.5574058331804</v>
+        <v>5802.8556477019965</v>
       </c>
       <c r="L40" s="25">
         <f t="shared" si="23"/>
-        <v>459393.19286361802</v>
+        <v>282966.95456403028</v>
       </c>
       <c r="M40" s="27">
         <f t="shared" si="24"/>
-        <v>0.20012894646269497</v>
+        <v>0.17513285485134672</v>
       </c>
       <c r="N40" s="27">
         <f t="shared" si="25"/>
-        <v>-0.13167382670949557</v>
+        <v>-0.15666991832084382</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
@@ -2527,27 +2526,27 @@
       </c>
       <c r="I41" s="19">
         <f t="shared" ref="I41" si="28">I40*(1+AVERAGE(M38:M40))</f>
-        <v>3306212.199077344</v>
+        <v>2231209.2791258134</v>
       </c>
       <c r="J41" s="25">
         <f t="shared" ref="J41" si="29">IF(I41&lt;=0,0, I41-B41)</f>
-        <v>-24926561.800922655</v>
+        <v>-26001564.720874187</v>
       </c>
       <c r="K41" s="26">
         <f t="shared" ref="K41" si="30">IF(I41&lt;=0,0, I41/$P$15*1000000)</f>
-        <v>10104.56051062758</v>
+        <v>6819.0992638319476</v>
       </c>
       <c r="L41" s="25">
         <f t="shared" ref="L41" si="31">IF(I41&lt;=0,0, I41-I40)</f>
-        <v>551333.01588872727</v>
+        <v>332514.91119772033</v>
       </c>
       <c r="M41" s="27">
         <f t="shared" ref="M41" si="32">IF(I41&lt;=0,0, L41/I40)</f>
-        <v>0.20012965332678964</v>
+        <v>0.17512819167445556</v>
       </c>
       <c r="N41" s="27">
         <f t="shared" ref="N41" si="33">IF(I41&lt;=0,0,M41-E41)</f>
-        <v>-0.13167311984540089</v>
+        <v>-0.15667458149773497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stats for Mar 30
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208A9C51-EC4D-844D-A1E3-831C91E6EDC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0F88B7-F632-5A46-8BB1-452040AAAC2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28720" yWindow="1860" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -581,7 +581,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1721,29 +1721,28 @@
         <f t="shared" si="0"/>
         <v>43920</v>
       </c>
-      <c r="I25" s="19">
-        <f t="shared" ref="I25:I29" si="17">I24*(1+AVERAGE(M22:M24))</f>
-        <v>168975.64411262303</v>
+      <c r="I25" s="18">
+        <v>163788</v>
       </c>
       <c r="J25" s="25">
         <f t="shared" si="2"/>
-        <v>-119238.35588737697</v>
+        <v>-124426</v>
       </c>
       <c r="K25" s="26">
         <f t="shared" si="7"/>
-        <v>516.42923017305327</v>
+        <v>500.57457212713933</v>
       </c>
       <c r="L25" s="25">
         <f t="shared" si="11"/>
-        <v>26515.644112623035</v>
+        <v>21328</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="12"/>
-        <v>0.18612694168624902</v>
+        <v>0.14971219991576584</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="8"/>
-        <v>-0.14567583148594151</v>
+        <v>-0.18209057325642469</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
@@ -1772,28 +1771,28 @@
         <v>43921</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="17"/>
-        <v>198587.68284855862</v>
+        <f>I25*(1+AVERAGE(M24:M25))</f>
+        <v>188561.45802285243</v>
       </c>
       <c r="J26" s="25">
         <f t="shared" si="2"/>
-        <v>-185256.31715144138</v>
+        <v>-195282.54197714757</v>
       </c>
       <c r="K26" s="26">
         <f t="shared" si="7"/>
-        <v>606.93057105305195</v>
+        <v>576.28807464196962</v>
       </c>
       <c r="L26" s="25">
         <f t="shared" si="11"/>
-        <v>29612.038735935581</v>
+        <v>24773.458022852428</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="12"/>
-        <v>0.17524441993663314</v>
+        <v>0.15125319329164791</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="8"/>
-        <v>-0.15655835323555739</v>
+        <v>-0.18054957988054263</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
@@ -1822,28 +1821,28 @@
         <v>43922</v>
       </c>
       <c r="I27" s="19">
-        <f t="shared" si="17"/>
-        <v>232623.33112707583</v>
+        <f t="shared" ref="I25:I29" si="17">I26*(1+AVERAGE(M24:M26))</f>
+        <v>217081.98068053788</v>
       </c>
       <c r="J27" s="25">
         <f t="shared" si="2"/>
-        <v>-278581.66887292417</v>
+        <v>-294123.01931946212</v>
       </c>
       <c r="K27" s="26">
         <f t="shared" si="7"/>
-        <v>710.95150099962052</v>
+        <v>663.453486187463</v>
       </c>
       <c r="L27" s="25">
         <f t="shared" si="11"/>
-        <v>34035.648278517212</v>
+        <v>28520.522657685447</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="12"/>
-        <v>0.17138851609680408</v>
+        <v>0.15125319329164788</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="8"/>
-        <v>-0.16041425707538645</v>
+        <v>-0.18054957988054265</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
@@ -1873,27 +1872,27 @@
       </c>
       <c r="I28" s="19">
         <f t="shared" si="17"/>
-        <v>273934.12360907817</v>
+        <v>249804.81616646104</v>
       </c>
       <c r="J28" s="25">
         <f t="shared" si="2"/>
-        <v>-406889.87639092183</v>
+        <v>-431019.18383353896</v>
       </c>
       <c r="K28" s="26">
         <f t="shared" si="7"/>
-        <v>837.20697924534898</v>
+        <v>763.46215209798606</v>
       </c>
       <c r="L28" s="25">
         <f t="shared" si="11"/>
-        <v>41310.792482002347</v>
+        <v>32722.835485923162</v>
       </c>
       <c r="M28" s="27">
         <f t="shared" si="12"/>
-        <v>0.17758662590656213</v>
+        <v>0.15073952883302061</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="8"/>
-        <v>-0.15421614726562841</v>
+        <v>-0.18106324433916993</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
@@ -1923,27 +1922,27 @@
       </c>
       <c r="I29" s="19">
         <f t="shared" si="17"/>
-        <v>321801.3323686677</v>
+        <v>287545.82035938511</v>
       </c>
       <c r="J29" s="25">
         <f t="shared" si="2"/>
-        <v>-584921.6676313323</v>
+        <v>-619177.17964061489</v>
       </c>
       <c r="K29" s="26">
         <f t="shared" si="7"/>
-        <v>983.50040454971793</v>
+        <v>878.80751943577354</v>
       </c>
       <c r="L29" s="25">
         <f t="shared" si="11"/>
-        <v>47867.208759589528</v>
+        <v>37741.004192924069</v>
       </c>
       <c r="M29" s="27">
         <f t="shared" si="12"/>
-        <v>0.17473985397999978</v>
+        <v>0.15108197180543873</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="8"/>
-        <v>-0.15706291919219076</v>
+        <v>-0.18072080136675181</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
@@ -1973,27 +1972,27 @@
       </c>
       <c r="I30" s="19">
         <f t="shared" ref="I30:I40" si="20">I29*(1+AVERAGE(M27:M29))</f>
-        <v>377978.72686496726</v>
+        <v>330972.3985427884</v>
       </c>
       <c r="J30" s="25">
         <f t="shared" ref="J30:J40" si="21">IF(I30&lt;=0,0, I30-B30)</f>
-        <v>-829597.27313503274</v>
+        <v>-876603.60145721165</v>
       </c>
       <c r="K30" s="26">
         <f t="shared" ref="K30:K40" si="22">IF(I30&lt;=0,0, I30/$P$15*1000000)</f>
-        <v>1155.1917080225162</v>
+        <v>1011.5293353997201</v>
       </c>
       <c r="L30" s="25">
         <f t="shared" ref="L30:L40" si="23">IF(I30&lt;=0,0, I30-I29)</f>
-        <v>56177.394496299559</v>
+        <v>43426.578183403297</v>
       </c>
       <c r="M30" s="27">
         <f t="shared" ref="M30:M40" si="24">IF(I30&lt;=0,0, L30/I29)</f>
-        <v>0.1745716653277887</v>
+        <v>0.15102489797670227</v>
       </c>
       <c r="N30" s="27">
         <f t="shared" ref="N30:N40" si="25">IF(I30&lt;=0,0,M30-E30)</f>
-        <v>-0.15723110784440184</v>
+        <v>-0.18077787519548827</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
@@ -2023,27 +2022,27 @@
       </c>
       <c r="I31" s="19">
         <f t="shared" si="20"/>
-        <v>444364.15690351161</v>
+        <v>380932.28478316293</v>
       </c>
       <c r="J31" s="25">
         <f t="shared" si="21"/>
-        <v>-1163888.8430964884</v>
+        <v>-1227320.7152168371</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="22"/>
-        <v>1358.0811641305368</v>
+        <v>1164.2184742761704</v>
       </c>
       <c r="L31" s="25">
         <f t="shared" si="23"/>
-        <v>66385.430038544349</v>
+        <v>49959.88624037453</v>
       </c>
       <c r="M31" s="27">
         <f t="shared" si="24"/>
-        <v>0.17563271507145034</v>
+        <v>0.15094879953838711</v>
       </c>
       <c r="N31" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15617005810074019</v>
+        <v>-0.18085397363380343</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -2073,27 +2072,27 @@
       </c>
       <c r="I32" s="19">
         <f t="shared" si="20"/>
-        <v>522119.62428060826</v>
+        <v>438460.12853257422</v>
       </c>
       <c r="J32" s="25">
         <f t="shared" si="21"/>
-        <v>-1619756.3757193917</v>
+        <v>-1703415.8714674257</v>
       </c>
       <c r="K32" s="26">
         <f t="shared" si="22"/>
-        <v>1595.7201231069935</v>
+        <v>1340.0370676423418</v>
       </c>
       <c r="L32" s="25">
         <f t="shared" si="23"/>
-        <v>77755.467377096647</v>
+        <v>57527.843749411288</v>
       </c>
       <c r="M32" s="27">
         <f t="shared" si="24"/>
-        <v>0.17498141145974633</v>
+        <v>0.151018556440176</v>
       </c>
       <c r="N32" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15682136171244421</v>
+        <v>-0.18078421673201453</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -2123,27 +2122,27 @@
       </c>
       <c r="I33" s="19">
         <f t="shared" si="20"/>
-        <v>613522.89372158388</v>
+        <v>504666.47583040298</v>
       </c>
       <c r="J33" s="25">
         <f t="shared" si="21"/>
-        <v>-2239033.1062784162</v>
+        <v>-2347889.5241695968</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="22"/>
-        <v>1875.0699685867478</v>
+        <v>1542.3792048606449</v>
       </c>
       <c r="L33" s="25">
         <f t="shared" si="23"/>
-        <v>91403.269440975622</v>
+        <v>66206.347297828761</v>
       </c>
       <c r="M33" s="27">
         <f t="shared" si="24"/>
-        <v>0.1750619306196616</v>
+        <v>0.15099741798508856</v>
       </c>
       <c r="N33" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15674084255252893</v>
+        <v>-0.18080535518710197</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
@@ -2173,27 +2172,27 @@
       </c>
       <c r="I34" s="19">
         <f t="shared" si="20"/>
-        <v>721027.65896936622</v>
+        <v>580865.18788092001</v>
       </c>
       <c r="J34" s="25">
         <f t="shared" si="21"/>
-        <v>-3078014.341030634</v>
+        <v>-3218176.8121190798</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="22"/>
-        <v>2203.6297645763029</v>
+        <v>1775.260354159291</v>
       </c>
       <c r="L34" s="25">
         <f t="shared" si="23"/>
-        <v>107504.76524778234</v>
+        <v>76198.712050517031</v>
       </c>
       <c r="M34" s="27">
         <f t="shared" si="24"/>
-        <v>0.1752253523836193</v>
+        <v>0.15098825798788384</v>
       </c>
       <c r="N34" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15657742078857123</v>
+        <v>-0.18081451518430669</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
@@ -2223,27 +2222,27 @@
       </c>
       <c r="I35" s="19">
         <f t="shared" si="20"/>
-        <v>847272.07800222351</v>
+        <v>668576.65073809191</v>
       </c>
       <c r="J35" s="25">
         <f t="shared" si="21"/>
-        <v>-4212302.9219977763</v>
+        <v>-4390998.3492619079</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="22"/>
-        <v>2589.4623410825902</v>
+        <v>2043.3271721824326</v>
       </c>
       <c r="L35" s="25">
         <f t="shared" si="23"/>
-        <v>126244.41903285729</v>
+        <v>87711.462857171893</v>
       </c>
       <c r="M35" s="27">
         <f t="shared" si="24"/>
-        <v>0.1750895648210091</v>
+        <v>0.15100141080438295</v>
       </c>
       <c r="N35" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15671320835118144</v>
+        <v>-0.18080136236780758</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -2273,27 +2272,27 @@
       </c>
       <c r="I36" s="19">
         <f t="shared" si="20"/>
-        <v>995651.12253233825</v>
+        <v>769528.8471731618</v>
       </c>
       <c r="J36" s="25">
         <f t="shared" si="21"/>
-        <v>-5742704.8774676621</v>
+        <v>-5968827.1528268382</v>
       </c>
       <c r="K36" s="26">
         <f t="shared" si="22"/>
-        <v>3042.9435285218165</v>
+        <v>2351.8607798690764</v>
       </c>
       <c r="L36" s="25">
         <f t="shared" si="23"/>
-        <v>148379.04453011474</v>
+        <v>100952.1964350699</v>
       </c>
       <c r="M36" s="27">
         <f t="shared" si="24"/>
-        <v>0.17512561594143003</v>
+        <v>0.15099569559245182</v>
       </c>
       <c r="N36" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15667715723076051</v>
+        <v>-0.18080707757973871</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -2323,27 +2322,27 @@
       </c>
       <c r="I37" s="19">
         <f t="shared" si="20"/>
-        <v>1170036.2747492928</v>
+        <v>885723.94892025751</v>
       </c>
       <c r="J37" s="25">
         <f t="shared" si="21"/>
-        <v>-7804124.725250707</v>
+        <v>-8088437.0510797426</v>
       </c>
       <c r="K37" s="26">
         <f t="shared" si="22"/>
-        <v>3575.9054851751002</v>
+        <v>2706.9802839861172</v>
       </c>
       <c r="L37" s="25">
         <f t="shared" si="23"/>
-        <v>174385.15221695451</v>
+        <v>116195.1017470957</v>
       </c>
       <c r="M37" s="27">
         <f t="shared" si="24"/>
-        <v>0.17514684438201952</v>
+        <v>0.15099512146157285</v>
       </c>
       <c r="N37" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15665592879017101</v>
+        <v>-0.18080765171061769</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
@@ -2373,27 +2372,27 @@
       </c>
       <c r="I38" s="19">
         <f t="shared" si="20"/>
-        <v>1374933.817014215</v>
+        <v>1019465.9705499022</v>
       </c>
       <c r="J38" s="25">
         <f t="shared" si="21"/>
-        <v>-10576879.182985784</v>
+        <v>-10932347.029450098</v>
       </c>
       <c r="K38" s="26">
         <f t="shared" si="22"/>
-        <v>4202.1204676473571</v>
+        <v>3115.7272938566693</v>
       </c>
       <c r="L38" s="25">
         <f t="shared" si="23"/>
-        <v>204897.54226492229</v>
+        <v>133742.02162964467</v>
       </c>
       <c r="M38" s="27">
         <f t="shared" si="24"/>
-        <v>0.17512067504815293</v>
+        <v>0.15099740928613592</v>
       </c>
       <c r="N38" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15668209812403761</v>
+        <v>-0.18080536388605462</v>
       </c>
       <c r="P38" t="s">
         <v>20</v>
@@ -2426,27 +2425,27 @@
       </c>
       <c r="I39" s="19">
         <f t="shared" si="20"/>
-        <v>1615727.4133640628</v>
+        <v>1173401.3311544189</v>
       </c>
       <c r="J39" s="25">
         <f t="shared" si="21"/>
-        <v>-14301730.586635938</v>
+        <v>-14744056.668845581</v>
       </c>
       <c r="K39" s="26">
         <f t="shared" si="22"/>
-        <v>4938.0422168828318</v>
+        <v>3586.1898873912555</v>
       </c>
       <c r="L39" s="25">
         <f t="shared" si="23"/>
-        <v>240793.59634984774</v>
+        <v>153935.3606045167</v>
       </c>
       <c r="M39" s="27">
         <f t="shared" si="24"/>
-        <v>0.1751310451238674</v>
+        <v>0.15099607544672003</v>
       </c>
       <c r="N39" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15667172804832313</v>
+        <v>-0.18080669772547051</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -2476,27 +2475,27 @@
       </c>
       <c r="I40" s="19">
         <f t="shared" si="20"/>
-        <v>1898694.3679280931</v>
+        <v>1350580.4756565283</v>
       </c>
       <c r="J40" s="25">
         <f t="shared" si="21"/>
-        <v>-19300220.632071909</v>
+        <v>-19848334.524343472</v>
       </c>
       <c r="K40" s="26">
         <f t="shared" si="22"/>
-        <v>5802.8556477019965</v>
+        <v>4127.6909402705633</v>
       </c>
       <c r="L40" s="25">
         <f t="shared" si="23"/>
-        <v>282966.95456403028</v>
+        <v>177179.14450210938</v>
       </c>
       <c r="M40" s="27">
         <f t="shared" si="24"/>
-        <v>0.17513285485134672</v>
+        <v>0.15099620206480976</v>
       </c>
       <c r="N40" s="27">
         <f t="shared" si="25"/>
-        <v>-0.15666991832084382</v>
+        <v>-0.18080657110738077</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
@@ -2526,27 +2525,27 @@
       </c>
       <c r="I41" s="19">
         <f t="shared" ref="I41" si="28">I40*(1+AVERAGE(M38:M40))</f>
-        <v>2231209.2791258134</v>
+        <v>1554513.4845440928</v>
       </c>
       <c r="J41" s="25">
         <f t="shared" ref="J41" si="29">IF(I41&lt;=0,0, I41-B41)</f>
-        <v>-26001564.720874187</v>
+        <v>-26678260.515455909</v>
       </c>
       <c r="K41" s="26">
         <f t="shared" ref="K41" si="30">IF(I41&lt;=0,0, I41/$P$15*1000000)</f>
-        <v>6819.0992638319476</v>
+        <v>4750.9580823474726</v>
       </c>
       <c r="L41" s="25">
         <f t="shared" ref="L41" si="31">IF(I41&lt;=0,0, I41-I40)</f>
-        <v>332514.91119772033</v>
+        <v>203933.00888756453</v>
       </c>
       <c r="M41" s="27">
         <f t="shared" ref="M41" si="32">IF(I41&lt;=0,0, L41/I40)</f>
-        <v>0.17512819167445556</v>
+        <v>0.1509965622658887</v>
       </c>
       <c r="N41" s="27">
         <f t="shared" ref="N41" si="33">IF(I41&lt;=0,0,M41-E41)</f>
-        <v>-0.15667458149773497</v>
+        <v>-0.18080621090630183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data for Apr 1, added US county data from NY Times dataset
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F297725-F84D-2B44-AEF6-A305B5A43DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1763B1F2-184C-F34E-90B5-D9C8EB8C0EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
+    <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -606,8 +606,8 @@
   <dimension ref="A1:Q59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -2283,29 +2283,28 @@
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-      <c r="I35" s="15">
-        <f t="shared" ref="I35:I37" si="29">I34*(1+AVERAGE(M32:M34))</f>
-        <v>217033.69449552009</v>
+      <c r="I35" s="14">
+        <v>215003</v>
       </c>
       <c r="J35" s="21">
         <f t="shared" si="14"/>
-        <v>-294171.30550447991</v>
+        <v>-296202</v>
       </c>
       <c r="K35" s="22">
         <f t="shared" si="18"/>
-        <v>663.30591227237187</v>
+        <v>657.09963325183378</v>
       </c>
       <c r="L35" s="21">
         <f t="shared" si="23"/>
-        <v>28503.694495520089</v>
+        <v>26473</v>
       </c>
       <c r="M35" s="23">
         <f t="shared" si="24"/>
-        <v>0.15118917146088204</v>
+        <v>0.14041797061475628</v>
       </c>
       <c r="N35" s="23">
         <f t="shared" si="19"/>
-        <v>-0.1806136017113085</v>
+        <v>-0.19138480255743426</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -2337,28 +2336,28 @@
         <v>43923</v>
       </c>
       <c r="I36" s="15">
-        <f t="shared" si="29"/>
-        <v>249730.72481871853</v>
+        <f t="shared" ref="I35:I37" si="29">I35*(1+AVERAGE(M33:M35))</f>
+        <v>246622.15090493916</v>
       </c>
       <c r="J36" s="21">
         <f t="shared" si="14"/>
-        <v>-431093.2751812815</v>
+        <v>-434201.84909506084</v>
       </c>
       <c r="K36" s="22">
         <f t="shared" si="18"/>
-        <v>763.23571154865078</v>
+        <v>753.7351800273201</v>
       </c>
       <c r="L36" s="21">
         <f t="shared" si="23"/>
-        <v>32697.030323198444</v>
+        <v>31619.150904939161</v>
       </c>
       <c r="M36" s="23">
         <f t="shared" si="24"/>
-        <v>0.15065416639199938</v>
+        <v>0.14706376610995736</v>
       </c>
       <c r="N36" s="23">
         <f t="shared" si="19"/>
-        <v>-0.18114860678019115</v>
+        <v>-0.18473900706223317</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -2391,27 +2390,27 @@
       </c>
       <c r="I37" s="15">
         <f t="shared" si="29"/>
-        <v>287432.11164570734</v>
+        <v>282673.6124092518</v>
       </c>
       <c r="J37" s="21">
         <f t="shared" si="14"/>
-        <v>-619290.88835429261</v>
+        <v>-624049.38759074826</v>
       </c>
       <c r="K37" s="22">
         <f t="shared" si="18"/>
-        <v>878.4599989171985</v>
+        <v>863.91690834123415</v>
       </c>
       <c r="L37" s="21">
         <f t="shared" si="23"/>
-        <v>37701.386826988804</v>
+        <v>36051.46150431264</v>
       </c>
       <c r="M37" s="23">
         <f t="shared" si="24"/>
-        <v>0.1509681552174108</v>
+        <v>0.14618095484135454</v>
       </c>
       <c r="N37" s="23">
         <f t="shared" si="19"/>
-        <v>-0.18083461795477973</v>
+        <v>-0.18562181833083599</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -2444,27 +2443,27 @@
       </c>
       <c r="I38" s="15">
         <f t="shared" ref="I38:I48" si="31">I37*(1+AVERAGE(M35:M37))</f>
-        <v>330816.29952258721</v>
+        <v>323535.27893995168</v>
       </c>
       <c r="J38" s="21">
         <f t="shared" ref="J38:J48" si="32">IF(I38&lt;=0,0, I38-B38)</f>
-        <v>-876759.70047741279</v>
+        <v>-884040.72106004832</v>
       </c>
       <c r="K38" s="22">
         <f t="shared" si="18"/>
-        <v>1011.0522601546063</v>
+        <v>988.7997522614661</v>
       </c>
       <c r="L38" s="21">
         <f t="shared" ref="L38:L48" si="33">IF(I38&lt;=0,0, I38-I37)</f>
-        <v>43384.187876879878</v>
+        <v>40861.666530699877</v>
       </c>
       <c r="M38" s="23">
         <f t="shared" ref="M38:M48" si="34">IF(I38&lt;=0,0, L38/I37)</f>
-        <v>0.15093716435676405</v>
+        <v>0.14455423052202268</v>
       </c>
       <c r="N38" s="23">
         <f t="shared" ref="N38:N48" si="35">IF(I38&lt;=0,0,M38-E38)</f>
-        <v>-0.18086560881542649</v>
+        <v>-0.18724854265016785</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2497,27 +2496,27 @@
       </c>
       <c r="I39" s="15">
         <f t="shared" si="31"/>
-        <v>380720.98434297857</v>
+        <v>370749.74756813288</v>
       </c>
       <c r="J39" s="21">
         <f t="shared" si="32"/>
-        <v>-1227532.0156570214</v>
+        <v>-1237503.2524318672</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="18"/>
-        <v>1163.5726905347756</v>
+        <v>1133.0982505138536</v>
       </c>
       <c r="L39" s="21">
         <f t="shared" si="33"/>
-        <v>49904.684820391354</v>
+        <v>47214.468628181203</v>
       </c>
       <c r="M39" s="23">
         <f t="shared" si="34"/>
-        <v>0.15085316198872481</v>
+        <v>0.14593298382444481</v>
       </c>
       <c r="N39" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18094961118346573</v>
+        <v>-0.18586978934774573</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2550,27 +2549,27 @@
       </c>
       <c r="I40" s="15">
         <f t="shared" si="31"/>
-        <v>438179.20259973174</v>
+        <v>424714.61873394076</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="32"/>
-        <v>-1703696.7974002683</v>
+        <v>-1717161.3812660594</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1339.1784920529699</v>
+        <v>1298.0275633677898</v>
       </c>
       <c r="L40" s="21">
         <f t="shared" si="33"/>
-        <v>57458.218256753171</v>
+        <v>53964.871165807883</v>
       </c>
       <c r="M40" s="23">
         <f t="shared" si="34"/>
-        <v>0.15091949385429992</v>
+        <v>0.14555605639594058</v>
       </c>
       <c r="N40" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18088327931789061</v>
+        <v>-0.18624671677624996</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2603,27 +2602,27 @@
       </c>
       <c r="I41" s="15">
         <f t="shared" si="31"/>
-        <v>504301.87860780221</v>
+        <v>486445.93589556153</v>
       </c>
       <c r="J41" s="21">
         <f t="shared" si="32"/>
-        <v>-2348254.1213921979</v>
+        <v>-2366110.0641044383</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1541.2649101705447</v>
+        <v>1486.6929581160193</v>
       </c>
       <c r="L41" s="21">
         <f t="shared" si="33"/>
-        <v>66122.67600807047</v>
+        <v>61731.317161620769</v>
       </c>
       <c r="M41" s="23">
         <f t="shared" si="34"/>
-        <v>0.15090327339992962</v>
+        <v>0.14534775691413598</v>
       </c>
       <c r="N41" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18089949977226091</v>
+        <v>-0.18645501625805455</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2656,27 +2655,27 @@
       </c>
       <c r="I42" s="15">
         <f t="shared" si="31"/>
-        <v>580396.98578038707</v>
+        <v>557278.43076746876</v>
       </c>
       <c r="J42" s="21">
         <f t="shared" si="32"/>
-        <v>-3218645.0142196128</v>
+        <v>-3241763.5692325314</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1773.8294186442147</v>
+        <v>1703.1736881646357</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="33"/>
-        <v>76095.10717258486</v>
+        <v>70832.494871907227</v>
       </c>
       <c r="M42" s="23">
         <f t="shared" si="34"/>
-        <v>0.15089197641431823</v>
+        <v>0.14561226571150704</v>
       </c>
       <c r="N42" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18091079675787231</v>
+        <v>-0.1861905074606835</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2709,27 +2708,27 @@
       </c>
       <c r="I43" s="15">
         <f t="shared" si="31"/>
-        <v>667981.74332824221</v>
+        <v>638365.42927477427</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="32"/>
-        <v>-4391593.2566717574</v>
+        <v>-4421209.5707252258</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>2041.5089955019625</v>
+        <v>1950.9945882480877</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="33"/>
-        <v>87584.757547855144</v>
+        <v>81086.998507305514</v>
       </c>
       <c r="M43" s="23">
         <f t="shared" si="34"/>
-        <v>0.15090491455618243</v>
+        <v>0.14550535967386122</v>
       </c>
       <c r="N43" s="23">
         <f t="shared" si="35"/>
-        <v>-0.1808978586160081</v>
+        <v>-0.18629741349832932</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2762,27 +2761,27 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" si="31"/>
-        <v>768780.22499528946</v>
+        <v>731240.23298650817</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="32"/>
-        <v>-5969575.775004711</v>
+        <v>-6007115.7670134921</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>2349.5728147777795</v>
+        <v>2234.8417878560763</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="33"/>
-        <v>100798.48166704725</v>
+        <v>92874.803711733897</v>
       </c>
       <c r="M44" s="23">
         <f t="shared" si="34"/>
-        <v>0.1509000547901434</v>
+        <v>0.14548846076650152</v>
       </c>
       <c r="N44" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18090271838204713</v>
+        <v>-0.18631431240568902</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2815,27 +2814,27 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" si="31"/>
-        <v>884788.37826747226</v>
+        <v>837661.54504018172</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="32"/>
-        <v>-8089372.6217325274</v>
+        <v>-8136499.4549598182</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>2704.1209604751598</v>
+        <v>2560.0902965775726</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="33"/>
-        <v>116008.1532721828</v>
+        <v>106421.31205367355</v>
       </c>
       <c r="M45" s="23">
         <f t="shared" si="34"/>
-        <v>0.15089898192021473</v>
+        <v>0.14553536205062323</v>
       </c>
       <c r="N45" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18090379125197581</v>
+        <v>-0.18626741112156731</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2868,27 +2867,27 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" si="31"/>
-        <v>1018304.1098929388</v>
+        <v>959549.44819369051</v>
       </c>
       <c r="J46" s="21">
         <f t="shared" si="32"/>
-        <v>-10933508.890107062</v>
+        <v>-10992263.55180631</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>3112.1763749784195</v>
+        <v>2932.6083380002769</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="33"/>
-        <v>133515.73162546649</v>
+        <v>121887.90315350879</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="34"/>
-        <v>0.15090131708884694</v>
+        <v>0.14550972749699517</v>
       </c>
       <c r="N46" s="23">
         <f t="shared" si="35"/>
-        <v>-0.1809014560833436</v>
+        <v>-0.18629304567519536</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2924,27 +2923,27 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" si="31"/>
-        <v>1171966.3201675112</v>
+        <v>1099174.6239676727</v>
       </c>
       <c r="J47" s="21">
         <f t="shared" si="32"/>
-        <v>-14745491.679832488</v>
+        <v>-14818283.376032326</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>3581.8041569911716</v>
+        <v>3359.3356478229603</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="33"/>
-        <v>153662.21027457248</v>
+        <v>139625.17577398219</v>
       </c>
       <c r="M47" s="23">
         <f t="shared" si="34"/>
-        <v>0.15090011793306818</v>
+        <v>0.14551118343804004</v>
       </c>
       <c r="N47" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18090265523912236</v>
+        <v>-0.1862915897341505</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2977,27 +2976,27 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" si="31"/>
-        <v>1348816.2007614998</v>
+        <v>1259125.1497009194</v>
       </c>
       <c r="J48" s="21">
         <f t="shared" si="32"/>
-        <v>-19850098.799238499</v>
+        <v>-19939789.850299079</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>4122.2989020828236</v>
+        <v>3848.1819978634453</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="33"/>
-        <v>176849.88059398858</v>
+        <v>159950.5257332467</v>
       </c>
       <c r="M48" s="23">
         <f t="shared" si="34"/>
-        <v>0.15090013898070989</v>
+        <v>0.14551875766188624</v>
       </c>
       <c r="N48" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18090263419148064</v>
+        <v>-0.1862840155103043</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3030,27 +3029,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="37">I48*(1+AVERAGE(M46:M48))</f>
-        <v>1552353.2731364903</v>
+        <v>1442344.5082250822</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="38">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-26680420.726863511</v>
+        <v>-26790429.491774917</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>4744.355969243552</v>
+        <v>4408.1433625460941</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="39">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>203537.07237499044</v>
+        <v>183219.35852416279</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="40">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.15090052466754159</v>
+        <v>0.14551322286564045</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="41">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.18090224850464895</v>
+        <v>-0.18628955030655009</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated stats for Apr 2
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1763B1F2-184C-F34E-90B5-D9C8EB8C0EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6CFAB-3444-1A44-85D7-6376B6CE60E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
     <col min="5" max="5" width="7.6640625" style="3" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="6" max="6" width="28.5" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="7" max="7" width="3.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="10.5" style="3" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="10.6640625" style="3" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="11" max="11" width="8.1640625" style="3" bestFit="1" customWidth="1" outlineLevel="1" collapsed="1"/>
@@ -2335,29 +2335,28 @@
         <f t="shared" si="0"/>
         <v>43923</v>
       </c>
-      <c r="I36" s="15">
-        <f t="shared" ref="I35:I37" si="29">I35*(1+AVERAGE(M33:M35))</f>
-        <v>246622.15090493916</v>
+      <c r="I36" s="14">
+        <v>244877</v>
       </c>
       <c r="J36" s="21">
         <f t="shared" si="14"/>
-        <v>-434201.84909506084</v>
+        <v>-435947</v>
       </c>
       <c r="K36" s="22">
         <f t="shared" si="18"/>
-        <v>753.7351800273201</v>
+        <v>748.40158924205377</v>
       </c>
       <c r="L36" s="21">
         <f t="shared" si="23"/>
-        <v>31619.150904939161</v>
+        <v>29874</v>
       </c>
       <c r="M36" s="23">
         <f t="shared" si="24"/>
-        <v>0.14706376610995736</v>
+        <v>0.13894689841537095</v>
       </c>
       <c r="N36" s="23">
         <f t="shared" si="19"/>
-        <v>-0.18473900706223317</v>
+        <v>-0.19285587475681959</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
@@ -2389,28 +2388,28 @@
         <v>43924</v>
       </c>
       <c r="I37" s="15">
-        <f t="shared" si="29"/>
-        <v>282673.6124092518</v>
+        <f t="shared" ref="I36:I37" si="29">I36*(1+AVERAGE(M34:M36))</f>
+        <v>280010.80894187069</v>
       </c>
       <c r="J37" s="21">
         <f t="shared" si="14"/>
-        <v>-624049.38759074826</v>
+        <v>-626712.19105812931</v>
       </c>
       <c r="K37" s="22">
         <f t="shared" si="18"/>
-        <v>863.91690834123415</v>
+        <v>855.77875593481269</v>
       </c>
       <c r="L37" s="21">
         <f t="shared" si="23"/>
-        <v>36051.46150431264</v>
+        <v>35133.808941870695</v>
       </c>
       <c r="M37" s="23">
         <f t="shared" si="24"/>
-        <v>0.14618095484135454</v>
+        <v>0.14347533227649267</v>
       </c>
       <c r="N37" s="23">
         <f t="shared" si="19"/>
-        <v>-0.18562181833083599</v>
+        <v>-0.18832744089569786</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -2443,27 +2442,27 @@
       </c>
       <c r="I38" s="15">
         <f t="shared" ref="I38:I48" si="31">I37*(1+AVERAGE(M35:M37))</f>
-        <v>323535.27893995168</v>
+        <v>319477.41788220737</v>
       </c>
       <c r="J38" s="21">
         <f t="shared" ref="J38:J48" si="32">IF(I38&lt;=0,0, I38-B38)</f>
-        <v>-884040.72106004832</v>
+        <v>-888098.58211779268</v>
       </c>
       <c r="K38" s="22">
         <f t="shared" si="18"/>
-        <v>988.7997522614661</v>
+        <v>976.39797641261418</v>
       </c>
       <c r="L38" s="21">
         <f t="shared" ref="L38:L48" si="33">IF(I38&lt;=0,0, I38-I37)</f>
-        <v>40861.666530699877</v>
+        <v>39466.608940336679</v>
       </c>
       <c r="M38" s="23">
         <f t="shared" ref="M38:M48" si="34">IF(I38&lt;=0,0, L38/I37)</f>
-        <v>0.14455423052202268</v>
+        <v>0.14094673376887323</v>
       </c>
       <c r="N38" s="23">
         <f t="shared" ref="N38:N48" si="35">IF(I38&lt;=0,0,M38-E38)</f>
-        <v>-0.18724854265016785</v>
+        <v>-0.1908560394033173</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2496,27 +2495,27 @@
       </c>
       <c r="I39" s="15">
         <f t="shared" si="31"/>
-        <v>370749.74756813288</v>
+        <v>364563.02574133413</v>
       </c>
       <c r="J39" s="21">
         <f t="shared" si="32"/>
-        <v>-1237503.2524318672</v>
+        <v>-1243689.9742586659</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="18"/>
-        <v>1133.0982505138536</v>
+        <v>1114.1901764710701</v>
       </c>
       <c r="L39" s="21">
         <f t="shared" si="33"/>
-        <v>47214.468628181203</v>
+        <v>45085.607859126758</v>
       </c>
       <c r="M39" s="23">
         <f t="shared" si="34"/>
-        <v>0.14593298382444481</v>
+        <v>0.14112298815357899</v>
       </c>
       <c r="N39" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18586978934774573</v>
+        <v>-0.19067978501861155</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2549,27 +2548,27 @@
       </c>
       <c r="I40" s="15">
         <f t="shared" si="31"/>
-        <v>424714.61873394076</v>
+        <v>416275.6899240099</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="32"/>
-        <v>-1717161.3812660594</v>
+        <v>-1725600.3100759902</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1298.0275633677898</v>
+        <v>1272.2362161491744</v>
       </c>
       <c r="L40" s="21">
         <f t="shared" si="33"/>
-        <v>53964.871165807883</v>
+        <v>51712.66418267577</v>
       </c>
       <c r="M40" s="23">
         <f t="shared" si="34"/>
-        <v>0.14555605639594058</v>
+        <v>0.14184835139964824</v>
       </c>
       <c r="N40" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18624671677624996</v>
+        <v>-0.18995442177254229</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2602,27 +2601,27 @@
       </c>
       <c r="I41" s="15">
         <f t="shared" si="31"/>
-        <v>486445.93589556153</v>
+        <v>475097.95273848134</v>
       </c>
       <c r="J41" s="21">
         <f t="shared" si="32"/>
-        <v>-2366110.0641044383</v>
+        <v>-2377458.0472615184</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1486.6929581160193</v>
+        <v>1452.0108580026936</v>
       </c>
       <c r="L41" s="21">
         <f t="shared" si="33"/>
-        <v>61731.317161620769</v>
+        <v>58822.26281447144</v>
       </c>
       <c r="M41" s="23">
         <f t="shared" si="34"/>
-        <v>0.14534775691413598</v>
+        <v>0.14130602444070009</v>
       </c>
       <c r="N41" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18645501625805455</v>
+        <v>-0.19049674873149045</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2655,27 +2654,27 @@
       </c>
       <c r="I42" s="15">
         <f t="shared" si="31"/>
-        <v>557278.43076746876</v>
+        <v>542289.05508074607</v>
       </c>
       <c r="J42" s="21">
         <f t="shared" si="32"/>
-        <v>-3241763.5692325314</v>
+        <v>-3256752.9449192537</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1703.1736881646357</v>
+        <v>1657.3626377773412</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="33"/>
-        <v>70832.494871907227</v>
+        <v>67191.102342264727</v>
       </c>
       <c r="M42" s="23">
         <f t="shared" si="34"/>
-        <v>0.14561226571150704</v>
+        <v>0.14142578799797567</v>
       </c>
       <c r="N42" s="23">
         <f t="shared" si="35"/>
-        <v>-0.1861905074606835</v>
+        <v>-0.19037698517421486</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2708,27 +2707,27 @@
       </c>
       <c r="I43" s="15">
         <f t="shared" si="31"/>
-        <v>638365.42927477427</v>
+        <v>619037.44703205046</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="32"/>
-        <v>-4421209.5707252258</v>
+        <v>-4440537.5529679498</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1950.9945882480877</v>
+        <v>1891.9237378730149</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="33"/>
-        <v>81086.998507305514</v>
+        <v>76748.391951304395</v>
       </c>
       <c r="M43" s="23">
         <f t="shared" si="34"/>
-        <v>0.14550535967386122</v>
+        <v>0.14152672127944141</v>
       </c>
       <c r="N43" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18629741349832932</v>
+        <v>-0.19027605189274913</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2761,27 +2760,27 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" si="31"/>
-        <v>731240.23298650817</v>
+        <v>706581.4202301919</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="32"/>
-        <v>-6007115.7670134921</v>
+        <v>-6031774.5797698079</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>2234.8417878560763</v>
+        <v>2159.4786681851833</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="33"/>
-        <v>92874.803711733897</v>
+        <v>87543.973198141437</v>
       </c>
       <c r="M44" s="23">
         <f t="shared" si="34"/>
-        <v>0.14548846076650152</v>
+        <v>0.14141951123937238</v>
       </c>
       <c r="N44" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18631431240568902</v>
+        <v>-0.19038326193281815</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2814,27 +2813,27 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" si="31"/>
-        <v>837661.54504018172</v>
+        <v>806532.54855109495</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="32"/>
-        <v>-8136499.4549598182</v>
+        <v>-8167628.4514489053</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>2560.0902965775726</v>
+        <v>2464.9527767454001</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="33"/>
-        <v>106421.31205367355</v>
+        <v>99951.128320903052</v>
       </c>
       <c r="M45" s="23">
         <f t="shared" si="34"/>
-        <v>0.14553536205062323</v>
+        <v>0.14145734017226311</v>
       </c>
       <c r="N45" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18626741112156731</v>
+        <v>-0.19034543299992743</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2867,27 +2866,27 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" si="31"/>
-        <v>959549.44819369051</v>
+        <v>920630.98025000293</v>
       </c>
       <c r="J46" s="21">
         <f t="shared" si="32"/>
-        <v>-10992263.55180631</v>
+        <v>-11031182.019749997</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>2932.6083380002769</v>
+        <v>2813.6643650672459</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="33"/>
-        <v>121887.90315350879</v>
+        <v>114098.43169890798</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="34"/>
-        <v>0.14550972749699517</v>
+        <v>0.14146785756369223</v>
       </c>
       <c r="N46" s="23">
         <f t="shared" si="35"/>
-        <v>-0.18629304567519536</v>
+        <v>-0.1903349156084983</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2923,27 +2922,27 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" si="31"/>
-        <v>1099174.6239676727</v>
+        <v>1050852.6087126224</v>
       </c>
       <c r="J47" s="21">
         <f t="shared" si="32"/>
-        <v>-14818283.376032326</v>
+        <v>-14866605.391287377</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>3359.3356478229603</v>
+        <v>3211.6522271168169</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="33"/>
-        <v>139625.17577398219</v>
+        <v>130221.6284626195</v>
       </c>
       <c r="M47" s="23">
         <f t="shared" si="34"/>
-        <v>0.14551118343804004</v>
+        <v>0.14144823632510936</v>
       </c>
       <c r="N47" s="23">
         <f t="shared" si="35"/>
-        <v>-0.1862915897341505</v>
+        <v>-0.19035453684708117</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2976,27 +2975,27 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" si="31"/>
-        <v>1259125.1497009194</v>
+        <v>1199503.9187964236</v>
       </c>
       <c r="J48" s="21">
         <f t="shared" si="32"/>
-        <v>-19939789.850299079</v>
+        <v>-19999411.081203576</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>3848.1819978634453</v>
+        <v>3665.9655219939596</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="33"/>
-        <v>159950.5257332467</v>
+        <v>148651.31008380116</v>
       </c>
       <c r="M48" s="23">
         <f t="shared" si="34"/>
-        <v>0.14551875766188624</v>
+        <v>0.1414578113536881</v>
       </c>
       <c r="N48" s="23">
         <f t="shared" si="35"/>
-        <v>-0.1862840155103043</v>
+        <v>-0.19034496181850244</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3029,27 +3028,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="37">I48*(1+AVERAGE(M46:M48))</f>
-        <v>1442344.5082250822</v>
+        <v>1369183.3062541932</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="38">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-26790429.491774917</v>
+        <v>-26863590.693745807</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>4408.1433625460941</v>
+        <v>4184.5455570115928</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="39">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>183219.35852416279</v>
+        <v>169679.3874577696</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="40">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.14551322286564045</v>
+        <v>0.1414579684141633</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="41">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.18628955030655009</v>
+        <v>-0.19034480475802723</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated stats for Apr 3
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE6CFAB-3444-1A44-85D7-6376B6CE60E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6675B3C5-79FB-7E47-B31C-9EF37E14F2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I37" sqref="I37"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -2387,29 +2387,28 @@
         <f t="shared" si="0"/>
         <v>43924</v>
       </c>
-      <c r="I37" s="15">
-        <f t="shared" ref="I36:I37" si="29">I36*(1+AVERAGE(M34:M36))</f>
-        <v>280010.80894187069</v>
+      <c r="I37" s="14">
+        <v>277161</v>
       </c>
       <c r="J37" s="21">
         <f t="shared" si="14"/>
-        <v>-626712.19105812931</v>
+        <v>-629562</v>
       </c>
       <c r="K37" s="22">
         <f t="shared" si="18"/>
-        <v>855.77875593481269</v>
+        <v>847.0690709046454</v>
       </c>
       <c r="L37" s="21">
         <f t="shared" si="23"/>
-        <v>35133.808941870695</v>
+        <v>32284</v>
       </c>
       <c r="M37" s="23">
         <f t="shared" si="24"/>
-        <v>0.14347533227649267</v>
+        <v>0.13183761643600664</v>
       </c>
       <c r="N37" s="23">
         <f t="shared" si="19"/>
-        <v>-0.18832744089569786</v>
+        <v>-0.1999651567361839</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -2437,32 +2436,32 @@
         <v>4</v>
       </c>
       <c r="H38" s="20">
-        <f t="shared" ref="H38:H48" si="30">A38</f>
+        <f t="shared" ref="H38:H48" si="29">A38</f>
         <v>43925</v>
       </c>
       <c r="I38" s="15">
-        <f t="shared" ref="I38:I48" si="31">I37*(1+AVERAGE(M35:M37))</f>
-        <v>319477.41788220737</v>
+        <f t="shared" ref="I38:I48" si="30">I37*(1+AVERAGE(M35:M37))</f>
+        <v>315150.76402475976</v>
       </c>
       <c r="J38" s="21">
-        <f t="shared" ref="J38:J48" si="32">IF(I38&lt;=0,0, I38-B38)</f>
-        <v>-888098.58211779268</v>
+        <f t="shared" ref="J38:J48" si="31">IF(I38&lt;=0,0, I38-B38)</f>
+        <v>-892425.23597524024</v>
       </c>
       <c r="K38" s="22">
         <f t="shared" si="18"/>
-        <v>976.39797641261418</v>
+        <v>963.1747066771386</v>
       </c>
       <c r="L38" s="21">
-        <f t="shared" ref="L38:L48" si="33">IF(I38&lt;=0,0, I38-I37)</f>
-        <v>39466.608940336679</v>
+        <f t="shared" ref="L38:L48" si="32">IF(I38&lt;=0,0, I38-I37)</f>
+        <v>37989.764024759759</v>
       </c>
       <c r="M38" s="23">
-        <f t="shared" ref="M38:M48" si="34">IF(I38&lt;=0,0, L38/I37)</f>
-        <v>0.14094673376887323</v>
+        <f t="shared" ref="M38:M48" si="33">IF(I38&lt;=0,0, L38/I37)</f>
+        <v>0.13706749515537814</v>
       </c>
       <c r="N38" s="23">
-        <f t="shared" ref="N38:N48" si="35">IF(I38&lt;=0,0,M38-E38)</f>
-        <v>-0.1908560394033173</v>
+        <f t="shared" ref="N38:N48" si="34">IF(I38&lt;=0,0,M38-E38)</f>
+        <v>-0.1947352780168124</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2490,32 +2489,32 @@
         <v>4</v>
       </c>
       <c r="H39" s="20">
+        <f t="shared" si="29"/>
+        <v>43926</v>
+      </c>
+      <c r="I39" s="15">
         <f t="shared" si="30"/>
-        <v>43926</v>
-      </c>
-      <c r="I39" s="15">
+        <v>357995.72154564742</v>
+      </c>
+      <c r="J39" s="21">
         <f t="shared" si="31"/>
-        <v>364563.02574133413</v>
-      </c>
-      <c r="J39" s="21">
-        <f t="shared" si="32"/>
-        <v>-1243689.9742586659</v>
+        <v>-1250257.2784543526</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="18"/>
-        <v>1114.1901764710701</v>
+        <v>1094.118953379118</v>
       </c>
       <c r="L39" s="21">
+        <f t="shared" si="32"/>
+        <v>42844.957520887663</v>
+      </c>
+      <c r="M39" s="23">
         <f t="shared" si="33"/>
-        <v>45085.607859126758</v>
-      </c>
-      <c r="M39" s="23">
+        <v>0.13595067000225186</v>
+      </c>
+      <c r="N39" s="23">
         <f t="shared" si="34"/>
-        <v>0.14112298815357899</v>
-      </c>
-      <c r="N39" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19067978501861155</v>
+        <v>-0.19585210316993867</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2543,32 +2542,32 @@
         <v>4</v>
       </c>
       <c r="H40" s="20">
+        <f t="shared" si="29"/>
+        <v>43927</v>
+      </c>
+      <c r="I40" s="15">
         <f t="shared" si="30"/>
-        <v>43927</v>
-      </c>
-      <c r="I40" s="15">
+        <v>406307.93409682775</v>
+      </c>
+      <c r="J40" s="21">
         <f t="shared" si="31"/>
-        <v>416275.6899240099</v>
-      </c>
-      <c r="J40" s="21">
-        <f t="shared" si="32"/>
-        <v>-1725600.3100759902</v>
+        <v>-1735568.0659031724</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1272.2362161491744</v>
+        <v>1241.7724147213562</v>
       </c>
       <c r="L40" s="21">
+        <f t="shared" si="32"/>
+        <v>48312.212551180332</v>
+      </c>
+      <c r="M40" s="23">
         <f t="shared" si="33"/>
-        <v>51712.66418267577</v>
-      </c>
-      <c r="M40" s="23">
+        <v>0.13495192719787888</v>
+      </c>
+      <c r="N40" s="23">
         <f t="shared" si="34"/>
-        <v>0.14184835139964824</v>
-      </c>
-      <c r="N40" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.18995442177254229</v>
+        <v>-0.19685084597431166</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2596,32 +2595,32 @@
         <v>4</v>
       </c>
       <c r="H41" s="20">
+        <f t="shared" si="29"/>
+        <v>43928</v>
+      </c>
+      <c r="I41" s="15">
         <f t="shared" si="30"/>
-        <v>43928</v>
-      </c>
-      <c r="I41" s="15">
+        <v>461561.76256291399</v>
+      </c>
+      <c r="J41" s="21">
         <f t="shared" si="31"/>
-        <v>475097.95273848134</v>
-      </c>
-      <c r="J41" s="21">
-        <f t="shared" si="32"/>
-        <v>-2377458.0472615184</v>
+        <v>-2390994.2374370862</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1452.0108580026936</v>
+        <v>1410.6410836274877</v>
       </c>
       <c r="L41" s="21">
+        <f t="shared" si="32"/>
+        <v>55253.828466086241</v>
+      </c>
+      <c r="M41" s="23">
         <f t="shared" si="33"/>
-        <v>58822.26281447144</v>
-      </c>
-      <c r="M41" s="23">
+        <v>0.13599003078516952</v>
+      </c>
+      <c r="N41" s="23">
         <f t="shared" si="34"/>
-        <v>0.14130602444070009</v>
-      </c>
-      <c r="N41" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19049674873149045</v>
+        <v>-0.19581274238702101</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2649,32 +2648,32 @@
         <v>4</v>
       </c>
       <c r="H42" s="20">
+        <f t="shared" si="29"/>
+        <v>43929</v>
+      </c>
+      <c r="I42" s="15">
         <f t="shared" si="30"/>
-        <v>43929</v>
-      </c>
-      <c r="I42" s="15">
+        <v>524163.78874516446</v>
+      </c>
+      <c r="J42" s="21">
         <f t="shared" si="31"/>
-        <v>542289.05508074607</v>
-      </c>
-      <c r="J42" s="21">
-        <f t="shared" si="32"/>
-        <v>-3256752.9449192537</v>
+        <v>-3274878.2112548356</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1657.3626377773412</v>
+        <v>1601.9675695145613</v>
       </c>
       <c r="L42" s="21">
+        <f t="shared" si="32"/>
+        <v>62602.026182250469</v>
+      </c>
+      <c r="M42" s="23">
         <f t="shared" si="33"/>
-        <v>67191.102342264727</v>
-      </c>
-      <c r="M42" s="23">
+        <v>0.13563087599510021</v>
+      </c>
+      <c r="N42" s="23">
         <f t="shared" si="34"/>
-        <v>0.14142578799797567</v>
-      </c>
-      <c r="N42" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19037698517421486</v>
+        <v>-0.19617189717709033</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2702,32 +2701,32 @@
         <v>4</v>
       </c>
       <c r="H43" s="20">
+        <f t="shared" si="29"/>
+        <v>43930</v>
+      </c>
+      <c r="I43" s="15">
         <f t="shared" si="30"/>
-        <v>43930</v>
-      </c>
-      <c r="I43" s="15">
+        <v>595200.70776477945</v>
+      </c>
+      <c r="J43" s="21">
         <f t="shared" si="31"/>
-        <v>619037.44703205046</v>
-      </c>
-      <c r="J43" s="21">
-        <f t="shared" si="32"/>
-        <v>-4440537.5529679498</v>
+        <v>-4464374.2922352208</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1891.9237378730149</v>
+        <v>1819.0730677407685</v>
       </c>
       <c r="L43" s="21">
+        <f t="shared" si="32"/>
+        <v>71036.919019614987</v>
+      </c>
+      <c r="M43" s="23">
         <f t="shared" si="33"/>
-        <v>76748.391951304395</v>
-      </c>
-      <c r="M43" s="23">
+        <v>0.1355242779927161</v>
+      </c>
+      <c r="N43" s="23">
         <f t="shared" si="34"/>
-        <v>0.14152672127944141</v>
-      </c>
-      <c r="N43" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19027605189274913</v>
+        <v>-0.19627849517947443</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2755,32 +2754,32 @@
         <v>4</v>
       </c>
       <c r="H44" s="20">
+        <f t="shared" si="29"/>
+        <v>43931</v>
+      </c>
+      <c r="I44" s="15">
         <f t="shared" si="30"/>
-        <v>43931</v>
-      </c>
-      <c r="I44" s="15">
+        <v>675978.40847808041</v>
+      </c>
+      <c r="J44" s="21">
         <f t="shared" si="31"/>
-        <v>706581.4202301919</v>
-      </c>
-      <c r="J44" s="21">
-        <f t="shared" si="32"/>
-        <v>-6031774.5797698079</v>
+        <v>-6062377.5915219197</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>2159.4786681851833</v>
+        <v>2065.9486811677275</v>
       </c>
       <c r="L44" s="21">
+        <f t="shared" si="32"/>
+        <v>80777.700713300961</v>
+      </c>
+      <c r="M44" s="23">
         <f t="shared" si="33"/>
-        <v>87543.973198141437</v>
-      </c>
-      <c r="M44" s="23">
+        <v>0.13571506159099517</v>
+      </c>
+      <c r="N44" s="23">
         <f t="shared" si="34"/>
-        <v>0.14141951123937238</v>
-      </c>
-      <c r="N44" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19038326193281815</v>
+        <v>-0.19608771158119537</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2808,32 +2807,32 @@
         <v>4</v>
       </c>
       <c r="H45" s="20">
+        <f t="shared" si="29"/>
+        <v>43932</v>
+      </c>
+      <c r="I45" s="15">
         <f t="shared" si="30"/>
-        <v>43932</v>
-      </c>
-      <c r="I45" s="15">
+        <v>767656.90207277995</v>
+      </c>
+      <c r="J45" s="21">
         <f t="shared" si="31"/>
-        <v>806532.54855109495</v>
-      </c>
-      <c r="J45" s="21">
-        <f t="shared" si="32"/>
-        <v>-8167628.4514489053</v>
+        <v>-8206504.0979272202</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>2464.9527767454001</v>
+        <v>2346.1396762615527</v>
       </c>
       <c r="L45" s="21">
+        <f t="shared" si="32"/>
+        <v>91678.493594699539</v>
+      </c>
+      <c r="M45" s="23">
         <f t="shared" si="33"/>
-        <v>99951.128320903052</v>
-      </c>
-      <c r="M45" s="23">
+        <v>0.13562340519293722</v>
+      </c>
+      <c r="N45" s="23">
         <f t="shared" si="34"/>
-        <v>0.14145734017226311</v>
-      </c>
-      <c r="N45" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19034543299992743</v>
+        <v>-0.19617936797925331</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2861,32 +2860,32 @@
         <v>4</v>
       </c>
       <c r="H46" s="20">
+        <f t="shared" si="29"/>
+        <v>43933</v>
+      </c>
+      <c r="I46" s="15">
         <f t="shared" si="30"/>
-        <v>43933</v>
-      </c>
-      <c r="I46" s="15">
+        <v>871767.2334808032</v>
+      </c>
+      <c r="J46" s="21">
         <f t="shared" si="31"/>
-        <v>920630.98025000293</v>
-      </c>
-      <c r="J46" s="21">
-        <f t="shared" si="32"/>
-        <v>-11031182.019749997</v>
+        <v>-11080045.766519196</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>2813.6643650672459</v>
+        <v>2664.3252856992763</v>
       </c>
       <c r="L46" s="21">
+        <f t="shared" si="32"/>
+        <v>104110.33140802325</v>
+      </c>
+      <c r="M46" s="23">
         <f t="shared" si="33"/>
-        <v>114098.43169890798</v>
-      </c>
-      <c r="M46" s="23">
+        <v>0.13562091492554934</v>
+      </c>
+      <c r="N46" s="23">
         <f t="shared" si="34"/>
-        <v>0.14146785756369223</v>
-      </c>
-      <c r="N46" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.1903349156084983</v>
+        <v>-0.19618185824664119</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2917,32 +2916,32 @@
         <v>4</v>
       </c>
       <c r="H47" s="20">
+        <f t="shared" si="29"/>
+        <v>43934</v>
+      </c>
+      <c r="I47" s="15">
         <f t="shared" si="30"/>
-        <v>43934</v>
-      </c>
-      <c r="I47" s="15">
+        <v>990025.18492478086</v>
+      </c>
+      <c r="J47" s="21">
         <f t="shared" si="31"/>
-        <v>1050852.6087126224</v>
-      </c>
-      <c r="J47" s="21">
-        <f t="shared" si="32"/>
-        <v>-14866605.391287377</v>
+        <v>-14927432.815075219</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>3211.6522271168169</v>
+        <v>3025.7493426796482</v>
       </c>
       <c r="L47" s="21">
+        <f t="shared" si="32"/>
+        <v>118257.95144397765</v>
+      </c>
+      <c r="M47" s="23">
         <f t="shared" si="33"/>
-        <v>130221.6284626195</v>
-      </c>
-      <c r="M47" s="23">
+        <v>0.13565312723649386</v>
+      </c>
+      <c r="N47" s="23">
         <f t="shared" si="34"/>
-        <v>0.14144823632510936</v>
-      </c>
-      <c r="N47" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19035453684708117</v>
+        <v>-0.19614964593569667</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2970,32 +2969,32 @@
         <v>4</v>
       </c>
       <c r="H48" s="20">
+        <f t="shared" si="29"/>
+        <v>43935</v>
+      </c>
+      <c r="I48" s="15">
         <f t="shared" si="30"/>
-        <v>43935</v>
-      </c>
-      <c r="I48" s="15">
+        <v>1124304.7584457928</v>
+      </c>
+      <c r="J48" s="21">
         <f t="shared" si="31"/>
-        <v>1199503.9187964236</v>
-      </c>
-      <c r="J48" s="21">
-        <f t="shared" si="32"/>
-        <v>-19999411.081203576</v>
+        <v>-20074610.241554208</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>3665.9655219939596</v>
+        <v>3436.1392373037679</v>
       </c>
       <c r="L48" s="21">
+        <f t="shared" si="32"/>
+        <v>134279.57352101197</v>
+      </c>
+      <c r="M48" s="23">
         <f t="shared" si="33"/>
-        <v>148651.31008380116</v>
-      </c>
-      <c r="M48" s="23">
+        <v>0.13563248245166018</v>
+      </c>
+      <c r="N48" s="23">
         <f t="shared" si="34"/>
-        <v>0.1414578113536881</v>
-      </c>
-      <c r="N48" s="23">
-        <f t="shared" si="35"/>
-        <v>-0.19034496181850244</v>
+        <v>-0.19617029072053035</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3023,32 +3022,32 @@
         <v>4</v>
       </c>
       <c r="H49" s="20">
-        <f t="shared" ref="H49" si="36">A49</f>
+        <f t="shared" ref="H49" si="35">A49</f>
         <v>43936</v>
       </c>
       <c r="I49" s="15">
-        <f t="shared" ref="I49" si="37">I48*(1+AVERAGE(M46:M48))</f>
-        <v>1369183.3062541932</v>
+        <f t="shared" ref="I49" si="36">I48*(1+AVERAGE(M46:M48))</f>
+        <v>1276800.4057344017</v>
       </c>
       <c r="J49" s="21">
-        <f t="shared" ref="J49" si="38">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-26863590.693745807</v>
+        <f t="shared" ref="J49" si="37">IF(I49&lt;=0,0, I49-B49)</f>
+        <v>-26955973.594265599</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>4184.5455570115928</v>
+        <v>3902.2017290171198</v>
       </c>
       <c r="L49" s="21">
-        <f t="shared" ref="L49" si="39">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>169679.3874577696</v>
+        <f t="shared" ref="L49" si="38">IF(I49&lt;=0,0, I49-I48)</f>
+        <v>152495.64728860883</v>
       </c>
       <c r="M49" s="23">
-        <f t="shared" ref="M49" si="40">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.1414579684141633</v>
+        <f t="shared" ref="M49" si="39">IF(I49&lt;=0,0, L49/I48)</f>
+        <v>0.13563550820456768</v>
       </c>
       <c r="N49" s="23">
-        <f t="shared" ref="N49" si="41">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.19034480475802723</v>
+        <f t="shared" ref="N49" si="40">IF(I49&lt;=0,0,M49-E49)</f>
+        <v>-0.19616726496762285</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated stats for Mar 4 (yesterday)
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6675B3C5-79FB-7E47-B31C-9EF37E14F2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F8F853-7A75-B246-8642-3667191F5A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -2439,29 +2439,28 @@
         <f t="shared" ref="H38:H48" si="29">A38</f>
         <v>43925</v>
       </c>
-      <c r="I38" s="15">
-        <f t="shared" ref="I38:I48" si="30">I37*(1+AVERAGE(M35:M37))</f>
-        <v>315150.76402475976</v>
+      <c r="I38" s="14">
+        <v>311357</v>
       </c>
       <c r="J38" s="21">
-        <f t="shared" ref="J38:J48" si="31">IF(I38&lt;=0,0, I38-B38)</f>
-        <v>-892425.23597524024</v>
+        <f t="shared" ref="J38:J48" si="30">IF(I38&lt;=0,0, I38-B38)</f>
+        <v>-896219</v>
       </c>
       <c r="K38" s="22">
         <f t="shared" si="18"/>
-        <v>963.1747066771386</v>
+        <v>951.58007334963327</v>
       </c>
       <c r="L38" s="21">
-        <f t="shared" ref="L38:L48" si="32">IF(I38&lt;=0,0, I38-I37)</f>
-        <v>37989.764024759759</v>
+        <f t="shared" ref="L38:L48" si="31">IF(I38&lt;=0,0, I38-I37)</f>
+        <v>34196</v>
       </c>
       <c r="M38" s="23">
-        <f t="shared" ref="M38:M48" si="33">IF(I38&lt;=0,0, L38/I37)</f>
-        <v>0.13706749515537814</v>
+        <f t="shared" ref="M38:M48" si="32">IF(I38&lt;=0,0, L38/I37)</f>
+        <v>0.12337955195716568</v>
       </c>
       <c r="N38" s="23">
-        <f t="shared" ref="N38:N48" si="34">IF(I38&lt;=0,0,M38-E38)</f>
-        <v>-0.1947352780168124</v>
+        <f t="shared" ref="N38:N48" si="33">IF(I38&lt;=0,0,M38-E38)</f>
+        <v>-0.20842322121502485</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
@@ -2493,28 +2492,28 @@
         <v>43926</v>
       </c>
       <c r="I39" s="15">
+        <f t="shared" ref="I38:I48" si="34">I38*(1+AVERAGE(M36:M38))</f>
+        <v>352265.58044976922</v>
+      </c>
+      <c r="J39" s="21">
         <f t="shared" si="30"/>
-        <v>357995.72154564742</v>
-      </c>
-      <c r="J39" s="21">
-        <f t="shared" si="31"/>
-        <v>-1250257.2784543526</v>
+        <v>-1255987.4195502307</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="18"/>
-        <v>1094.118953379118</v>
+        <v>1076.6062972181212</v>
       </c>
       <c r="L39" s="21">
+        <f t="shared" si="31"/>
+        <v>40908.580449769215</v>
+      </c>
+      <c r="M39" s="23">
         <f t="shared" si="32"/>
-        <v>42844.957520887663</v>
-      </c>
-      <c r="M39" s="23">
+        <v>0.13138802226951446</v>
+      </c>
+      <c r="N39" s="23">
         <f t="shared" si="33"/>
-        <v>0.13595067000225186</v>
-      </c>
-      <c r="N39" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19585210316993867</v>
+        <v>-0.20041475090267608</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2546,28 +2545,28 @@
         <v>43927</v>
       </c>
       <c r="I40" s="15">
+        <f t="shared" si="34"/>
+        <v>397661.48108099762</v>
+      </c>
+      <c r="J40" s="21">
         <f t="shared" si="30"/>
-        <v>406307.93409682775</v>
-      </c>
-      <c r="J40" s="21">
-        <f t="shared" si="31"/>
-        <v>-1735568.0659031724</v>
+        <v>-1744214.5189190023</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1241.7724147213562</v>
+        <v>1215.346824819675</v>
       </c>
       <c r="L40" s="21">
+        <f t="shared" si="31"/>
+        <v>45395.900631228404</v>
+      </c>
+      <c r="M40" s="23">
         <f t="shared" si="32"/>
-        <v>48312.212551180332</v>
-      </c>
-      <c r="M40" s="23">
+        <v>0.12886839688756241</v>
+      </c>
+      <c r="N40" s="23">
         <f t="shared" si="33"/>
-        <v>0.13495192719787888</v>
-      </c>
-      <c r="N40" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19685084597431166</v>
+        <v>-0.20293437628462813</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2599,28 +2598,28 @@
         <v>43928</v>
       </c>
       <c r="I41" s="15">
+        <f t="shared" si="34"/>
+        <v>448513.89723740978</v>
+      </c>
+      <c r="J41" s="21">
         <f t="shared" si="30"/>
-        <v>461561.76256291399</v>
-      </c>
-      <c r="J41" s="21">
-        <f t="shared" si="31"/>
-        <v>-2390994.2374370862</v>
+        <v>-2404042.1027625902</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1410.6410836274877</v>
+        <v>1370.7637446131107</v>
       </c>
       <c r="L41" s="21">
+        <f t="shared" si="31"/>
+        <v>50852.41615641216</v>
+      </c>
+      <c r="M41" s="23">
         <f t="shared" si="32"/>
-        <v>55253.828466086241</v>
-      </c>
-      <c r="M41" s="23">
+        <v>0.12787865703808082</v>
+      </c>
+      <c r="N41" s="23">
         <f t="shared" si="33"/>
-        <v>0.13599003078516952</v>
-      </c>
-      <c r="N41" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19581274238702101</v>
+        <v>-0.20392411613410971</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2652,28 +2651,28 @@
         <v>43929</v>
       </c>
       <c r="I42" s="15">
+        <f t="shared" si="34"/>
+        <v>506541.88913035282</v>
+      </c>
+      <c r="J42" s="21">
         <f t="shared" si="30"/>
-        <v>524163.78874516446</v>
-      </c>
-      <c r="J42" s="21">
-        <f t="shared" si="31"/>
-        <v>-3274878.2112548356</v>
+        <v>-3292500.110869647</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1601.9675695145613</v>
+        <v>1548.1109081001002</v>
       </c>
       <c r="L42" s="21">
+        <f t="shared" si="31"/>
+        <v>58027.991892943042</v>
+      </c>
+      <c r="M42" s="23">
         <f t="shared" si="32"/>
-        <v>62602.026182250469</v>
-      </c>
-      <c r="M42" s="23">
+        <v>0.12937835873171918</v>
+      </c>
+      <c r="N42" s="23">
         <f t="shared" si="33"/>
-        <v>0.13563087599510021</v>
-      </c>
-      <c r="N42" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19617189717709033</v>
+        <v>-0.20242441444047135</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2705,28 +2704,28 @@
         <v>43930</v>
       </c>
       <c r="I43" s="15">
+        <f t="shared" si="34"/>
+        <v>571738.12111991865</v>
+      </c>
+      <c r="J43" s="21">
         <f t="shared" si="30"/>
-        <v>595200.70776477945</v>
-      </c>
-      <c r="J43" s="21">
-        <f t="shared" si="31"/>
-        <v>-4464374.2922352208</v>
+        <v>-4487836.8788800817</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1819.0730677407685</v>
+        <v>1747.3658958432723</v>
       </c>
       <c r="L43" s="21">
+        <f t="shared" si="31"/>
+        <v>65196.231989565829</v>
+      </c>
+      <c r="M43" s="23">
         <f t="shared" si="32"/>
-        <v>71036.919019614987</v>
-      </c>
-      <c r="M43" s="23">
+        <v>0.12870847088578752</v>
+      </c>
+      <c r="N43" s="23">
         <f t="shared" si="33"/>
-        <v>0.1355242779927161</v>
-      </c>
-      <c r="N43" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19627849517947443</v>
+        <v>-0.20309430228640302</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2758,28 +2757,28 @@
         <v>43931</v>
       </c>
       <c r="I44" s="15">
+        <f t="shared" si="34"/>
+        <v>645295.18183911894</v>
+      </c>
+      <c r="J44" s="21">
         <f t="shared" si="30"/>
-        <v>675978.40847808041</v>
-      </c>
-      <c r="J44" s="21">
-        <f t="shared" si="31"/>
-        <v>-6062377.5915219197</v>
+        <v>-6093060.8181608813</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>2065.9486811677275</v>
+        <v>1972.1735386281141</v>
       </c>
       <c r="L44" s="21">
+        <f t="shared" si="31"/>
+        <v>73557.060719200294</v>
+      </c>
+      <c r="M44" s="23">
         <f t="shared" si="32"/>
-        <v>80777.700713300961</v>
-      </c>
-      <c r="M44" s="23">
+        <v>0.12865516221852932</v>
+      </c>
+      <c r="N44" s="23">
         <f t="shared" si="33"/>
-        <v>0.13571506159099517</v>
-      </c>
-      <c r="N44" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19608771158119537</v>
+        <v>-0.20314761095366121</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2811,28 +2810,28 @@
         <v>43932</v>
       </c>
       <c r="I45" s="15">
+        <f t="shared" si="34"/>
+        <v>728482.76315467153</v>
+      </c>
+      <c r="J45" s="21">
         <f t="shared" si="30"/>
-        <v>767656.90207277995</v>
-      </c>
-      <c r="J45" s="21">
-        <f t="shared" si="31"/>
-        <v>-8206504.0979272202</v>
+        <v>-8245678.2368453285</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>2346.1396762615527</v>
+        <v>2226.4143128199012</v>
       </c>
       <c r="L45" s="21">
+        <f t="shared" si="31"/>
+        <v>83187.581315552583</v>
+      </c>
+      <c r="M45" s="23">
         <f t="shared" si="32"/>
-        <v>91678.493594699539</v>
-      </c>
-      <c r="M45" s="23">
+        <v>0.12891399727867858</v>
+      </c>
+      <c r="N45" s="23">
         <f t="shared" si="33"/>
-        <v>0.13562340519293722</v>
-      </c>
-      <c r="N45" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19617936797925331</v>
+        <v>-0.20288877589351195</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2864,28 +2863,28 @@
         <v>43933</v>
       </c>
       <c r="I46" s="15">
+        <f t="shared" si="34"/>
+        <v>822281.62833008601</v>
+      </c>
+      <c r="J46" s="21">
         <f t="shared" si="30"/>
-        <v>871767.2334808032</v>
-      </c>
-      <c r="J46" s="21">
-        <f t="shared" si="31"/>
-        <v>-11080045.766519196</v>
+        <v>-11129531.371669915</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>2664.3252856992763</v>
+        <v>2513.0856611555196</v>
       </c>
       <c r="L46" s="21">
+        <f t="shared" si="31"/>
+        <v>93798.865175414481</v>
+      </c>
+      <c r="M46" s="23">
         <f t="shared" si="32"/>
-        <v>104110.33140802325</v>
-      </c>
-      <c r="M46" s="23">
+        <v>0.12875921012766517</v>
+      </c>
+      <c r="N46" s="23">
         <f t="shared" si="33"/>
-        <v>0.13562091492554934</v>
-      </c>
-      <c r="N46" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19618185824664119</v>
+        <v>-0.20304356304452537</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2920,28 +2919,28 @@
         <v>43934</v>
       </c>
       <c r="I47" s="15">
+        <f t="shared" si="34"/>
+        <v>928171.86861183541</v>
+      </c>
+      <c r="J47" s="21">
         <f t="shared" si="30"/>
-        <v>990025.18492478086</v>
-      </c>
-      <c r="J47" s="21">
-        <f t="shared" si="31"/>
-        <v>-14927432.815075219</v>
+        <v>-14989286.131388165</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>3025.7493426796482</v>
+        <v>2836.7110898894725</v>
       </c>
       <c r="L47" s="21">
+        <f t="shared" si="31"/>
+        <v>105890.2402817494</v>
+      </c>
+      <c r="M47" s="23">
         <f t="shared" si="32"/>
-        <v>118257.95144397765</v>
-      </c>
-      <c r="M47" s="23">
+        <v>0.12877612320829113</v>
+      </c>
+      <c r="N47" s="23">
         <f t="shared" si="33"/>
-        <v>0.13565312723649386</v>
-      </c>
-      <c r="N47" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19614964593569667</v>
+        <v>-0.20302664996389941</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2973,28 +2972,28 @@
         <v>43935</v>
       </c>
       <c r="I48" s="15">
+        <f t="shared" si="34"/>
+        <v>1047735.6677186282</v>
+      </c>
+      <c r="J48" s="21">
         <f t="shared" si="30"/>
-        <v>1124304.7584457928</v>
-      </c>
-      <c r="J48" s="21">
-        <f t="shared" si="31"/>
-        <v>-20074610.241554208</v>
+        <v>-20151179.332281373</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>3436.1392373037679</v>
+        <v>3202.1261238344382</v>
       </c>
       <c r="L48" s="21">
+        <f t="shared" si="31"/>
+        <v>119563.79910679278</v>
+      </c>
+      <c r="M48" s="23">
         <f t="shared" si="32"/>
-        <v>134279.57352101197</v>
-      </c>
-      <c r="M48" s="23">
+        <v>0.12881644353821153</v>
+      </c>
+      <c r="N48" s="23">
         <f t="shared" si="33"/>
-        <v>0.13563248245166018</v>
-      </c>
-      <c r="N48" s="23">
-        <f t="shared" si="34"/>
-        <v>-0.19617029072053035</v>
+        <v>-0.202986329633979</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3027,27 +3026,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="36">I48*(1+AVERAGE(M46:M48))</f>
-        <v>1276800.4057344017</v>
+        <v>1182667.180024473</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="37">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-26955973.594265599</v>
+        <v>-27050106.819975525</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>3902.2017290171198</v>
+        <v>3614.5084964073135</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="38">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>152495.64728860883</v>
+        <v>134931.51230584481</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="39">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.13563550820456768</v>
+        <v>0.12878392562472252</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="40">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.19616726496762285</v>
+        <v>-0.20301884754746802</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated stats for Apr 5
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F8F853-7A75-B246-8642-3667191F5A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5101C4-E16F-404E-8FFA-CDD441639A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
+      <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
@@ -2491,29 +2491,28 @@
         <f t="shared" si="29"/>
         <v>43926</v>
       </c>
-      <c r="I39" s="15">
-        <f t="shared" ref="I38:I48" si="34">I38*(1+AVERAGE(M36:M38))</f>
-        <v>352265.58044976922</v>
+      <c r="I39" s="14">
+        <v>336673</v>
       </c>
       <c r="J39" s="21">
         <f t="shared" si="30"/>
-        <v>-1255987.4195502307</v>
+        <v>-1271580</v>
       </c>
       <c r="K39" s="22">
         <f t="shared" si="18"/>
-        <v>1076.6062972181212</v>
+        <v>1028.9517114914424</v>
       </c>
       <c r="L39" s="21">
         <f t="shared" si="31"/>
-        <v>40908.580449769215</v>
+        <v>25316</v>
       </c>
       <c r="M39" s="23">
         <f t="shared" si="32"/>
-        <v>0.13138802226951446</v>
+        <v>8.1308594314564955E-2</v>
       </c>
       <c r="N39" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20041475090267608</v>
+        <v>-0.25049417885762559</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -2545,28 +2544,28 @@
         <v>43927</v>
       </c>
       <c r="I40" s="15">
-        <f t="shared" si="34"/>
-        <v>397661.48108099762</v>
+        <f t="shared" ref="I39:I48" si="34">I39*(1+AVERAGE(M37:M39))</f>
+        <v>374439.37936936738</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="30"/>
-        <v>-1744214.5189190023</v>
+        <v>-1767436.6206306326</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1215.346824819675</v>
+        <v>1144.3746313244724</v>
       </c>
       <c r="L40" s="21">
         <f t="shared" si="31"/>
-        <v>45395.900631228404</v>
+        <v>37766.37936936738</v>
       </c>
       <c r="M40" s="23">
         <f t="shared" si="32"/>
-        <v>0.12886839688756241</v>
+        <v>0.11217525423591253</v>
       </c>
       <c r="N40" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20293437628462813</v>
+        <v>-0.21962751893627802</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2599,27 +2598,27 @@
       </c>
       <c r="I41" s="15">
         <f t="shared" si="34"/>
-        <v>448513.89723740978</v>
+        <v>413988.09104635043</v>
       </c>
       <c r="J41" s="21">
         <f t="shared" si="30"/>
-        <v>-2404042.1027625902</v>
+        <v>-2438567.9089536495</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1370.7637446131107</v>
+        <v>1265.2447770365231</v>
       </c>
       <c r="L41" s="21">
         <f t="shared" si="31"/>
-        <v>50852.41615641216</v>
+        <v>39548.711676983046</v>
       </c>
       <c r="M41" s="23">
         <f t="shared" si="32"/>
-        <v>0.12787865703808082</v>
+        <v>0.10562113350254768</v>
       </c>
       <c r="N41" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20392411613410971</v>
+        <v>-0.22618163966964286</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2652,27 +2651,27 @@
       </c>
       <c r="I42" s="15">
         <f t="shared" si="34"/>
-        <v>506541.88913035282</v>
+        <v>455263.39122721204</v>
       </c>
       <c r="J42" s="21">
         <f t="shared" si="30"/>
-        <v>-3292500.110869647</v>
+        <v>-3343778.6087727882</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1548.1109081001002</v>
+        <v>1391.3917824792545</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="31"/>
-        <v>58027.991892943042</v>
+        <v>41275.30018086161</v>
       </c>
       <c r="M42" s="23">
         <f t="shared" si="32"/>
-        <v>0.12937835873171918</v>
+        <v>9.9701660684341747E-2</v>
       </c>
       <c r="N42" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20242441444047135</v>
+        <v>-0.23210111248784879</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2705,27 +2704,27 @@
       </c>
       <c r="I43" s="15">
         <f t="shared" si="34"/>
-        <v>571738.12111991865</v>
+        <v>503445.13730487414</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="30"/>
-        <v>-4487836.8788800817</v>
+        <v>-4556129.8626951259</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1747.3658958432723</v>
+        <v>1538.6465076554832</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="31"/>
-        <v>65196.231989565829</v>
+        <v>48181.746077662101</v>
       </c>
       <c r="M43" s="23">
         <f t="shared" si="32"/>
-        <v>0.12870847088578752</v>
+        <v>0.10583268280760058</v>
       </c>
       <c r="N43" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20309430228640302</v>
+        <v>-0.22597009036458995</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2758,27 +2757,27 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" si="34"/>
-        <v>645295.18183911894</v>
+        <v>555661.70791775896</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="30"/>
-        <v>-6093060.8181608813</v>
+        <v>-6182694.2920822408</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>1972.1735386281141</v>
+        <v>1698.2326036606325</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="31"/>
-        <v>73557.060719200294</v>
+        <v>52216.570612884825</v>
       </c>
       <c r="M44" s="23">
         <f t="shared" si="32"/>
-        <v>0.12865516221852932</v>
+        <v>0.10371849233149656</v>
       </c>
       <c r="N44" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20314761095366121</v>
+        <v>-0.22808428084069399</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2811,27 +2810,27 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" si="34"/>
-        <v>728482.76315467153</v>
+        <v>612941.69422844646</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="30"/>
-        <v>-8245678.2368453285</v>
+        <v>-8361219.3057715539</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>2226.4143128199012</v>
+        <v>1873.2936865172569</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="31"/>
-        <v>83187.581315552583</v>
+        <v>57279.986310687498</v>
       </c>
       <c r="M45" s="23">
         <f t="shared" si="32"/>
-        <v>0.12891399727867858</v>
+        <v>0.10308427860781304</v>
       </c>
       <c r="N45" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20288877589351195</v>
+        <v>-0.22871849456437748</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2864,27 +2863,27 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" si="34"/>
-        <v>822281.62833008601</v>
+        <v>676817.46246028331</v>
       </c>
       <c r="J46" s="21">
         <f t="shared" si="30"/>
-        <v>-11129531.371669915</v>
+        <v>-11274995.537539717</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>2513.0856611555196</v>
+        <v>2068.5130270791055</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="31"/>
-        <v>93798.865175414481</v>
+        <v>63875.768231836846</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="32"/>
-        <v>0.12875921012766517</v>
+        <v>0.1042118179156369</v>
       </c>
       <c r="N46" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20304356304452537</v>
+        <v>-0.22759095525655365</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2920,27 +2919,27 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" si="34"/>
-        <v>928171.86861183541</v>
+        <v>746984.16406592773</v>
       </c>
       <c r="J47" s="21">
         <f t="shared" si="30"/>
-        <v>-14989286.131388165</v>
+        <v>-15170473.835934073</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>2836.7110898894725</v>
+        <v>2282.9589366318082</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="31"/>
-        <v>105890.2402817494</v>
+        <v>70166.701605644426</v>
       </c>
       <c r="M47" s="23">
         <f t="shared" si="32"/>
-        <v>0.12877612320829113</v>
+        <v>0.10367152961831554</v>
       </c>
       <c r="N47" s="23">
         <f t="shared" si="33"/>
-        <v>-0.20302664996389941</v>
+        <v>-0.22813124355387498</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2973,27 +2972,27 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" si="34"/>
-        <v>1047735.6677186282</v>
+        <v>824413.46148761862</v>
       </c>
       <c r="J48" s="21">
         <f t="shared" si="30"/>
-        <v>-20151179.332281373</v>
+        <v>-20374501.538512383</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>3202.1261238344382</v>
+        <v>2519.6010436663159</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="31"/>
-        <v>119563.79910679278</v>
+        <v>77429.297421690891</v>
       </c>
       <c r="M48" s="23">
         <f t="shared" si="32"/>
-        <v>0.12881644353821153</v>
+        <v>0.10365587538058851</v>
       </c>
       <c r="N48" s="23">
         <f t="shared" si="33"/>
-        <v>-0.202986329633979</v>
+        <v>-0.22814689779160202</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3026,27 +3025,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="36">I48*(1+AVERAGE(M46:M48))</f>
-        <v>1182667.180024473</v>
+        <v>910025.83787166525</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="37">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-27050106.819975525</v>
+        <v>-27322748.162128333</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>3614.5084964073135</v>
+        <v>2781.2525607324733</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="38">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>134931.51230584481</v>
+        <v>85612.376384046627</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="39">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.12878392562472252</v>
+        <v>0.10384640763818045</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="40">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.20301884754746802</v>
+        <v>-0.22795636553401008</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated data for Apr 7
</commit_message>
<xml_diff>
--- a/CoronaVirus US Lockdown Forecast (Excel).xlsx
+++ b/CoronaVirus US Lockdown Forecast (Excel).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brian/Dropbox/Programming/Projects/DS Projects/CoronaVirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5101C4-E16F-404E-8FFA-CDD441639A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D323715-A1B7-6B47-AD97-7DE0578FB0FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26880" yWindow="-360" windowWidth="38400" windowHeight="21140" xr2:uid="{2DCD77F1-C1DF-40E4-8CFE-958F60BFDE9D}"/>
   </bookViews>
@@ -2543,29 +2543,29 @@
         <f t="shared" si="29"/>
         <v>43927</v>
       </c>
-      <c r="I40" s="15">
-        <f t="shared" ref="I39:I48" si="34">I39*(1+AVERAGE(M37:M39))</f>
-        <v>374439.37936936738</v>
+      <c r="I40" s="6">
+        <f>I39*1.08</f>
+        <v>363606.84</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" si="30"/>
-        <v>-1767436.6206306326</v>
+        <v>-1778269.16</v>
       </c>
       <c r="K40" s="22">
         <f t="shared" si="18"/>
-        <v>1144.3746313244724</v>
+        <v>1111.267848410758</v>
       </c>
       <c r="L40" s="21">
         <f t="shared" si="31"/>
-        <v>37766.37936936738</v>
+        <v>26933.840000000026</v>
       </c>
       <c r="M40" s="23">
         <f t="shared" si="32"/>
-        <v>0.11217525423591253</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="N40" s="23">
         <f t="shared" si="33"/>
-        <v>-0.21962751893627802</v>
+        <v>-0.25180277317219046</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -2596,29 +2596,28 @@
         <f t="shared" si="29"/>
         <v>43928</v>
       </c>
-      <c r="I41" s="15">
-        <f t="shared" si="34"/>
-        <v>413988.09104635043</v>
+      <c r="I41" s="14">
+        <v>400335</v>
       </c>
       <c r="J41" s="21">
         <f t="shared" si="30"/>
-        <v>-2438567.9089536495</v>
+        <v>-2452221</v>
       </c>
       <c r="K41" s="22">
         <f t="shared" si="18"/>
-        <v>1265.2447770365231</v>
+        <v>1223.5177261613692</v>
       </c>
       <c r="L41" s="21">
         <f t="shared" si="31"/>
-        <v>39548.711676983046</v>
+        <v>36728.159999999974</v>
       </c>
       <c r="M41" s="23">
         <f t="shared" si="32"/>
-        <v>0.10562113350254768</v>
+        <v>0.1010106410539471</v>
       </c>
       <c r="N41" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22618163966964286</v>
+        <v>-0.23079213211824345</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
@@ -2650,28 +2649,28 @@
         <v>43929</v>
       </c>
       <c r="I42" s="15">
-        <f t="shared" si="34"/>
-        <v>455263.39122721204</v>
+        <f t="shared" ref="I40:I48" si="34">I41*(1+AVERAGE(M39:M41))</f>
+        <v>435340.19036375114</v>
       </c>
       <c r="J42" s="21">
         <f t="shared" si="30"/>
-        <v>-3343778.6087727882</v>
+        <v>-3363701.8096362487</v>
       </c>
       <c r="K42" s="22">
         <f t="shared" si="18"/>
-        <v>1391.3917824792545</v>
+        <v>1330.5018042901929</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="31"/>
-        <v>41275.30018086161</v>
+        <v>35005.190363751142</v>
       </c>
       <c r="M42" s="23">
         <f t="shared" si="32"/>
-        <v>9.9701660684341747E-2</v>
+        <v>8.7439745122837476E-2</v>
       </c>
       <c r="N42" s="23">
         <f t="shared" si="33"/>
-        <v>-0.23210111248784879</v>
+        <v>-0.24436302804935306</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
@@ -2704,27 +2703,27 @@
       </c>
       <c r="I43" s="15">
         <f t="shared" si="34"/>
-        <v>503445.13730487414</v>
+        <v>474295.93777089246</v>
       </c>
       <c r="J43" s="21">
         <f t="shared" si="30"/>
-        <v>-4556129.8626951259</v>
+        <v>-4585279.0622291071</v>
       </c>
       <c r="K43" s="22">
         <f t="shared" si="18"/>
-        <v>1538.6465076554832</v>
+        <v>1449.5597120137302</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="31"/>
-        <v>48181.746077662101</v>
+        <v>38955.747407141316</v>
       </c>
       <c r="M43" s="23">
         <f t="shared" si="32"/>
-        <v>0.10583268280760058</v>
+        <v>8.9483462058928223E-2</v>
       </c>
       <c r="N43" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22597009036458995</v>
+        <v>-0.24231931111326233</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
@@ -2757,27 +2756,27 @@
       </c>
       <c r="I44" s="15">
         <f t="shared" si="34"/>
-        <v>555661.70791775896</v>
+        <v>518236.90283330256</v>
       </c>
       <c r="J44" s="21">
         <f t="shared" si="30"/>
-        <v>-6182694.2920822408</v>
+        <v>-6220119.0971666975</v>
       </c>
       <c r="K44" s="22">
         <f t="shared" si="18"/>
-        <v>1698.2326036606325</v>
+        <v>1583.8536150162058</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="31"/>
-        <v>52216.570612884825</v>
+        <v>43940.965062410105</v>
       </c>
       <c r="M44" s="23">
         <f t="shared" si="32"/>
-        <v>0.10371849233149656</v>
+        <v>9.264461607857094E-2</v>
       </c>
       <c r="N44" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22808428084069399</v>
+        <v>-0.23915815709361959</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
@@ -2810,27 +2809,27 @@
       </c>
       <c r="I45" s="15">
         <f t="shared" si="34"/>
-        <v>612941.69422844646</v>
+        <v>564803.56744328665</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="30"/>
-        <v>-8361219.3057715539</v>
+        <v>-8409357.432556713</v>
       </c>
       <c r="K45" s="22">
         <f t="shared" si="18"/>
-        <v>1873.2936865172569</v>
+        <v>1726.1722721371841</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="31"/>
-        <v>57279.986310687498</v>
+        <v>46566.664609984087</v>
       </c>
       <c r="M45" s="23">
         <f t="shared" si="32"/>
-        <v>0.10308427860781304</v>
+        <v>8.9855941086779079E-2</v>
       </c>
       <c r="N45" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22871849456437748</v>
+        <v>-0.24194683208541146</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
@@ -2863,27 +2862,27 @@
       </c>
       <c r="I46" s="15">
         <f t="shared" si="34"/>
-        <v>676817.46246028331</v>
+        <v>616009.41555843188</v>
       </c>
       <c r="J46" s="21">
         <f t="shared" si="30"/>
-        <v>-11274995.537539717</v>
+        <v>-11335803.584441569</v>
       </c>
       <c r="K46" s="22">
         <f t="shared" si="18"/>
-        <v>2068.5130270791055</v>
+        <v>1882.6693629536426</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="31"/>
-        <v>63875.768231836846</v>
+        <v>51205.848115145229</v>
       </c>
       <c r="M46" s="23">
         <f t="shared" si="32"/>
-        <v>0.1042118179156369</v>
+        <v>9.0661339741426011E-2</v>
       </c>
       <c r="N46" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22759095525655365</v>
+        <v>-0.24114143343076452</v>
       </c>
       <c r="O46" t="s">
         <v>19</v>
@@ -2919,27 +2918,27 @@
       </c>
       <c r="I47" s="15">
         <f t="shared" si="34"/>
-        <v>746984.16406592773</v>
+        <v>672099.51571389043</v>
       </c>
       <c r="J47" s="21">
         <f t="shared" si="30"/>
-        <v>-15170473.835934073</v>
+        <v>-15245358.484286109</v>
       </c>
       <c r="K47" s="22">
         <f t="shared" si="18"/>
-        <v>2282.9589366318082</v>
+        <v>2054.0938744312052</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="31"/>
-        <v>70166.701605644426</v>
+        <v>56090.100155458553</v>
       </c>
       <c r="M47" s="23">
         <f t="shared" si="32"/>
-        <v>0.10367152961831554</v>
+        <v>9.1053965635591969E-2</v>
       </c>
       <c r="N47" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22813124355387498</v>
+        <v>-0.24074880753659855</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
@@ -2972,27 +2971,27 @@
       </c>
       <c r="I48" s="15">
         <f t="shared" si="34"/>
-        <v>824413.46148761862</v>
+        <v>732940.48345726891</v>
       </c>
       <c r="J48" s="21">
         <f t="shared" si="30"/>
-        <v>-20374501.538512383</v>
+        <v>-20465974.516542733</v>
       </c>
       <c r="K48" s="22">
         <f t="shared" si="18"/>
-        <v>2519.6010436663159</v>
+        <v>2240.0381523755159</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="31"/>
-        <v>77429.297421690891</v>
+        <v>60840.967743378482</v>
       </c>
       <c r="M48" s="23">
         <f t="shared" si="32"/>
-        <v>0.10365587538058851</v>
+        <v>9.0523748821265612E-2</v>
       </c>
       <c r="N48" s="23">
         <f t="shared" si="33"/>
-        <v>-0.22814689779160202</v>
+        <v>-0.24127902435092491</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3025,27 +3024,27 @@
       </c>
       <c r="I49" s="15">
         <f t="shared" ref="I49" si="36">I48*(1+AVERAGE(M46:M48))</f>
-        <v>910025.83787166525</v>
+        <v>799452.15812394873</v>
       </c>
       <c r="J49" s="21">
         <f t="shared" ref="J49" si="37">IF(I49&lt;=0,0, I49-B49)</f>
-        <v>-27322748.162128333</v>
+        <v>-27433321.841876052</v>
       </c>
       <c r="K49" s="22">
         <f t="shared" si="18"/>
-        <v>2781.2525607324733</v>
+        <v>2443.3134416991097</v>
       </c>
       <c r="L49" s="21">
         <f t="shared" ref="L49" si="38">IF(I49&lt;=0,0, I49-I48)</f>
-        <v>85612.376384046627</v>
+        <v>66511.674666679814</v>
       </c>
       <c r="M49" s="23">
         <f t="shared" ref="M49" si="39">IF(I49&lt;=0,0, L49/I48)</f>
-        <v>0.10384640763818045</v>
+        <v>9.0746351399427785E-2</v>
       </c>
       <c r="N49" s="23">
         <f t="shared" ref="N49" si="40">IF(I49&lt;=0,0,M49-E49)</f>
-        <v>-0.22795636553401008</v>
+        <v>-0.24105642177276276</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>